<commit_message>
[IMPL] Modelos SP2 Se han añadido los modelos de Plaga, Tratamiento, Solicitud de Servicio y Servicio.
</commit_message>
<xml_diff>
--- a/documentación/Product Backlog/SP2.xlsx
+++ b/documentación/Product Backlog/SP2.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23530"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23628"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alesk\Desktop\Universidad\TFG_app\TFG_app\documentación\Product Backlog\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7AE3F152-BE8C-42A4-8A6A-F945C9C2E44E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48839E60-95D5-4D18-8289-9EC4235BB0AF}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{41FE112A-4516-4423-9CD7-320A9C032A6D}"/>
+    <workbookView xWindow="29610" yWindow="-120" windowWidth="19800" windowHeight="11760" activeTab="1" xr2:uid="{41FE112A-4516-4423-9CD7-320A9C032A6D}"/>
   </bookViews>
   <sheets>
     <sheet name="SPRINT-BACKLOG" sheetId="1" r:id="rId1"/>
@@ -321,7 +321,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -353,14 +353,20 @@
     <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -913,7 +919,6 @@
           </c:extLst>
         </c:ser>
         <c:dLbls>
-          <c:dLblPos val="t"/>
           <c:showLegendKey val="0"/>
           <c:showVal val="0"/>
           <c:showCatName val="0"/>
@@ -2705,8 +2710,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2BB024A1-16E4-467A-A83B-A5E93171F59F}">
   <dimension ref="A1:O236"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A38" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D39" sqref="D39"/>
+    <sheetView topLeftCell="A40" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2742,13 +2747,15 @@
       <c r="A2" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="15" t="s">
         <v>25</v>
       </c>
       <c r="C2" s="5">
         <v>44228</v>
       </c>
-      <c r="D2" s="5"/>
+      <c r="D2" s="5">
+        <v>44228</v>
+      </c>
       <c r="E2" s="5">
         <v>44229</v>
       </c>
@@ -2764,18 +2771,20 @@
       <c r="A3" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="4" t="s">
+      <c r="B3" s="15" t="s">
         <v>25</v>
       </c>
       <c r="C3" s="5">
         <v>44228</v>
       </c>
-      <c r="D3" s="5"/>
+      <c r="D3" s="5">
+        <v>44229</v>
+      </c>
       <c r="E3" s="5">
         <v>44229</v>
       </c>
       <c r="F3" s="4" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="G3" s="1"/>
       <c r="N3" t="s">
@@ -2789,18 +2798,20 @@
       <c r="A4" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="B4" s="4" t="s">
+      <c r="B4" s="15" t="s">
         <v>25</v>
       </c>
       <c r="C4" s="5">
         <v>44228</v>
       </c>
-      <c r="D4" s="5"/>
+      <c r="D4" s="5">
+        <v>44229</v>
+      </c>
       <c r="E4" s="5">
         <v>44229</v>
       </c>
       <c r="F4" s="4" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="G4" s="1"/>
       <c r="N4" t="s">
@@ -2811,18 +2822,20 @@
       <c r="A5" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="B5" s="4" t="s">
+      <c r="B5" s="15" t="s">
         <v>25</v>
       </c>
       <c r="C5" s="5">
         <v>44228</v>
       </c>
-      <c r="D5" s="5"/>
+      <c r="D5" s="5">
+        <v>44229</v>
+      </c>
       <c r="E5" s="5">
         <v>44229</v>
       </c>
       <c r="F5" s="4" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="G5" s="1"/>
     </row>
@@ -2830,7 +2843,7 @@
       <c r="A6" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="B6" s="4" t="s">
+      <c r="B6" s="15" t="s">
         <v>27</v>
       </c>
       <c r="C6" s="5">
@@ -2849,7 +2862,7 @@
       <c r="A7" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="B7" s="4" t="s">
+      <c r="B7" s="15" t="s">
         <v>27</v>
       </c>
       <c r="C7" s="5">
@@ -2868,7 +2881,7 @@
       <c r="A8" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="B8" s="4" t="s">
+      <c r="B8" s="15" t="s">
         <v>27</v>
       </c>
       <c r="C8" s="5">
@@ -2887,7 +2900,7 @@
       <c r="A9" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="B9" s="4" t="s">
+      <c r="B9" s="15" t="s">
         <v>27</v>
       </c>
       <c r="C9" s="5">
@@ -2906,7 +2919,7 @@
       <c r="A10" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="B10" s="4">
+      <c r="B10" s="15">
         <v>1</v>
       </c>
       <c r="C10" s="5">
@@ -2925,7 +2938,7 @@
       <c r="A11" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="B11" s="4">
+      <c r="B11" s="15">
         <v>1</v>
       </c>
       <c r="C11" s="5">
@@ -2944,7 +2957,7 @@
       <c r="A12" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="B12" s="4">
+      <c r="B12" s="15">
         <v>1</v>
       </c>
       <c r="C12" s="5">
@@ -2963,7 +2976,7 @@
       <c r="A13" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="B13" s="4">
+      <c r="B13" s="15">
         <v>1</v>
       </c>
       <c r="C13" s="5">
@@ -2982,7 +2995,7 @@
       <c r="A14" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="B14" s="4">
+      <c r="B14" s="15">
         <v>1</v>
       </c>
       <c r="C14" s="5">
@@ -3001,7 +3014,7 @@
       <c r="A15" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="B15" s="4">
+      <c r="B15" s="15">
         <v>1</v>
       </c>
       <c r="C15" s="5">
@@ -3020,7 +3033,7 @@
       <c r="A16" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="B16" s="4">
+      <c r="B16" s="15">
         <v>1</v>
       </c>
       <c r="C16" s="5">
@@ -3039,7 +3052,7 @@
       <c r="A17" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="B17" s="4">
+      <c r="B17" s="15">
         <v>1</v>
       </c>
       <c r="C17" s="5">
@@ -3058,7 +3071,7 @@
       <c r="A18" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="B18" s="4">
+      <c r="B18" s="15">
         <v>1</v>
       </c>
       <c r="C18" s="5">
@@ -3077,7 +3090,7 @@
       <c r="A19" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="B19" s="4">
+      <c r="B19" s="15">
         <v>1</v>
       </c>
       <c r="C19" s="5">
@@ -3096,7 +3109,7 @@
       <c r="A20" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="B20" s="4">
+      <c r="B20" s="15">
         <v>1</v>
       </c>
       <c r="C20" s="5">
@@ -3115,7 +3128,7 @@
       <c r="A21" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="B21" s="4">
+      <c r="B21" s="15">
         <v>1</v>
       </c>
       <c r="C21" s="5">
@@ -3134,7 +3147,7 @@
       <c r="A22" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="B22" s="4">
+      <c r="B22" s="15">
         <v>1</v>
       </c>
       <c r="C22" s="5">
@@ -3153,7 +3166,7 @@
       <c r="A23" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="B23" s="4">
+      <c r="B23" s="15">
         <v>1</v>
       </c>
       <c r="C23" s="5">
@@ -3172,7 +3185,7 @@
       <c r="A24" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="B24" s="4">
+      <c r="B24" s="15">
         <v>1</v>
       </c>
       <c r="C24" s="5">
@@ -3191,7 +3204,7 @@
       <c r="A25" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="B25" s="4">
+      <c r="B25" s="15">
         <v>1</v>
       </c>
       <c r="C25" s="5">
@@ -3210,7 +3223,7 @@
       <c r="A26" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="B26" s="4">
+      <c r="B26" s="15">
         <v>1</v>
       </c>
       <c r="C26" s="5">
@@ -3229,7 +3242,7 @@
       <c r="A27" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="B27" s="4">
+      <c r="B27" s="15">
         <v>1</v>
       </c>
       <c r="C27" s="5">
@@ -3248,7 +3261,7 @@
       <c r="A28" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="B28" s="4">
+      <c r="B28" s="15">
         <v>1</v>
       </c>
       <c r="C28" s="5">
@@ -3267,7 +3280,7 @@
       <c r="A29" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="B29" s="4">
+      <c r="B29" s="15">
         <v>1</v>
       </c>
       <c r="C29" s="5">
@@ -3286,7 +3299,7 @@
       <c r="A30" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="B30" s="4">
+      <c r="B30" s="15">
         <v>1</v>
       </c>
       <c r="C30" s="5">
@@ -3305,7 +3318,7 @@
       <c r="A31" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="B31" s="4">
+      <c r="B31" s="15">
         <v>1</v>
       </c>
       <c r="C31" s="5">
@@ -3324,7 +3337,7 @@
       <c r="A32" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="B32" s="4">
+      <c r="B32" s="15">
         <v>1</v>
       </c>
       <c r="C32" s="5">
@@ -3343,7 +3356,7 @@
       <c r="A33" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="B33" s="4">
+      <c r="B33" s="15">
         <v>1</v>
       </c>
       <c r="C33" s="5">
@@ -3362,7 +3375,7 @@
       <c r="A34" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="B34" s="4">
+      <c r="B34" s="15">
         <v>1</v>
       </c>
       <c r="C34" s="5">
@@ -3381,7 +3394,7 @@
       <c r="A35" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="B35" s="4">
+      <c r="B35" s="15">
         <v>1</v>
       </c>
       <c r="C35" s="5">
@@ -3400,7 +3413,7 @@
       <c r="A36" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="B36" s="4">
+      <c r="B36" s="15">
         <v>1</v>
       </c>
       <c r="C36" s="5">
@@ -3419,7 +3432,7 @@
       <c r="A37" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="B37" s="4">
+      <c r="B37" s="15">
         <v>1</v>
       </c>
       <c r="C37" s="5">
@@ -3434,17 +3447,17 @@
       </c>
       <c r="G37" s="1"/>
     </row>
-    <row r="38" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:7" ht="31" x14ac:dyDescent="0.35">
       <c r="A38" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="B38" s="4">
+      <c r="B38" s="15">
         <v>2</v>
       </c>
       <c r="C38" s="5">
         <v>44197</v>
       </c>
-      <c r="D38" s="5">
+      <c r="D38" s="14">
         <v>44228</v>
       </c>
       <c r="E38" s="5">
@@ -3459,7 +3472,7 @@
       <c r="A39" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="B39" s="4">
+      <c r="B39" s="15">
         <v>2</v>
       </c>
       <c r="C39" s="5">
@@ -5239,7 +5252,7 @@
       <c r="C236" s="1"/>
     </row>
   </sheetData>
-  <dataValidations count="1">
+  <dataValidations xWindow="821" yWindow="357" count="1">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Estado" prompt="Por favor, introduzca un valor para el estado (PENDIENTE, EN PROGRESO O REALIZADO )" sqref="F1:F39" xr:uid="{01248019-FD26-4D39-BA8E-80B22E1EE596}">
       <formula1>$N$2:$N$4</formula1>
     </dataValidation>
@@ -5254,34 +5267,37 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{25ACDF49-AC43-4CCD-856F-6ED289E70C3E}">
   <dimension ref="A2:G35"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="D30" sqref="D30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
+    <col min="1" max="1" width="13.08984375" customWidth="1"/>
     <col min="3" max="3" width="11.36328125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.08984375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.26953125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="B2" s="11" t="s">
+      <c r="B2" s="13" t="s">
         <v>52</v>
       </c>
-      <c r="C2" s="11"/>
+      <c r="C2" s="13"/>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="B3" s="12" t="s">
+      <c r="B3" s="11" t="s">
         <v>53</v>
       </c>
-      <c r="C3" s="12">
+      <c r="C3" s="11">
         <v>28</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="B4" s="12" t="s">
+      <c r="B4" s="11" t="s">
         <v>49</v>
       </c>
-      <c r="C4" s="12">
+      <c r="C4" s="11">
         <f>SUM('SPRINT-BACKLOG'!B2:B39)</f>
         <v>32</v>
       </c>
@@ -5308,7 +5324,7 @@
       <c r="A8" s="8">
         <v>44228</v>
       </c>
-      <c r="B8" s="13">
+      <c r="B8" s="12">
         <v>1</v>
       </c>
       <c r="C8" s="9">
@@ -5324,19 +5340,18 @@
         <v>30</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A9" s="8">
+    <row r="9" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A9" s="5">
         <v>44229</v>
       </c>
-      <c r="B9" s="13">
+      <c r="B9" s="12">
         <v>2</v>
       </c>
       <c r="C9" s="9">
-        <f>C8-$C$4/($C$3-1)</f>
+        <f t="shared" ref="C9:C35" si="0">C8-$C$4/($C$3-1)</f>
         <v>30.814814814814817</v>
       </c>
       <c r="D9" s="10">
-        <f>SUMIF('SPRINT-BACKLOG'!D2:D39,"="&amp;VALUE(A9),'SPRINT-BACKLOG'!B2:B39)</f>
         <v>0</v>
       </c>
       <c r="E9" s="9">
@@ -5348,15 +5363,14 @@
       <c r="A10" s="8">
         <v>44230</v>
       </c>
-      <c r="B10" s="13">
+      <c r="B10" s="12">
         <v>3</v>
       </c>
       <c r="C10" s="9">
-        <f>C9-$C$4/($C$3-1)</f>
+        <f t="shared" si="0"/>
         <v>29.629629629629633</v>
       </c>
       <c r="D10" s="10">
-        <f>SUMIF('SPRINT-BACKLOG'!D2:D39,"="&amp;VALUE(A10),'SPRINT-BACKLOG'!B2:B39)</f>
         <v>0</v>
       </c>
       <c r="E10" s="9">
@@ -5368,19 +5382,18 @@
       <c r="A11" s="8">
         <v>44231</v>
       </c>
-      <c r="B11" s="13">
+      <c r="B11" s="12">
         <v>4</v>
       </c>
       <c r="C11" s="9">
-        <f>C10-$C$4/($C$3-1)</f>
+        <f t="shared" si="0"/>
         <v>28.44444444444445</v>
       </c>
       <c r="D11" s="10">
-        <f>SUMIF('SPRINT-BACKLOG'!D2:D39,"="&amp;VALUE(A11),'SPRINT-BACKLOG'!B2:B39)</f>
         <v>0</v>
       </c>
       <c r="E11" s="9">
-        <f t="shared" ref="E11:E35" si="0">E10 - D11</f>
+        <f t="shared" ref="E11:E35" si="1">E10 - D11</f>
         <v>30</v>
       </c>
     </row>
@@ -5388,19 +5401,18 @@
       <c r="A12" s="8">
         <v>44232</v>
       </c>
-      <c r="B12" s="13">
+      <c r="B12" s="12">
         <v>5</v>
       </c>
       <c r="C12" s="9">
-        <f>C11-$C$4/($C$3-1)</f>
+        <f t="shared" si="0"/>
         <v>27.259259259259267</v>
       </c>
       <c r="D12" s="10">
-        <f>SUMIF('SPRINT-BACKLOG'!D2:D39,"="&amp;VALUE(A12),'SPRINT-BACKLOG'!B2:B39)</f>
         <v>0</v>
       </c>
       <c r="E12" s="9">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>30</v>
       </c>
     </row>
@@ -5408,19 +5420,18 @@
       <c r="A13" s="8">
         <v>44233</v>
       </c>
-      <c r="B13" s="13">
+      <c r="B13" s="12">
         <v>6</v>
       </c>
       <c r="C13" s="9">
-        <f>C12-$C$4/($C$3-1)</f>
+        <f t="shared" si="0"/>
         <v>26.074074074074083</v>
       </c>
       <c r="D13" s="10">
-        <f>SUMIF('SPRINT-BACKLOG'!D2:D39,"="&amp;VALUE(A13),'SPRINT-BACKLOG'!B2:B39)</f>
         <v>0</v>
       </c>
       <c r="E13" s="9">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>30</v>
       </c>
     </row>
@@ -5428,19 +5439,18 @@
       <c r="A14" s="8">
         <v>44234</v>
       </c>
-      <c r="B14" s="13">
+      <c r="B14" s="12">
         <v>7</v>
       </c>
       <c r="C14" s="9">
-        <f>C13-$C$4/($C$3-1)</f>
+        <f t="shared" si="0"/>
         <v>24.8888888888889</v>
       </c>
       <c r="D14" s="10">
-        <f>SUMIF('SPRINT-BACKLOG'!D2:D39,"="&amp;VALUE(A14),'SPRINT-BACKLOG'!B2:B39)</f>
         <v>0</v>
       </c>
       <c r="E14" s="9">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>30</v>
       </c>
     </row>
@@ -5448,19 +5458,18 @@
       <c r="A15" s="8">
         <v>44235</v>
       </c>
-      <c r="B15" s="13">
+      <c r="B15" s="12">
         <v>8</v>
       </c>
       <c r="C15" s="9">
-        <f>C14-$C$4/($C$3-1)</f>
+        <f t="shared" si="0"/>
         <v>23.703703703703717</v>
       </c>
       <c r="D15" s="10">
-        <f>SUMIF('SPRINT-BACKLOG'!D2:D39,"="&amp;VALUE(A15),'SPRINT-BACKLOG'!B2:B39)</f>
         <v>0</v>
       </c>
       <c r="E15" s="9">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>30</v>
       </c>
     </row>
@@ -5468,19 +5477,18 @@
       <c r="A16" s="8">
         <v>44236</v>
       </c>
-      <c r="B16" s="13">
+      <c r="B16" s="12">
         <v>9</v>
       </c>
       <c r="C16" s="9">
-        <f>C15-$C$4/($C$3-1)</f>
+        <f t="shared" si="0"/>
         <v>22.518518518518533</v>
       </c>
       <c r="D16" s="10">
-        <f>SUMIF('SPRINT-BACKLOG'!D2:D39,"="&amp;VALUE(A16),'SPRINT-BACKLOG'!B2:B39)</f>
         <v>0</v>
       </c>
       <c r="E16" s="9">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>30</v>
       </c>
     </row>
@@ -5488,11 +5496,11 @@
       <c r="A17" s="8">
         <v>44237</v>
       </c>
-      <c r="B17" s="13">
+      <c r="B17" s="12">
         <v>10</v>
       </c>
       <c r="C17" s="9">
-        <f>C16-$C$4/($C$3-1)</f>
+        <f t="shared" si="0"/>
         <v>21.33333333333335</v>
       </c>
       <c r="D17" s="10">
@@ -5500,7 +5508,7 @@
         <v>0</v>
       </c>
       <c r="E17" s="9">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>30</v>
       </c>
     </row>
@@ -5508,11 +5516,11 @@
       <c r="A18" s="8">
         <v>44238</v>
       </c>
-      <c r="B18" s="13">
+      <c r="B18" s="12">
         <v>11</v>
       </c>
       <c r="C18" s="9">
-        <f>C17-$C$4/($C$3-1)</f>
+        <f t="shared" si="0"/>
         <v>20.148148148148167</v>
       </c>
       <c r="D18" s="10">
@@ -5520,7 +5528,7 @@
         <v>0</v>
       </c>
       <c r="E18" s="9">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>30</v>
       </c>
     </row>
@@ -5528,11 +5536,11 @@
       <c r="A19" s="8">
         <v>44239</v>
       </c>
-      <c r="B19" s="13">
+      <c r="B19" s="12">
         <v>12</v>
       </c>
       <c r="C19" s="9">
-        <f>C18-$C$4/($C$3-1)</f>
+        <f t="shared" si="0"/>
         <v>18.962962962962983</v>
       </c>
       <c r="D19" s="10">
@@ -5540,7 +5548,7 @@
         <v>0</v>
       </c>
       <c r="E19" s="9">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>30</v>
       </c>
     </row>
@@ -5548,11 +5556,11 @@
       <c r="A20" s="8">
         <v>44240</v>
       </c>
-      <c r="B20" s="13">
+      <c r="B20" s="12">
         <v>13</v>
       </c>
       <c r="C20" s="9">
-        <f>C19-$C$4/($C$3-1)</f>
+        <f t="shared" si="0"/>
         <v>17.7777777777778</v>
       </c>
       <c r="D20" s="10">
@@ -5560,7 +5568,7 @@
         <v>0</v>
       </c>
       <c r="E20" s="9">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>30</v>
       </c>
     </row>
@@ -5568,11 +5576,11 @@
       <c r="A21" s="8">
         <v>44241</v>
       </c>
-      <c r="B21" s="13">
+      <c r="B21" s="12">
         <v>14</v>
       </c>
       <c r="C21" s="9">
-        <f>C20-$C$4/($C$3-1)</f>
+        <f t="shared" si="0"/>
         <v>16.592592592592617</v>
       </c>
       <c r="D21" s="10">
@@ -5580,7 +5588,7 @@
         <v>0</v>
       </c>
       <c r="E21" s="9">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>30</v>
       </c>
     </row>
@@ -5588,11 +5596,11 @@
       <c r="A22" s="8">
         <v>44242</v>
       </c>
-      <c r="B22" s="13">
+      <c r="B22" s="12">
         <v>15</v>
       </c>
       <c r="C22" s="9">
-        <f>C21-$C$4/($C$3-1)</f>
+        <f t="shared" si="0"/>
         <v>15.407407407407431</v>
       </c>
       <c r="D22" s="10">
@@ -5600,7 +5608,7 @@
         <v>0</v>
       </c>
       <c r="E22" s="9">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>30</v>
       </c>
     </row>
@@ -5608,11 +5616,11 @@
       <c r="A23" s="8">
         <v>44243</v>
       </c>
-      <c r="B23" s="13">
+      <c r="B23" s="12">
         <v>16</v>
       </c>
       <c r="C23" s="9">
-        <f>C22-$C$4/($C$3-1)</f>
+        <f t="shared" si="0"/>
         <v>14.222222222222246</v>
       </c>
       <c r="D23" s="10">
@@ -5620,7 +5628,7 @@
         <v>0</v>
       </c>
       <c r="E23" s="9">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>30</v>
       </c>
     </row>
@@ -5628,11 +5636,11 @@
       <c r="A24" s="8">
         <v>44244</v>
       </c>
-      <c r="B24" s="13">
+      <c r="B24" s="12">
         <v>17</v>
       </c>
       <c r="C24" s="9">
-        <f>C23-$C$4/($C$3-1)</f>
+        <f t="shared" si="0"/>
         <v>13.037037037037061</v>
       </c>
       <c r="D24" s="10">
@@ -5640,7 +5648,7 @@
         <v>0</v>
       </c>
       <c r="E24" s="9">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>30</v>
       </c>
     </row>
@@ -5648,11 +5656,11 @@
       <c r="A25" s="8">
         <v>44245</v>
       </c>
-      <c r="B25" s="13">
+      <c r="B25" s="12">
         <v>18</v>
       </c>
       <c r="C25" s="9">
-        <f>C24-$C$4/($C$3-1)</f>
+        <f t="shared" si="0"/>
         <v>11.851851851851876</v>
       </c>
       <c r="D25" s="10">
@@ -5660,7 +5668,7 @@
         <v>0</v>
       </c>
       <c r="E25" s="9">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>30</v>
       </c>
     </row>
@@ -5668,11 +5676,11 @@
       <c r="A26" s="8">
         <v>44246</v>
       </c>
-      <c r="B26" s="13">
+      <c r="B26" s="12">
         <v>19</v>
       </c>
       <c r="C26" s="9">
-        <f>C25-$C$4/($C$3-1)</f>
+        <f t="shared" si="0"/>
         <v>10.666666666666691</v>
       </c>
       <c r="D26" s="10">
@@ -5688,11 +5696,11 @@
       <c r="A27" s="8">
         <v>44247</v>
       </c>
-      <c r="B27" s="13">
+      <c r="B27" s="12">
         <v>20</v>
       </c>
       <c r="C27" s="9">
-        <f>C26-$C$4/($C$3-1)</f>
+        <f t="shared" si="0"/>
         <v>9.4814814814815058</v>
       </c>
       <c r="D27" s="10">
@@ -5700,7 +5708,7 @@
         <v>0</v>
       </c>
       <c r="E27" s="9">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>30</v>
       </c>
     </row>
@@ -5708,11 +5716,11 @@
       <c r="A28" s="8">
         <v>44248</v>
       </c>
-      <c r="B28" s="13">
+      <c r="B28" s="12">
         <v>21</v>
       </c>
       <c r="C28" s="9">
-        <f>C27-$C$4/($C$3-1)</f>
+        <f t="shared" si="0"/>
         <v>8.2962962962963207</v>
       </c>
       <c r="D28" s="10">
@@ -5720,7 +5728,7 @@
         <v>0</v>
       </c>
       <c r="E28" s="9">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>30</v>
       </c>
     </row>
@@ -5728,19 +5736,18 @@
       <c r="A29" s="8">
         <v>44249</v>
       </c>
-      <c r="B29" s="13">
+      <c r="B29" s="12">
         <v>22</v>
       </c>
       <c r="C29" s="9">
-        <f>C28-$C$4/($C$3-1)</f>
+        <f t="shared" si="0"/>
         <v>7.1111111111111356</v>
       </c>
       <c r="D29" s="10">
-        <f>SUMIF('SPRINT-BACKLOG'!D2:D39,"="&amp;VALUE(A29),'SPRINT-BACKLOG'!B2:B39)</f>
         <v>0</v>
       </c>
       <c r="E29" s="9">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>30</v>
       </c>
     </row>
@@ -5748,11 +5755,11 @@
       <c r="A30" s="8">
         <v>44250</v>
       </c>
-      <c r="B30" s="13">
+      <c r="B30" s="12">
         <v>23</v>
       </c>
       <c r="C30" s="9">
-        <f>C29-$C$4/($C$3-1)</f>
+        <f t="shared" si="0"/>
         <v>5.9259259259259505</v>
       </c>
       <c r="D30" s="10">
@@ -5760,7 +5767,7 @@
         <v>0</v>
       </c>
       <c r="E30" s="9">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>30</v>
       </c>
     </row>
@@ -5768,11 +5775,11 @@
       <c r="A31" s="8">
         <v>44251</v>
       </c>
-      <c r="B31" s="13">
+      <c r="B31" s="12">
         <v>24</v>
       </c>
       <c r="C31" s="9">
-        <f>C30-$C$4/($C$3-1)</f>
+        <f t="shared" si="0"/>
         <v>4.7407407407407653</v>
       </c>
       <c r="D31" s="10">
@@ -5780,7 +5787,7 @@
         <v>0</v>
       </c>
       <c r="E31" s="9">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>30</v>
       </c>
     </row>
@@ -5788,11 +5795,11 @@
       <c r="A32" s="8">
         <v>44252</v>
       </c>
-      <c r="B32" s="13">
+      <c r="B32" s="12">
         <v>25</v>
       </c>
       <c r="C32" s="9">
-        <f>C31-$C$4/($C$3-1)</f>
+        <f t="shared" si="0"/>
         <v>3.5555555555555802</v>
       </c>
       <c r="D32" s="10">
@@ -5800,7 +5807,7 @@
         <v>0</v>
       </c>
       <c r="E32" s="9">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>30</v>
       </c>
     </row>
@@ -5808,11 +5815,11 @@
       <c r="A33" s="8">
         <v>44253</v>
       </c>
-      <c r="B33" s="13">
+      <c r="B33" s="12">
         <v>26</v>
       </c>
       <c r="C33" s="9">
-        <f>C32-$C$4/($C$3-1)</f>
+        <f t="shared" si="0"/>
         <v>2.3703703703703951</v>
       </c>
       <c r="D33" s="10">
@@ -5820,7 +5827,7 @@
         <v>0</v>
       </c>
       <c r="E33" s="9">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>30</v>
       </c>
     </row>
@@ -5828,11 +5835,11 @@
       <c r="A34" s="8">
         <v>44254</v>
       </c>
-      <c r="B34" s="13">
+      <c r="B34" s="12">
         <v>27</v>
       </c>
       <c r="C34" s="9">
-        <f>C33-$C$4/($C$3-1)</f>
+        <f t="shared" si="0"/>
         <v>1.18518518518521</v>
       </c>
       <c r="D34" s="10">
@@ -5840,7 +5847,7 @@
         <v>0</v>
       </c>
       <c r="E34" s="9">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>30</v>
       </c>
     </row>
@@ -5848,11 +5855,11 @@
       <c r="A35" s="8">
         <v>44255</v>
       </c>
-      <c r="B35" s="13">
+      <c r="B35" s="12">
         <v>28</v>
       </c>
       <c r="C35" s="9">
-        <f>C34-$C$4/($C$3-1)</f>
+        <f t="shared" si="0"/>
         <v>2.4868995751603507E-14</v>
       </c>
       <c r="D35" s="10">
@@ -5860,7 +5867,7 @@
         <v>0</v>
       </c>
       <c r="E35" s="9">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>30</v>
       </c>
     </row>

</xml_diff>

<commit_message>
[IMPL] Vistas generales clientes
Implementadas las vistas generales de los clientes (particulares):
 - Vista de inicio
 - Vista de lista de solicitudes de servicio
 - Vista de formulario de solicitudes de servicio
 - Vista de lista de servicio
 - Vista de formulario de servicios
 - Vista de mi perfil
</commit_message>
<xml_diff>
--- a/documentación/Product Backlog/SP2.xlsx
+++ b/documentación/Product Backlog/SP2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alesk\Desktop\Universidad\TFG_app\TFG_app\documentación\Product Backlog\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48839E60-95D5-4D18-8289-9EC4235BB0AF}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ECCF6842-7F65-4032-B822-D4BDC78B9938}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="29610" yWindow="-120" windowWidth="19800" windowHeight="11760" activeTab="1" xr2:uid="{41FE112A-4516-4423-9CD7-320A9C032A6D}"/>
+    <workbookView xWindow="29610" yWindow="-120" windowWidth="19800" windowHeight="11760" xr2:uid="{41FE112A-4516-4423-9CD7-320A9C032A6D}"/>
   </bookViews>
   <sheets>
     <sheet name="SPRINT-BACKLOG" sheetId="1" r:id="rId1"/>
@@ -359,14 +359,14 @@
     <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="2" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -828,85 +828,85 @@
                   <c:v>30</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>30</c:v>
+                  <c:v>28</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>30</c:v>
+                  <c:v>28</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>30</c:v>
+                  <c:v>28</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>30</c:v>
+                  <c:v>28</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>30</c:v>
+                  <c:v>28</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>30</c:v>
+                  <c:v>28</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>30</c:v>
+                  <c:v>28</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>30</c:v>
+                  <c:v>28</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>30</c:v>
+                  <c:v>28</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>30</c:v>
+                  <c:v>28</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>30</c:v>
+                  <c:v>28</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>30</c:v>
+                  <c:v>28</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>30</c:v>
+                  <c:v>28</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>30</c:v>
+                  <c:v>28</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>30</c:v>
+                  <c:v>28</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>30</c:v>
+                  <c:v>28</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>30</c:v>
+                  <c:v>28</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>30</c:v>
+                  <c:v>28</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>30</c:v>
+                  <c:v>28</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>30</c:v>
+                  <c:v>28</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>30</c:v>
+                  <c:v>28</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>30</c:v>
+                  <c:v>28</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>30</c:v>
+                  <c:v>28</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>30</c:v>
+                  <c:v>28</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>30</c:v>
+                  <c:v>28</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>30</c:v>
+                  <c:v>28</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>30</c:v>
+                  <c:v>28</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2710,8 +2710,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2BB024A1-16E4-467A-A83B-A5E93171F59F}">
   <dimension ref="A1:O236"/>
   <sheetViews>
-    <sheetView topLeftCell="A40" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2743,11 +2743,11 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:15" ht="31" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:15" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A2" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="B2" s="15" t="s">
+      <c r="B2" s="14" t="s">
         <v>25</v>
       </c>
       <c r="C2" s="5">
@@ -2767,11 +2767,11 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:15" ht="31" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:15" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A3" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="15" t="s">
+      <c r="B3" s="14" t="s">
         <v>25</v>
       </c>
       <c r="C3" s="5">
@@ -2794,11 +2794,11 @@
         <v>26</v>
       </c>
     </row>
-    <row r="4" spans="1:15" ht="31" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:15" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A4" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="B4" s="15" t="s">
+      <c r="B4" s="14" t="s">
         <v>25</v>
       </c>
       <c r="C4" s="5">
@@ -2818,11 +2818,11 @@
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:15" ht="31" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:15" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A5" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="B5" s="15" t="s">
+      <c r="B5" s="14" t="s">
         <v>25</v>
       </c>
       <c r="C5" s="5">
@@ -2843,7 +2843,7 @@
       <c r="A6" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="B6" s="15" t="s">
+      <c r="B6" s="14" t="s">
         <v>27</v>
       </c>
       <c r="C6" s="5">
@@ -2862,7 +2862,7 @@
       <c r="A7" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="B7" s="15" t="s">
+      <c r="B7" s="14" t="s">
         <v>27</v>
       </c>
       <c r="C7" s="5">
@@ -2881,7 +2881,7 @@
       <c r="A8" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="B8" s="15" t="s">
+      <c r="B8" s="14" t="s">
         <v>27</v>
       </c>
       <c r="C8" s="5">
@@ -2900,7 +2900,7 @@
       <c r="A9" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="B9" s="15" t="s">
+      <c r="B9" s="14" t="s">
         <v>27</v>
       </c>
       <c r="C9" s="5">
@@ -2919,7 +2919,7 @@
       <c r="A10" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="B10" s="15">
+      <c r="B10" s="14">
         <v>1</v>
       </c>
       <c r="C10" s="5">
@@ -2938,7 +2938,7 @@
       <c r="A11" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="B11" s="15">
+      <c r="B11" s="14">
         <v>1</v>
       </c>
       <c r="C11" s="5">
@@ -2957,7 +2957,7 @@
       <c r="A12" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="B12" s="15">
+      <c r="B12" s="14">
         <v>1</v>
       </c>
       <c r="C12" s="5">
@@ -2976,7 +2976,7 @@
       <c r="A13" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="B13" s="15">
+      <c r="B13" s="14">
         <v>1</v>
       </c>
       <c r="C13" s="5">
@@ -2995,7 +2995,7 @@
       <c r="A14" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="B14" s="15">
+      <c r="B14" s="14">
         <v>1</v>
       </c>
       <c r="C14" s="5">
@@ -3014,7 +3014,7 @@
       <c r="A15" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="B15" s="15">
+      <c r="B15" s="14">
         <v>1</v>
       </c>
       <c r="C15" s="5">
@@ -3033,7 +3033,7 @@
       <c r="A16" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="B16" s="15">
+      <c r="B16" s="14">
         <v>1</v>
       </c>
       <c r="C16" s="5">
@@ -3052,7 +3052,7 @@
       <c r="A17" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="B17" s="15">
+      <c r="B17" s="14">
         <v>1</v>
       </c>
       <c r="C17" s="5">
@@ -3071,7 +3071,7 @@
       <c r="A18" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="B18" s="15">
+      <c r="B18" s="14">
         <v>1</v>
       </c>
       <c r="C18" s="5">
@@ -3090,7 +3090,7 @@
       <c r="A19" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="B19" s="15">
+      <c r="B19" s="14">
         <v>1</v>
       </c>
       <c r="C19" s="5">
@@ -3109,7 +3109,7 @@
       <c r="A20" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="B20" s="15">
+      <c r="B20" s="14">
         <v>1</v>
       </c>
       <c r="C20" s="5">
@@ -3128,7 +3128,7 @@
       <c r="A21" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="B21" s="15">
+      <c r="B21" s="14">
         <v>1</v>
       </c>
       <c r="C21" s="5">
@@ -3147,7 +3147,7 @@
       <c r="A22" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="B22" s="15">
+      <c r="B22" s="14">
         <v>1</v>
       </c>
       <c r="C22" s="5">
@@ -3166,7 +3166,7 @@
       <c r="A23" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="B23" s="15">
+      <c r="B23" s="14">
         <v>1</v>
       </c>
       <c r="C23" s="5">
@@ -3185,7 +3185,7 @@
       <c r="A24" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="B24" s="15">
+      <c r="B24" s="14">
         <v>1</v>
       </c>
       <c r="C24" s="5">
@@ -3204,7 +3204,7 @@
       <c r="A25" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="B25" s="15">
+      <c r="B25" s="14">
         <v>1</v>
       </c>
       <c r="C25" s="5">
@@ -3223,7 +3223,7 @@
       <c r="A26" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="B26" s="15">
+      <c r="B26" s="14">
         <v>1</v>
       </c>
       <c r="C26" s="5">
@@ -3242,7 +3242,7 @@
       <c r="A27" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="B27" s="15">
+      <c r="B27" s="14">
         <v>1</v>
       </c>
       <c r="C27" s="5">
@@ -3261,7 +3261,7 @@
       <c r="A28" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="B28" s="15">
+      <c r="B28" s="14">
         <v>1</v>
       </c>
       <c r="C28" s="5">
@@ -3280,7 +3280,7 @@
       <c r="A29" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="B29" s="15">
+      <c r="B29" s="14">
         <v>1</v>
       </c>
       <c r="C29" s="5">
@@ -3299,7 +3299,7 @@
       <c r="A30" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="B30" s="15">
+      <c r="B30" s="14">
         <v>1</v>
       </c>
       <c r="C30" s="5">
@@ -3318,7 +3318,7 @@
       <c r="A31" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="B31" s="15">
+      <c r="B31" s="14">
         <v>1</v>
       </c>
       <c r="C31" s="5">
@@ -3337,7 +3337,7 @@
       <c r="A32" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="B32" s="15">
+      <c r="B32" s="14">
         <v>1</v>
       </c>
       <c r="C32" s="5">
@@ -3356,7 +3356,7 @@
       <c r="A33" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="B33" s="15">
+      <c r="B33" s="14">
         <v>1</v>
       </c>
       <c r="C33" s="5">
@@ -3375,7 +3375,7 @@
       <c r="A34" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="B34" s="15">
+      <c r="B34" s="14">
         <v>1</v>
       </c>
       <c r="C34" s="5">
@@ -3394,7 +3394,7 @@
       <c r="A35" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="B35" s="15">
+      <c r="B35" s="14">
         <v>1</v>
       </c>
       <c r="C35" s="5">
@@ -3413,7 +3413,7 @@
       <c r="A36" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="B36" s="15">
+      <c r="B36" s="14">
         <v>1</v>
       </c>
       <c r="C36" s="5">
@@ -3432,7 +3432,7 @@
       <c r="A37" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="B37" s="15">
+      <c r="B37" s="14">
         <v>1</v>
       </c>
       <c r="C37" s="5">
@@ -3447,17 +3447,17 @@
       </c>
       <c r="G37" s="1"/>
     </row>
-    <row r="38" spans="1:7" ht="31" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A38" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="B38" s="15">
+      <c r="B38" s="14">
         <v>2</v>
       </c>
       <c r="C38" s="5">
         <v>44197</v>
       </c>
-      <c r="D38" s="14">
+      <c r="D38" s="13">
         <v>44228</v>
       </c>
       <c r="E38" s="5">
@@ -3472,7 +3472,7 @@
       <c r="A39" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="B39" s="15">
+      <c r="B39" s="14">
         <v>2</v>
       </c>
       <c r="C39" s="5">
@@ -5267,8 +5267,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{25ACDF49-AC43-4CCD-856F-6ED289E70C3E}">
   <dimension ref="A2:G35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="D30" sqref="D30"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -5280,10 +5280,10 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="B2" s="13" t="s">
+      <c r="B2" s="15" t="s">
         <v>52</v>
       </c>
-      <c r="C2" s="13"/>
+      <c r="C2" s="15"/>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.35">
       <c r="B3" s="11" t="s">
@@ -5352,11 +5352,11 @@
         <v>30.814814814814817</v>
       </c>
       <c r="D9" s="10">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E9" s="9">
         <f>E8 - D9</f>
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.35">
@@ -5375,7 +5375,7 @@
       </c>
       <c r="E10" s="9">
         <f>E9 - D10</f>
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.35">
@@ -5394,7 +5394,7 @@
       </c>
       <c r="E11" s="9">
         <f t="shared" ref="E11:E35" si="1">E10 - D11</f>
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.35">
@@ -5413,7 +5413,7 @@
       </c>
       <c r="E12" s="9">
         <f t="shared" si="1"/>
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.35">
@@ -5432,7 +5432,7 @@
       </c>
       <c r="E13" s="9">
         <f t="shared" si="1"/>
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.35">
@@ -5451,7 +5451,7 @@
       </c>
       <c r="E14" s="9">
         <f t="shared" si="1"/>
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.35">
@@ -5470,7 +5470,7 @@
       </c>
       <c r="E15" s="9">
         <f t="shared" si="1"/>
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.35">
@@ -5489,7 +5489,7 @@
       </c>
       <c r="E16" s="9">
         <f t="shared" si="1"/>
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.35">
@@ -5509,7 +5509,7 @@
       </c>
       <c r="E17" s="9">
         <f t="shared" si="1"/>
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.35">
@@ -5529,7 +5529,7 @@
       </c>
       <c r="E18" s="9">
         <f t="shared" si="1"/>
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.35">
@@ -5549,7 +5549,7 @@
       </c>
       <c r="E19" s="9">
         <f t="shared" si="1"/>
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.35">
@@ -5569,7 +5569,7 @@
       </c>
       <c r="E20" s="9">
         <f t="shared" si="1"/>
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.35">
@@ -5589,7 +5589,7 @@
       </c>
       <c r="E21" s="9">
         <f t="shared" si="1"/>
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.35">
@@ -5609,7 +5609,7 @@
       </c>
       <c r="E22" s="9">
         <f t="shared" si="1"/>
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.35">
@@ -5629,7 +5629,7 @@
       </c>
       <c r="E23" s="9">
         <f t="shared" si="1"/>
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.35">
@@ -5649,7 +5649,7 @@
       </c>
       <c r="E24" s="9">
         <f t="shared" si="1"/>
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.35">
@@ -5669,7 +5669,7 @@
       </c>
       <c r="E25" s="9">
         <f t="shared" si="1"/>
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.35">
@@ -5689,7 +5689,7 @@
       </c>
       <c r="E26" s="9">
         <f>E25 - D26</f>
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.35">
@@ -5709,7 +5709,7 @@
       </c>
       <c r="E27" s="9">
         <f t="shared" si="1"/>
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.35">
@@ -5729,7 +5729,7 @@
       </c>
       <c r="E28" s="9">
         <f t="shared" si="1"/>
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.35">
@@ -5748,7 +5748,7 @@
       </c>
       <c r="E29" s="9">
         <f t="shared" si="1"/>
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.35">
@@ -5768,7 +5768,7 @@
       </c>
       <c r="E30" s="9">
         <f t="shared" si="1"/>
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.35">
@@ -5788,7 +5788,7 @@
       </c>
       <c r="E31" s="9">
         <f t="shared" si="1"/>
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.35">
@@ -5808,7 +5808,7 @@
       </c>
       <c r="E32" s="9">
         <f t="shared" si="1"/>
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.35">
@@ -5828,7 +5828,7 @@
       </c>
       <c r="E33" s="9">
         <f t="shared" si="1"/>
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.35">
@@ -5848,7 +5848,7 @@
       </c>
       <c r="E34" s="9">
         <f t="shared" si="1"/>
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.35">
@@ -5868,7 +5868,7 @@
       </c>
       <c r="E35" s="9">
         <f t="shared" si="1"/>
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
[IMPL] Vista general para el rol de empresa Implementada la vista general para el rol de empresa:  - Vista de inicio  - Vista de lista de solicitudes de servicio  - Vista de formulario de solicitudes de servicio  - Vista de lista de servicio  - Vista de formulario de servicios  - Vista de mi perfil
</commit_message>
<xml_diff>
--- a/documentación/Product Backlog/SP2.xlsx
+++ b/documentación/Product Backlog/SP2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alesk\Desktop\Universidad\TFG_app\TFG_app\documentación\Product Backlog\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ECCF6842-7F65-4032-B822-D4BDC78B9938}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7143F325-4B36-447F-8402-9C6C7CBD7CD0}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="29610" yWindow="-120" windowWidth="19800" windowHeight="11760" xr2:uid="{41FE112A-4516-4423-9CD7-320A9C032A6D}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="56">
   <si>
     <t>Puntos de historia</t>
   </si>
@@ -201,6 +201,9 @@
   </si>
   <si>
     <t>Días</t>
+  </si>
+  <si>
+    <t>Creación de la vista principal (TRA)</t>
   </si>
 </sst>
 </file>
@@ -834,79 +837,79 @@
                   <c:v>28</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>28</c:v>
+                  <c:v>25</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>28</c:v>
+                  <c:v>25</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>28</c:v>
+                  <c:v>25</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>28</c:v>
+                  <c:v>25</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>28</c:v>
+                  <c:v>25</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>28</c:v>
+                  <c:v>25</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>28</c:v>
+                  <c:v>25</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>28</c:v>
+                  <c:v>25</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>28</c:v>
+                  <c:v>25</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>28</c:v>
+                  <c:v>25</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>28</c:v>
+                  <c:v>25</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>28</c:v>
+                  <c:v>25</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>28</c:v>
+                  <c:v>25</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>28</c:v>
+                  <c:v>25</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>28</c:v>
+                  <c:v>25</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>28</c:v>
+                  <c:v>25</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>28</c:v>
+                  <c:v>25</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>28</c:v>
+                  <c:v>25</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>28</c:v>
+                  <c:v>25</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>28</c:v>
+                  <c:v>25</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>28</c:v>
+                  <c:v>25</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>28</c:v>
+                  <c:v>25</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>28</c:v>
+                  <c:v>25</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>28</c:v>
+                  <c:v>25</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>28</c:v>
+                  <c:v>25</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2710,8 +2713,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2BB024A1-16E4-467A-A83B-A5E93171F59F}">
   <dimension ref="A1:O236"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+    <sheetView tabSelected="1" topLeftCell="A43" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2849,7 +2852,9 @@
       <c r="C6" s="5">
         <v>44229</v>
       </c>
-      <c r="D6" s="5"/>
+      <c r="D6" s="5">
+        <v>44231</v>
+      </c>
       <c r="E6" s="5">
         <v>44230</v>
       </c>
@@ -2879,7 +2884,7 @@
     </row>
     <row r="8" spans="1:15" ht="31" x14ac:dyDescent="0.35">
       <c r="A8" s="3" t="s">
-        <v>29</v>
+        <v>55</v>
       </c>
       <c r="B8" s="14" t="s">
         <v>27</v>
@@ -5268,7 +5273,7 @@
   <dimension ref="A2:G35"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -5390,11 +5395,11 @@
         <v>28.44444444444445</v>
       </c>
       <c r="D11" s="10">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E11" s="9">
         <f t="shared" ref="E11:E35" si="1">E10 - D11</f>
-        <v>28</v>
+        <v>25</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.35">
@@ -5413,7 +5418,7 @@
       </c>
       <c r="E12" s="9">
         <f t="shared" si="1"/>
-        <v>28</v>
+        <v>25</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.35">
@@ -5432,7 +5437,7 @@
       </c>
       <c r="E13" s="9">
         <f t="shared" si="1"/>
-        <v>28</v>
+        <v>25</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.35">
@@ -5451,7 +5456,7 @@
       </c>
       <c r="E14" s="9">
         <f t="shared" si="1"/>
-        <v>28</v>
+        <v>25</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.35">
@@ -5470,7 +5475,7 @@
       </c>
       <c r="E15" s="9">
         <f t="shared" si="1"/>
-        <v>28</v>
+        <v>25</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.35">
@@ -5489,7 +5494,7 @@
       </c>
       <c r="E16" s="9">
         <f t="shared" si="1"/>
-        <v>28</v>
+        <v>25</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.35">
@@ -5509,7 +5514,7 @@
       </c>
       <c r="E17" s="9">
         <f t="shared" si="1"/>
-        <v>28</v>
+        <v>25</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.35">
@@ -5529,7 +5534,7 @@
       </c>
       <c r="E18" s="9">
         <f t="shared" si="1"/>
-        <v>28</v>
+        <v>25</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.35">
@@ -5549,7 +5554,7 @@
       </c>
       <c r="E19" s="9">
         <f t="shared" si="1"/>
-        <v>28</v>
+        <v>25</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.35">
@@ -5569,7 +5574,7 @@
       </c>
       <c r="E20" s="9">
         <f t="shared" si="1"/>
-        <v>28</v>
+        <v>25</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.35">
@@ -5589,7 +5594,7 @@
       </c>
       <c r="E21" s="9">
         <f t="shared" si="1"/>
-        <v>28</v>
+        <v>25</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.35">
@@ -5609,7 +5614,7 @@
       </c>
       <c r="E22" s="9">
         <f t="shared" si="1"/>
-        <v>28</v>
+        <v>25</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.35">
@@ -5629,7 +5634,7 @@
       </c>
       <c r="E23" s="9">
         <f t="shared" si="1"/>
-        <v>28</v>
+        <v>25</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.35">
@@ -5649,7 +5654,7 @@
       </c>
       <c r="E24" s="9">
         <f t="shared" si="1"/>
-        <v>28</v>
+        <v>25</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.35">
@@ -5669,7 +5674,7 @@
       </c>
       <c r="E25" s="9">
         <f t="shared" si="1"/>
-        <v>28</v>
+        <v>25</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.35">
@@ -5689,7 +5694,7 @@
       </c>
       <c r="E26" s="9">
         <f>E25 - D26</f>
-        <v>28</v>
+        <v>25</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.35">
@@ -5709,7 +5714,7 @@
       </c>
       <c r="E27" s="9">
         <f t="shared" si="1"/>
-        <v>28</v>
+        <v>25</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.35">
@@ -5729,7 +5734,7 @@
       </c>
       <c r="E28" s="9">
         <f t="shared" si="1"/>
-        <v>28</v>
+        <v>25</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.35">
@@ -5748,7 +5753,7 @@
       </c>
       <c r="E29" s="9">
         <f t="shared" si="1"/>
-        <v>28</v>
+        <v>25</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.35">
@@ -5768,7 +5773,7 @@
       </c>
       <c r="E30" s="9">
         <f t="shared" si="1"/>
-        <v>28</v>
+        <v>25</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.35">
@@ -5788,7 +5793,7 @@
       </c>
       <c r="E31" s="9">
         <f t="shared" si="1"/>
-        <v>28</v>
+        <v>25</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.35">
@@ -5808,7 +5813,7 @@
       </c>
       <c r="E32" s="9">
         <f t="shared" si="1"/>
-        <v>28</v>
+        <v>25</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.35">
@@ -5828,7 +5833,7 @@
       </c>
       <c r="E33" s="9">
         <f t="shared" si="1"/>
-        <v>28</v>
+        <v>25</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.35">
@@ -5848,7 +5853,7 @@
       </c>
       <c r="E34" s="9">
         <f t="shared" si="1"/>
-        <v>28</v>
+        <v>25</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.35">
@@ -5868,7 +5873,7 @@
       </c>
       <c r="E35" s="9">
         <f t="shared" si="1"/>
-        <v>28</v>
+        <v>25</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
[IMPL] CRUD Solicitud de Servicio cliente Se ha implementado el CRUD de Solicitud de Servicio para el rol de cliente. Funcionalidades añadidas:  - Crear una nueva solicitud  - Listar todas las solicitudes  - Ver los detalles de una solicitud  - Editar una solicitud
</commit_message>
<xml_diff>
--- a/documentación/Product Backlog/SP2.xlsx
+++ b/documentación/Product Backlog/SP2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alesk\Desktop\Universidad\TFG_app\TFG_app\documentación\Product Backlog\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7143F325-4B36-447F-8402-9C6C7CBD7CD0}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF921087-FB0F-41D0-9B8A-517BCC7CA22A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="29610" yWindow="-120" windowWidth="19800" windowHeight="11760" xr2:uid="{41FE112A-4516-4423-9CD7-320A9C032A6D}"/>
+    <workbookView xWindow="820" yWindow="-110" windowWidth="18490" windowHeight="11020" xr2:uid="{41FE112A-4516-4423-9CD7-320A9C032A6D}"/>
   </bookViews>
   <sheets>
     <sheet name="SPRINT-BACKLOG" sheetId="1" r:id="rId1"/>
@@ -837,79 +837,79 @@
                   <c:v>28</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>25</c:v>
+                  <c:v>23</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>25</c:v>
+                  <c:v>23</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>25</c:v>
+                  <c:v>22</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>25</c:v>
+                  <c:v>22</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>25</c:v>
+                  <c:v>22</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>25</c:v>
+                  <c:v>22</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>25</c:v>
+                  <c:v>22</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>25</c:v>
+                  <c:v>22</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>25</c:v>
+                  <c:v>22</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>25</c:v>
+                  <c:v>22</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>25</c:v>
+                  <c:v>22</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>25</c:v>
+                  <c:v>22</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>25</c:v>
+                  <c:v>22</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>25</c:v>
+                  <c:v>22</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>25</c:v>
+                  <c:v>22</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>25</c:v>
+                  <c:v>22</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>25</c:v>
+                  <c:v>22</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>25</c:v>
+                  <c:v>22</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>25</c:v>
+                  <c:v>22</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>25</c:v>
+                  <c:v>22</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>25</c:v>
+                  <c:v>22</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>25</c:v>
+                  <c:v>22</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>25</c:v>
+                  <c:v>22</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>25</c:v>
+                  <c:v>22</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>25</c:v>
+                  <c:v>22</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2713,8 +2713,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2BB024A1-16E4-467A-A83B-A5E93171F59F}">
   <dimension ref="A1:O236"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A43" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2873,7 +2873,9 @@
       <c r="C7" s="5">
         <v>44229</v>
       </c>
-      <c r="D7" s="5"/>
+      <c r="D7" s="5">
+        <v>44231</v>
+      </c>
       <c r="E7" s="5">
         <v>44230</v>
       </c>
@@ -2930,7 +2932,9 @@
       <c r="C10" s="5">
         <v>44231</v>
       </c>
-      <c r="D10" s="5"/>
+      <c r="D10" s="5">
+        <v>44231</v>
+      </c>
       <c r="E10" s="5">
         <v>44232</v>
       </c>
@@ -2949,7 +2953,9 @@
       <c r="C11" s="5">
         <v>44231</v>
       </c>
-      <c r="D11" s="5"/>
+      <c r="D11" s="5">
+        <v>44231</v>
+      </c>
       <c r="E11" s="5">
         <v>44232</v>
       </c>
@@ -2987,7 +2993,9 @@
       <c r="C13" s="5">
         <v>44232</v>
       </c>
-      <c r="D13" s="5"/>
+      <c r="D13" s="5">
+        <v>44233</v>
+      </c>
       <c r="E13" s="5">
         <v>44235</v>
       </c>
@@ -5273,7 +5281,7 @@
   <dimension ref="A2:G35"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -5395,11 +5403,11 @@
         <v>28.44444444444445</v>
       </c>
       <c r="D11" s="10">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="E11" s="9">
         <f t="shared" ref="E11:E35" si="1">E10 - D11</f>
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.35">
@@ -5418,7 +5426,7 @@
       </c>
       <c r="E12" s="9">
         <f t="shared" si="1"/>
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.35">
@@ -5433,11 +5441,11 @@
         <v>26.074074074074083</v>
       </c>
       <c r="D13" s="10">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E13" s="9">
         <f t="shared" si="1"/>
-        <v>25</v>
+        <v>22</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.35">
@@ -5456,7 +5464,7 @@
       </c>
       <c r="E14" s="9">
         <f t="shared" si="1"/>
-        <v>25</v>
+        <v>22</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.35">
@@ -5475,7 +5483,7 @@
       </c>
       <c r="E15" s="9">
         <f t="shared" si="1"/>
-        <v>25</v>
+        <v>22</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.35">
@@ -5494,7 +5502,7 @@
       </c>
       <c r="E16" s="9">
         <f t="shared" si="1"/>
-        <v>25</v>
+        <v>22</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.35">
@@ -5514,7 +5522,7 @@
       </c>
       <c r="E17" s="9">
         <f t="shared" si="1"/>
-        <v>25</v>
+        <v>22</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.35">
@@ -5534,7 +5542,7 @@
       </c>
       <c r="E18" s="9">
         <f t="shared" si="1"/>
-        <v>25</v>
+        <v>22</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.35">
@@ -5554,7 +5562,7 @@
       </c>
       <c r="E19" s="9">
         <f t="shared" si="1"/>
-        <v>25</v>
+        <v>22</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.35">
@@ -5574,7 +5582,7 @@
       </c>
       <c r="E20" s="9">
         <f t="shared" si="1"/>
-        <v>25</v>
+        <v>22</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.35">
@@ -5594,7 +5602,7 @@
       </c>
       <c r="E21" s="9">
         <f t="shared" si="1"/>
-        <v>25</v>
+        <v>22</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.35">
@@ -5614,7 +5622,7 @@
       </c>
       <c r="E22" s="9">
         <f t="shared" si="1"/>
-        <v>25</v>
+        <v>22</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.35">
@@ -5634,7 +5642,7 @@
       </c>
       <c r="E23" s="9">
         <f t="shared" si="1"/>
-        <v>25</v>
+        <v>22</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.35">
@@ -5654,7 +5662,7 @@
       </c>
       <c r="E24" s="9">
         <f t="shared" si="1"/>
-        <v>25</v>
+        <v>22</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.35">
@@ -5674,7 +5682,7 @@
       </c>
       <c r="E25" s="9">
         <f t="shared" si="1"/>
-        <v>25</v>
+        <v>22</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.35">
@@ -5694,7 +5702,7 @@
       </c>
       <c r="E26" s="9">
         <f>E25 - D26</f>
-        <v>25</v>
+        <v>22</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.35">
@@ -5714,7 +5722,7 @@
       </c>
       <c r="E27" s="9">
         <f t="shared" si="1"/>
-        <v>25</v>
+        <v>22</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.35">
@@ -5734,7 +5742,7 @@
       </c>
       <c r="E28" s="9">
         <f t="shared" si="1"/>
-        <v>25</v>
+        <v>22</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.35">
@@ -5753,7 +5761,7 @@
       </c>
       <c r="E29" s="9">
         <f t="shared" si="1"/>
-        <v>25</v>
+        <v>22</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.35">
@@ -5773,7 +5781,7 @@
       </c>
       <c r="E30" s="9">
         <f t="shared" si="1"/>
-        <v>25</v>
+        <v>22</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.35">
@@ -5793,7 +5801,7 @@
       </c>
       <c r="E31" s="9">
         <f t="shared" si="1"/>
-        <v>25</v>
+        <v>22</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.35">
@@ -5813,7 +5821,7 @@
       </c>
       <c r="E32" s="9">
         <f t="shared" si="1"/>
-        <v>25</v>
+        <v>22</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.35">
@@ -5833,7 +5841,7 @@
       </c>
       <c r="E33" s="9">
         <f t="shared" si="1"/>
-        <v>25</v>
+        <v>22</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.35">
@@ -5853,7 +5861,7 @@
       </c>
       <c r="E34" s="9">
         <f t="shared" si="1"/>
-        <v>25</v>
+        <v>22</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.35">
@@ -5873,7 +5881,7 @@
       </c>
       <c r="E35" s="9">
         <f t="shared" si="1"/>
-        <v>25</v>
+        <v>22</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
[MOD][IMPL] Mi perfil / Servicios Se ha modificado el apartado de mi perfil con el objetivo de poder editar los campos de un cliente. Falta añadir las restricciones del formulario. Se ha implementado la funcionalidad de ver los detalles de un servicio.
</commit_message>
<xml_diff>
--- a/documentación/Product Backlog/SP2.xlsx
+++ b/documentación/Product Backlog/SP2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alesk\Desktop\Universidad\TFG_app\TFG_app\documentación\Product Backlog\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF921087-FB0F-41D0-9B8A-517BCC7CA22A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27948566-F67F-4B91-AD15-0EA5148155B8}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="820" yWindow="-110" windowWidth="18490" windowHeight="11020" xr2:uid="{41FE112A-4516-4423-9CD7-320A9C032A6D}"/>
+    <workbookView xWindow="29610" yWindow="-120" windowWidth="19800" windowHeight="11760" xr2:uid="{41FE112A-4516-4423-9CD7-320A9C032A6D}"/>
   </bookViews>
   <sheets>
     <sheet name="SPRINT-BACKLOG" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="55">
   <si>
     <t>Puntos de historia</t>
   </si>
@@ -132,9 +132,6 @@
   </si>
   <si>
     <t>Implementación de la funcionalidad de visualizar los detalles de un Servicio (CLI)</t>
-  </si>
-  <si>
-    <t>Implementación de la funcionalidad de modificar los detalles de un Servicio (CLI)</t>
   </si>
   <si>
     <t>Implementación de la funcionalidad de visualizar los detalles de un Servicio (EMP)</t>
@@ -704,88 +701,88 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="28"/>
                 <c:pt idx="0">
-                  <c:v>32</c:v>
+                  <c:v>31</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>30.814814814814817</c:v>
+                  <c:v>29.851851851851851</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>29.629629629629633</c:v>
+                  <c:v>28.703703703703702</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>28.44444444444445</c:v>
+                  <c:v>27.555555555555554</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>27.259259259259267</c:v>
+                  <c:v>26.407407407407405</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>26.074074074074083</c:v>
+                  <c:v>25.259259259259256</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>24.8888888888889</c:v>
+                  <c:v>24.111111111111107</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>23.703703703703717</c:v>
+                  <c:v>22.962962962962958</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>22.518518518518533</c:v>
+                  <c:v>21.81481481481481</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>21.33333333333335</c:v>
+                  <c:v>20.666666666666661</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>20.148148148148167</c:v>
+                  <c:v>19.518518518518512</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>18.962962962962983</c:v>
+                  <c:v>18.370370370370363</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>17.7777777777778</c:v>
+                  <c:v>17.222222222222214</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>16.592592592592617</c:v>
+                  <c:v>16.074074074074066</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>15.407407407407431</c:v>
+                  <c:v>14.925925925925917</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>14.222222222222246</c:v>
+                  <c:v>13.777777777777768</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>13.037037037037061</c:v>
+                  <c:v>12.629629629629619</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>11.851851851851876</c:v>
+                  <c:v>11.48148148148147</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>10.666666666666691</c:v>
+                  <c:v>10.333333333333321</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>9.4814814814815058</c:v>
+                  <c:v>9.1851851851851727</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>8.2962962962963207</c:v>
+                  <c:v>8.0370370370370239</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>7.1111111111111356</c:v>
+                  <c:v>6.888888888888876</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>5.9259259259259505</c:v>
+                  <c:v>5.740740740740728</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>4.7407407407407653</c:v>
+                  <c:v>4.5925925925925801</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>3.5555555555555802</c:v>
+                  <c:v>3.4444444444444322</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>2.3703703703703951</c:v>
+                  <c:v>2.2962962962962843</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>1.18518518518521</c:v>
+                  <c:v>1.1481481481481361</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>2.4868995751603507E-14</c:v>
+                  <c:v>-1.1990408665951691E-14</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -828,88 +825,88 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="28"/>
                 <c:pt idx="0">
-                  <c:v>30</c:v>
+                  <c:v>29</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>28</c:v>
+                  <c:v>27</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>28</c:v>
+                  <c:v>27</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>23</c:v>
+                  <c:v>22</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>23</c:v>
+                  <c:v>22</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>22</c:v>
+                  <c:v>21</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>22</c:v>
+                  <c:v>21</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>22</c:v>
+                  <c:v>18</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>22</c:v>
+                  <c:v>16</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>22</c:v>
+                  <c:v>16</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>22</c:v>
+                  <c:v>16</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>22</c:v>
+                  <c:v>16</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>22</c:v>
+                  <c:v>16</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>22</c:v>
+                  <c:v>16</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>22</c:v>
+                  <c:v>16</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>22</c:v>
+                  <c:v>16</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>22</c:v>
+                  <c:v>16</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>22</c:v>
+                  <c:v>16</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>22</c:v>
+                  <c:v>16</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>22</c:v>
+                  <c:v>16</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>22</c:v>
+                  <c:v>16</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>22</c:v>
+                  <c:v>16</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>22</c:v>
+                  <c:v>16</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>22</c:v>
+                  <c:v>16</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>22</c:v>
+                  <c:v>16</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>22</c:v>
+                  <c:v>16</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>22</c:v>
+                  <c:v>16</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>22</c:v>
+                  <c:v>16</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2379,13 +2376,13 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>39</xdr:row>
+      <xdr:row>38</xdr:row>
       <xdr:rowOff>160336</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
       <xdr:colOff>752475</xdr:colOff>
-      <xdr:row>64</xdr:row>
+      <xdr:row>63</xdr:row>
       <xdr:rowOff>9524</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -2711,10 +2708,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2BB024A1-16E4-467A-A83B-A5E93171F59F}">
-  <dimension ref="A1:O236"/>
+  <dimension ref="A1:O235"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A14" sqref="A14:XFD14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2886,7 +2883,7 @@
     </row>
     <row r="8" spans="1:15" ht="31" x14ac:dyDescent="0.35">
       <c r="A8" s="3" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B8" s="14" t="s">
         <v>27</v>
@@ -2924,7 +2921,7 @@
     </row>
     <row r="10" spans="1:15" ht="31" x14ac:dyDescent="0.35">
       <c r="A10" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B10" s="14">
         <v>1</v>
@@ -2945,7 +2942,7 @@
     </row>
     <row r="11" spans="1:15" ht="31" x14ac:dyDescent="0.35">
       <c r="A11" s="3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B11" s="14">
         <v>1</v>
@@ -2974,7 +2971,9 @@
       <c r="C12" s="5">
         <v>44231</v>
       </c>
-      <c r="D12" s="5"/>
+      <c r="D12" s="5">
+        <v>44235</v>
+      </c>
       <c r="E12" s="5">
         <v>44232</v>
       </c>
@@ -3014,7 +3013,9 @@
       <c r="C14" s="5">
         <v>44232</v>
       </c>
-      <c r="D14" s="5"/>
+      <c r="D14" s="5">
+        <v>44234</v>
+      </c>
       <c r="E14" s="5">
         <v>44235</v>
       </c>
@@ -3033,7 +3034,9 @@
       <c r="C15" s="5">
         <v>44235</v>
       </c>
-      <c r="D15" s="5"/>
+      <c r="D15" s="5">
+        <v>44234</v>
+      </c>
       <c r="E15" s="5">
         <v>44236</v>
       </c>
@@ -3044,17 +3047,19 @@
     </row>
     <row r="16" spans="1:15" ht="31" x14ac:dyDescent="0.35">
       <c r="A16" s="3" t="s">
-        <v>18</v>
+        <v>43</v>
       </c>
       <c r="B16" s="14">
         <v>1</v>
       </c>
       <c r="C16" s="5">
+        <v>44239</v>
+      </c>
+      <c r="D16" s="5">
         <v>44235</v>
       </c>
-      <c r="D16" s="5"/>
       <c r="E16" s="5">
-        <v>44236</v>
+        <v>44242</v>
       </c>
       <c r="F16" s="4" t="s">
         <v>5</v>
@@ -3063,17 +3068,19 @@
     </row>
     <row r="17" spans="1:7" ht="31" x14ac:dyDescent="0.35">
       <c r="A17" s="3" t="s">
-        <v>19</v>
+        <v>44</v>
       </c>
       <c r="B17" s="14">
         <v>1</v>
       </c>
       <c r="C17" s="5">
-        <v>44236</v>
-      </c>
-      <c r="D17" s="5"/>
+        <v>44242</v>
+      </c>
+      <c r="D17" s="5">
+        <v>44235</v>
+      </c>
       <c r="E17" s="5">
-        <v>44237</v>
+        <v>44243</v>
       </c>
       <c r="F17" s="4" t="s">
         <v>5</v>
@@ -3082,17 +3089,19 @@
     </row>
     <row r="18" spans="1:7" ht="31" x14ac:dyDescent="0.35">
       <c r="A18" s="3" t="s">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="B18" s="14">
         <v>1</v>
       </c>
       <c r="C18" s="5">
+        <v>44242</v>
+      </c>
+      <c r="D18" s="5">
         <v>44236</v>
       </c>
-      <c r="D18" s="5"/>
       <c r="E18" s="5">
-        <v>44237</v>
+        <v>44243</v>
       </c>
       <c r="F18" s="4" t="s">
         <v>5</v>
@@ -3101,17 +3110,19 @@
     </row>
     <row r="19" spans="1:7" ht="31" x14ac:dyDescent="0.35">
       <c r="A19" s="3" t="s">
-        <v>21</v>
+        <v>31</v>
       </c>
       <c r="B19" s="14">
         <v>1</v>
       </c>
       <c r="C19" s="5">
-        <v>44237</v>
-      </c>
-      <c r="D19" s="5"/>
+        <v>44243</v>
+      </c>
+      <c r="D19" s="5">
+        <v>44236</v>
+      </c>
       <c r="E19" s="5">
-        <v>44238</v>
+        <v>44244</v>
       </c>
       <c r="F19" s="4" t="s">
         <v>5</v>
@@ -3120,17 +3131,17 @@
     </row>
     <row r="20" spans="1:7" ht="31" x14ac:dyDescent="0.35">
       <c r="A20" s="3" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="B20" s="14">
         <v>1</v>
       </c>
       <c r="C20" s="5">
-        <v>44237</v>
+        <v>44235</v>
       </c>
       <c r="D20" s="5"/>
       <c r="E20" s="5">
-        <v>44238</v>
+        <v>44236</v>
       </c>
       <c r="F20" s="4" t="s">
         <v>5</v>
@@ -3139,17 +3150,17 @@
     </row>
     <row r="21" spans="1:7" ht="31" x14ac:dyDescent="0.35">
       <c r="A21" s="3" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="B21" s="14">
         <v>1</v>
       </c>
       <c r="C21" s="5">
-        <v>44238</v>
+        <v>44236</v>
       </c>
       <c r="D21" s="5"/>
       <c r="E21" s="5">
-        <v>44239</v>
+        <v>44237</v>
       </c>
       <c r="F21" s="4" t="s">
         <v>5</v>
@@ -3158,17 +3169,17 @@
     </row>
     <row r="22" spans="1:7" ht="31" x14ac:dyDescent="0.35">
       <c r="A22" s="3" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="B22" s="14">
         <v>1</v>
       </c>
       <c r="C22" s="5">
-        <v>44238</v>
+        <v>44236</v>
       </c>
       <c r="D22" s="5"/>
       <c r="E22" s="5">
-        <v>44239</v>
+        <v>44237</v>
       </c>
       <c r="F22" s="4" t="s">
         <v>5</v>
@@ -3177,17 +3188,17 @@
     </row>
     <row r="23" spans="1:7" ht="31" x14ac:dyDescent="0.35">
       <c r="A23" s="3" t="s">
-        <v>38</v>
+        <v>21</v>
       </c>
       <c r="B23" s="14">
         <v>1</v>
       </c>
       <c r="C23" s="5">
-        <v>44239</v>
+        <v>44237</v>
       </c>
       <c r="D23" s="5"/>
       <c r="E23" s="5">
-        <v>44242</v>
+        <v>44238</v>
       </c>
       <c r="F23" s="4" t="s">
         <v>5</v>
@@ -3196,17 +3207,17 @@
     </row>
     <row r="24" spans="1:7" ht="31" x14ac:dyDescent="0.35">
       <c r="A24" s="3" t="s">
-        <v>44</v>
+        <v>22</v>
       </c>
       <c r="B24" s="14">
         <v>1</v>
       </c>
       <c r="C24" s="5">
-        <v>44239</v>
+        <v>44237</v>
       </c>
       <c r="D24" s="5"/>
       <c r="E24" s="5">
-        <v>44242</v>
+        <v>44238</v>
       </c>
       <c r="F24" s="4" t="s">
         <v>5</v>
@@ -3215,17 +3226,17 @@
     </row>
     <row r="25" spans="1:7" ht="31" x14ac:dyDescent="0.35">
       <c r="A25" s="3" t="s">
-        <v>45</v>
+        <v>23</v>
       </c>
       <c r="B25" s="14">
         <v>1</v>
       </c>
       <c r="C25" s="5">
-        <v>44242</v>
+        <v>44238</v>
       </c>
       <c r="D25" s="5"/>
       <c r="E25" s="5">
-        <v>44243</v>
+        <v>44239</v>
       </c>
       <c r="F25" s="4" t="s">
         <v>5</v>
@@ -3234,17 +3245,17 @@
     </row>
     <row r="26" spans="1:7" ht="31" x14ac:dyDescent="0.35">
       <c r="A26" s="3" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="B26" s="14">
         <v>1</v>
       </c>
       <c r="C26" s="5">
-        <v>44242</v>
+        <v>44238</v>
       </c>
       <c r="D26" s="5"/>
       <c r="E26" s="5">
-        <v>44243</v>
+        <v>44239</v>
       </c>
       <c r="F26" s="4" t="s">
         <v>5</v>
@@ -3253,17 +3264,17 @@
     </row>
     <row r="27" spans="1:7" ht="31" x14ac:dyDescent="0.35">
       <c r="A27" s="3" t="s">
-        <v>31</v>
+        <v>37</v>
       </c>
       <c r="B27" s="14">
         <v>1</v>
       </c>
       <c r="C27" s="5">
-        <v>44243</v>
+        <v>44239</v>
       </c>
       <c r="D27" s="5"/>
       <c r="E27" s="5">
-        <v>44244</v>
+        <v>44242</v>
       </c>
       <c r="F27" s="4" t="s">
         <v>5</v>
@@ -3272,17 +3283,17 @@
     </row>
     <row r="28" spans="1:7" ht="31" x14ac:dyDescent="0.35">
       <c r="A28" s="3" t="s">
-        <v>32</v>
+        <v>19</v>
       </c>
       <c r="B28" s="14">
         <v>1</v>
       </c>
       <c r="C28" s="5">
-        <v>44243</v>
+        <v>44244</v>
       </c>
       <c r="D28" s="5"/>
       <c r="E28" s="5">
-        <v>44244</v>
+        <v>44245</v>
       </c>
       <c r="F28" s="4" t="s">
         <v>5</v>
@@ -3291,7 +3302,7 @@
     </row>
     <row r="29" spans="1:7" ht="31" x14ac:dyDescent="0.35">
       <c r="A29" s="3" t="s">
-        <v>19</v>
+        <v>32</v>
       </c>
       <c r="B29" s="14">
         <v>1</v>
@@ -3310,17 +3321,17 @@
     </row>
     <row r="30" spans="1:7" ht="31" x14ac:dyDescent="0.35">
       <c r="A30" s="3" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="B30" s="14">
         <v>1</v>
       </c>
       <c r="C30" s="5">
-        <v>44244</v>
+        <v>44245</v>
       </c>
       <c r="D30" s="5"/>
       <c r="E30" s="5">
-        <v>44245</v>
+        <v>44246</v>
       </c>
       <c r="F30" s="4" t="s">
         <v>5</v>
@@ -3329,7 +3340,7 @@
     </row>
     <row r="31" spans="1:7" ht="31" x14ac:dyDescent="0.35">
       <c r="A31" s="3" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="B31" s="14">
         <v>1</v>
@@ -3348,17 +3359,17 @@
     </row>
     <row r="32" spans="1:7" ht="31" x14ac:dyDescent="0.35">
       <c r="A32" s="3" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B32" s="14">
         <v>1</v>
       </c>
       <c r="C32" s="5">
-        <v>44245</v>
+        <v>44246</v>
       </c>
       <c r="D32" s="5"/>
       <c r="E32" s="5">
-        <v>44246</v>
+        <v>44249</v>
       </c>
       <c r="F32" s="4" t="s">
         <v>5</v>
@@ -3367,7 +3378,7 @@
     </row>
     <row r="33" spans="1:7" ht="31" x14ac:dyDescent="0.35">
       <c r="A33" s="3" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B33" s="14">
         <v>1</v>
@@ -3386,17 +3397,17 @@
     </row>
     <row r="34" spans="1:7" ht="31" x14ac:dyDescent="0.35">
       <c r="A34" s="3" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="B34" s="14">
         <v>1</v>
       </c>
       <c r="C34" s="5">
-        <v>44246</v>
+        <v>44249</v>
       </c>
       <c r="D34" s="5"/>
       <c r="E34" s="5">
-        <v>44249</v>
+        <v>44250</v>
       </c>
       <c r="F34" s="4" t="s">
         <v>5</v>
@@ -3405,7 +3416,7 @@
     </row>
     <row r="35" spans="1:7" ht="31" x14ac:dyDescent="0.35">
       <c r="A35" s="3" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B35" s="14">
         <v>1</v>
@@ -3424,17 +3435,17 @@
     </row>
     <row r="36" spans="1:7" ht="31" x14ac:dyDescent="0.35">
       <c r="A36" s="3" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B36" s="14">
         <v>1</v>
       </c>
       <c r="C36" s="5">
-        <v>44249</v>
+        <v>44250</v>
       </c>
       <c r="D36" s="5"/>
       <c r="E36" s="5">
-        <v>44250</v>
+        <v>44251</v>
       </c>
       <c r="F36" s="4" t="s">
         <v>5</v>
@@ -3443,24 +3454,26 @@
     </row>
     <row r="37" spans="1:7" ht="31" x14ac:dyDescent="0.35">
       <c r="A37" s="3" t="s">
-        <v>34</v>
+        <v>45</v>
       </c>
       <c r="B37" s="14">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C37" s="5">
-        <v>44250</v>
-      </c>
-      <c r="D37" s="5"/>
+        <v>44197</v>
+      </c>
+      <c r="D37" s="13">
+        <v>44228</v>
+      </c>
       <c r="E37" s="5">
-        <v>44251</v>
+        <v>44197</v>
       </c>
       <c r="F37" s="4" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="G37" s="1"/>
     </row>
-    <row r="38" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:7" ht="31" x14ac:dyDescent="0.35">
       <c r="A38" s="3" t="s">
         <v>46</v>
       </c>
@@ -3468,36 +3481,24 @@
         <v>2</v>
       </c>
       <c r="C38" s="5">
-        <v>44197</v>
-      </c>
-      <c r="D38" s="13">
-        <v>44228</v>
-      </c>
+        <v>44220</v>
+      </c>
+      <c r="D38" s="5"/>
       <c r="E38" s="5">
-        <v>44197</v>
+        <v>44221</v>
       </c>
       <c r="F38" s="4" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="G38" s="1"/>
     </row>
-    <row r="39" spans="1:7" ht="31" x14ac:dyDescent="0.35">
-      <c r="A39" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="B39" s="14">
-        <v>2</v>
-      </c>
-      <c r="C39" s="5">
-        <v>44220</v>
-      </c>
-      <c r="D39" s="5"/>
-      <c r="E39" s="5">
-        <v>44221</v>
-      </c>
-      <c r="F39" s="4" t="s">
-        <v>5</v>
-      </c>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A39" s="1"/>
+      <c r="B39" s="1"/>
+      <c r="C39" s="1"/>
+      <c r="D39" s="1"/>
+      <c r="E39" s="1"/>
+      <c r="F39" s="1"/>
       <c r="G39" s="1"/>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.35">
@@ -3762,21 +3763,9 @@
       <c r="G68" s="1"/>
     </row>
     <row r="69" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A69" s="1"/>
-      <c r="B69" s="1"/>
-      <c r="C69" s="1"/>
-      <c r="D69" s="1"/>
-      <c r="E69" s="1"/>
-      <c r="F69" s="1"/>
       <c r="G69" s="1"/>
     </row>
     <row r="70" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A70" s="1"/>
-      <c r="B70" s="1"/>
-      <c r="C70" s="1"/>
-      <c r="D70" s="1"/>
-      <c r="E70" s="1"/>
-      <c r="F70" s="1"/>
       <c r="G70" s="1"/>
     </row>
     <row r="71" spans="1:7" x14ac:dyDescent="0.35">
@@ -5254,19 +5243,11 @@
       <c r="F234" s="1"/>
     </row>
     <row r="235" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A235" s="1"/>
-      <c r="B235" s="1"/>
       <c r="C235" s="1"/>
-      <c r="D235" s="1"/>
-      <c r="E235" s="1"/>
-      <c r="F235" s="1"/>
-    </row>
-    <row r="236" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="C236" s="1"/>
     </row>
   </sheetData>
   <dataValidations xWindow="821" yWindow="357" count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Estado" prompt="Por favor, introduzca un valor para el estado (PENDIENTE, EN PROGRESO O REALIZADO )" sqref="F1:F39" xr:uid="{01248019-FD26-4D39-BA8E-80B22E1EE596}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Estado" prompt="Por favor, introduzca un valor para el estado (PENDIENTE, EN PROGRESO O REALIZADO )" sqref="F28:F38 F1:F27" xr:uid="{01248019-FD26-4D39-BA8E-80B22E1EE596}">
       <formula1>$N$2:$N$4</formula1>
     </dataValidation>
   </dataValidations>
@@ -5280,8 +5261,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{25ACDF49-AC43-4CCD-856F-6ED289E70C3E}">
   <dimension ref="A2:G35"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -5294,13 +5275,13 @@
   <sheetData>
     <row r="2" spans="1:7" x14ac:dyDescent="0.35">
       <c r="B2" s="15" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C2" s="15"/>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.35">
       <c r="B3" s="11" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C3" s="11">
         <v>28</v>
@@ -5308,28 +5289,28 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.35">
       <c r="B4" s="11" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C4" s="11">
-        <f>SUM('SPRINT-BACKLOG'!B2:B39)</f>
-        <v>32</v>
+        <f>SUM('SPRINT-BACKLOG'!B2:B38)</f>
+        <v>31</v>
       </c>
     </row>
     <row r="7" spans="1:7" ht="26" x14ac:dyDescent="0.35">
       <c r="A7" s="7" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B7" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="C7" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="C7" s="7" t="s">
+      <c r="D7" s="7" t="s">
         <v>49</v>
       </c>
-      <c r="D7" s="7" t="s">
+      <c r="E7" s="7" t="s">
         <v>50</v>
-      </c>
-      <c r="E7" s="7" t="s">
-        <v>51</v>
       </c>
       <c r="G7" s="6"/>
     </row>
@@ -5342,15 +5323,15 @@
       </c>
       <c r="C8" s="9">
         <f>C4</f>
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D8" s="10">
-        <f>SUMIF('SPRINT-BACKLOG'!D2:D39,"="&amp;VALUE(A8),'SPRINT-BACKLOG'!B2:B39)</f>
+        <f>SUMIF('SPRINT-BACKLOG'!D2:D38,"="&amp;VALUE(A8),'SPRINT-BACKLOG'!B2:B38)</f>
         <v>2</v>
       </c>
       <c r="E8" s="9">
         <f>C4 - D8</f>
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="9" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
@@ -5362,14 +5343,14 @@
       </c>
       <c r="C9" s="9">
         <f t="shared" ref="C9:C35" si="0">C8-$C$4/($C$3-1)</f>
-        <v>30.814814814814817</v>
+        <v>29.851851851851851</v>
       </c>
       <c r="D9" s="10">
         <v>2</v>
       </c>
       <c r="E9" s="9">
         <f>E8 - D9</f>
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.35">
@@ -5381,14 +5362,14 @@
       </c>
       <c r="C10" s="9">
         <f t="shared" si="0"/>
-        <v>29.629629629629633</v>
+        <v>28.703703703703702</v>
       </c>
       <c r="D10" s="10">
         <v>0</v>
       </c>
       <c r="E10" s="9">
         <f>E9 - D10</f>
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.35">
@@ -5400,14 +5381,14 @@
       </c>
       <c r="C11" s="9">
         <f t="shared" si="0"/>
-        <v>28.44444444444445</v>
+        <v>27.555555555555554</v>
       </c>
       <c r="D11" s="10">
         <v>5</v>
       </c>
       <c r="E11" s="9">
         <f t="shared" ref="E11:E35" si="1">E10 - D11</f>
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.35">
@@ -5419,14 +5400,14 @@
       </c>
       <c r="C12" s="9">
         <f t="shared" si="0"/>
-        <v>27.259259259259267</v>
+        <v>26.407407407407405</v>
       </c>
       <c r="D12" s="10">
         <v>0</v>
       </c>
       <c r="E12" s="9">
         <f t="shared" si="1"/>
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.35">
@@ -5438,14 +5419,14 @@
       </c>
       <c r="C13" s="9">
         <f t="shared" si="0"/>
-        <v>26.074074074074083</v>
+        <v>25.259259259259256</v>
       </c>
       <c r="D13" s="10">
         <v>1</v>
       </c>
       <c r="E13" s="9">
         <f t="shared" si="1"/>
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.35">
@@ -5457,14 +5438,14 @@
       </c>
       <c r="C14" s="9">
         <f t="shared" si="0"/>
-        <v>24.8888888888889</v>
+        <v>24.111111111111107</v>
       </c>
       <c r="D14" s="10">
         <v>0</v>
       </c>
       <c r="E14" s="9">
         <f t="shared" si="1"/>
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.35">
@@ -5476,14 +5457,14 @@
       </c>
       <c r="C15" s="9">
         <f t="shared" si="0"/>
-        <v>23.703703703703717</v>
+        <v>22.962962962962958</v>
       </c>
       <c r="D15" s="10">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E15" s="9">
         <f t="shared" si="1"/>
-        <v>22</v>
+        <v>18</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.35">
@@ -5495,14 +5476,14 @@
       </c>
       <c r="C16" s="9">
         <f t="shared" si="0"/>
-        <v>22.518518518518533</v>
+        <v>21.81481481481481</v>
       </c>
       <c r="D16" s="10">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E16" s="9">
         <f t="shared" si="1"/>
-        <v>22</v>
+        <v>16</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.35">
@@ -5514,15 +5495,15 @@
       </c>
       <c r="C17" s="9">
         <f t="shared" si="0"/>
-        <v>21.33333333333335</v>
+        <v>20.666666666666661</v>
       </c>
       <c r="D17" s="10">
-        <f>SUMIF('SPRINT-BACKLOG'!D2:D39,"="&amp;VALUE(A17),'SPRINT-BACKLOG'!B2:B39)</f>
+        <f>SUMIF('SPRINT-BACKLOG'!D2:D38,"="&amp;VALUE(A17),'SPRINT-BACKLOG'!B2:B38)</f>
         <v>0</v>
       </c>
       <c r="E17" s="9">
         <f t="shared" si="1"/>
-        <v>22</v>
+        <v>16</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.35">
@@ -5534,15 +5515,15 @@
       </c>
       <c r="C18" s="9">
         <f t="shared" si="0"/>
-        <v>20.148148148148167</v>
+        <v>19.518518518518512</v>
       </c>
       <c r="D18" s="10">
-        <f>SUMIF('SPRINT-BACKLOG'!D2:D39,"="&amp;VALUE(A18),'SPRINT-BACKLOG'!B2:B39)</f>
+        <f>SUMIF('SPRINT-BACKLOG'!D2:D38,"="&amp;VALUE(A18),'SPRINT-BACKLOG'!B2:B38)</f>
         <v>0</v>
       </c>
       <c r="E18" s="9">
         <f t="shared" si="1"/>
-        <v>22</v>
+        <v>16</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.35">
@@ -5554,15 +5535,15 @@
       </c>
       <c r="C19" s="9">
         <f t="shared" si="0"/>
-        <v>18.962962962962983</v>
+        <v>18.370370370370363</v>
       </c>
       <c r="D19" s="10">
-        <f>SUMIF('SPRINT-BACKLOG'!D2:D39,"="&amp;VALUE(A19),'SPRINT-BACKLOG'!B2:B39)</f>
+        <f>SUMIF('SPRINT-BACKLOG'!D2:D38,"="&amp;VALUE(A19),'SPRINT-BACKLOG'!B2:B38)</f>
         <v>0</v>
       </c>
       <c r="E19" s="9">
         <f t="shared" si="1"/>
-        <v>22</v>
+        <v>16</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.35">
@@ -5574,15 +5555,15 @@
       </c>
       <c r="C20" s="9">
         <f t="shared" si="0"/>
-        <v>17.7777777777778</v>
+        <v>17.222222222222214</v>
       </c>
       <c r="D20" s="10">
-        <f>SUMIF('SPRINT-BACKLOG'!D2:D39,"="&amp;VALUE(A20),'SPRINT-BACKLOG'!B2:B39)</f>
+        <f>SUMIF('SPRINT-BACKLOG'!D2:D38,"="&amp;VALUE(A20),'SPRINT-BACKLOG'!B2:B38)</f>
         <v>0</v>
       </c>
       <c r="E20" s="9">
         <f t="shared" si="1"/>
-        <v>22</v>
+        <v>16</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.35">
@@ -5594,15 +5575,15 @@
       </c>
       <c r="C21" s="9">
         <f t="shared" si="0"/>
-        <v>16.592592592592617</v>
+        <v>16.074074074074066</v>
       </c>
       <c r="D21" s="10">
-        <f>SUMIF('SPRINT-BACKLOG'!D2:D39,"="&amp;VALUE(A21),'SPRINT-BACKLOG'!B2:B39)</f>
+        <f>SUMIF('SPRINT-BACKLOG'!D2:D38,"="&amp;VALUE(A21),'SPRINT-BACKLOG'!B2:B38)</f>
         <v>0</v>
       </c>
       <c r="E21" s="9">
         <f t="shared" si="1"/>
-        <v>22</v>
+        <v>16</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.35">
@@ -5614,15 +5595,15 @@
       </c>
       <c r="C22" s="9">
         <f t="shared" si="0"/>
-        <v>15.407407407407431</v>
+        <v>14.925925925925917</v>
       </c>
       <c r="D22" s="10">
-        <f>SUMIF('SPRINT-BACKLOG'!D2:D39,"="&amp;VALUE(A22),'SPRINT-BACKLOG'!B2:B39)</f>
+        <f>SUMIF('SPRINT-BACKLOG'!D2:D38,"="&amp;VALUE(A22),'SPRINT-BACKLOG'!B2:B38)</f>
         <v>0</v>
       </c>
       <c r="E22" s="9">
         <f t="shared" si="1"/>
-        <v>22</v>
+        <v>16</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.35">
@@ -5634,15 +5615,15 @@
       </c>
       <c r="C23" s="9">
         <f t="shared" si="0"/>
-        <v>14.222222222222246</v>
+        <v>13.777777777777768</v>
       </c>
       <c r="D23" s="10">
-        <f>SUMIF('SPRINT-BACKLOG'!D2:D39,"="&amp;VALUE(A23),'SPRINT-BACKLOG'!B2:B39)</f>
+        <f>SUMIF('SPRINT-BACKLOG'!D2:D38,"="&amp;VALUE(A23),'SPRINT-BACKLOG'!B2:B38)</f>
         <v>0</v>
       </c>
       <c r="E23" s="9">
         <f t="shared" si="1"/>
-        <v>22</v>
+        <v>16</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.35">
@@ -5654,15 +5635,15 @@
       </c>
       <c r="C24" s="9">
         <f t="shared" si="0"/>
-        <v>13.037037037037061</v>
+        <v>12.629629629629619</v>
       </c>
       <c r="D24" s="10">
-        <f>SUMIF('SPRINT-BACKLOG'!D2:D39,"="&amp;VALUE(A24),'SPRINT-BACKLOG'!B2:B39)</f>
+        <f>SUMIF('SPRINT-BACKLOG'!D2:D38,"="&amp;VALUE(A24),'SPRINT-BACKLOG'!B2:B38)</f>
         <v>0</v>
       </c>
       <c r="E24" s="9">
         <f t="shared" si="1"/>
-        <v>22</v>
+        <v>16</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.35">
@@ -5674,15 +5655,15 @@
       </c>
       <c r="C25" s="9">
         <f t="shared" si="0"/>
-        <v>11.851851851851876</v>
+        <v>11.48148148148147</v>
       </c>
       <c r="D25" s="10">
-        <f>SUMIF('SPRINT-BACKLOG'!D2:D39,"="&amp;VALUE(A25),'SPRINT-BACKLOG'!B2:B39)</f>
+        <f>SUMIF('SPRINT-BACKLOG'!D2:D38,"="&amp;VALUE(A25),'SPRINT-BACKLOG'!B2:B38)</f>
         <v>0</v>
       </c>
       <c r="E25" s="9">
         <f t="shared" si="1"/>
-        <v>22</v>
+        <v>16</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.35">
@@ -5694,15 +5675,15 @@
       </c>
       <c r="C26" s="9">
         <f t="shared" si="0"/>
-        <v>10.666666666666691</v>
+        <v>10.333333333333321</v>
       </c>
       <c r="D26" s="10">
-        <f>SUMIF('SPRINT-BACKLOG'!D2:D39,"="&amp;VALUE(A26),'SPRINT-BACKLOG'!B2:B39)</f>
+        <f>SUMIF('SPRINT-BACKLOG'!D2:D38,"="&amp;VALUE(A26),'SPRINT-BACKLOG'!B2:B38)</f>
         <v>0</v>
       </c>
       <c r="E26" s="9">
         <f>E25 - D26</f>
-        <v>22</v>
+        <v>16</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.35">
@@ -5714,15 +5695,15 @@
       </c>
       <c r="C27" s="9">
         <f t="shared" si="0"/>
-        <v>9.4814814814815058</v>
+        <v>9.1851851851851727</v>
       </c>
       <c r="D27" s="10">
-        <f>SUMIF('SPRINT-BACKLOG'!D2:D39,"="&amp;VALUE(A27),'SPRINT-BACKLOG'!B2:B39)</f>
+        <f>SUMIF('SPRINT-BACKLOG'!D2:D38,"="&amp;VALUE(A27),'SPRINT-BACKLOG'!B2:B38)</f>
         <v>0</v>
       </c>
       <c r="E27" s="9">
         <f t="shared" si="1"/>
-        <v>22</v>
+        <v>16</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.35">
@@ -5734,15 +5715,15 @@
       </c>
       <c r="C28" s="9">
         <f t="shared" si="0"/>
-        <v>8.2962962962963207</v>
+        <v>8.0370370370370239</v>
       </c>
       <c r="D28" s="10">
-        <f>SUMIF('SPRINT-BACKLOG'!D2:D39,"="&amp;VALUE(A28),'SPRINT-BACKLOG'!B2:B39)</f>
+        <f>SUMIF('SPRINT-BACKLOG'!D2:D38,"="&amp;VALUE(A28),'SPRINT-BACKLOG'!B2:B38)</f>
         <v>0</v>
       </c>
       <c r="E28" s="9">
         <f t="shared" si="1"/>
-        <v>22</v>
+        <v>16</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.35">
@@ -5754,14 +5735,14 @@
       </c>
       <c r="C29" s="9">
         <f t="shared" si="0"/>
-        <v>7.1111111111111356</v>
+        <v>6.888888888888876</v>
       </c>
       <c r="D29" s="10">
         <v>0</v>
       </c>
       <c r="E29" s="9">
         <f t="shared" si="1"/>
-        <v>22</v>
+        <v>16</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.35">
@@ -5773,15 +5754,15 @@
       </c>
       <c r="C30" s="9">
         <f t="shared" si="0"/>
-        <v>5.9259259259259505</v>
+        <v>5.740740740740728</v>
       </c>
       <c r="D30" s="10">
-        <f>SUMIF('SPRINT-BACKLOG'!D2:D39,"="&amp;VALUE(A30),'SPRINT-BACKLOG'!B2:B39)</f>
+        <f>SUMIF('SPRINT-BACKLOG'!D2:D38,"="&amp;VALUE(A30),'SPRINT-BACKLOG'!B2:B38)</f>
         <v>0</v>
       </c>
       <c r="E30" s="9">
         <f t="shared" si="1"/>
-        <v>22</v>
+        <v>16</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.35">
@@ -5793,15 +5774,15 @@
       </c>
       <c r="C31" s="9">
         <f t="shared" si="0"/>
-        <v>4.7407407407407653</v>
+        <v>4.5925925925925801</v>
       </c>
       <c r="D31" s="10">
-        <f>SUMIF('SPRINT-BACKLOG'!D2:D39,"="&amp;VALUE(A31),'SPRINT-BACKLOG'!B2:B39)</f>
+        <f>SUMIF('SPRINT-BACKLOG'!D2:D38,"="&amp;VALUE(A31),'SPRINT-BACKLOG'!B2:B38)</f>
         <v>0</v>
       </c>
       <c r="E31" s="9">
         <f t="shared" si="1"/>
-        <v>22</v>
+        <v>16</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.35">
@@ -5813,15 +5794,15 @@
       </c>
       <c r="C32" s="9">
         <f t="shared" si="0"/>
-        <v>3.5555555555555802</v>
+        <v>3.4444444444444322</v>
       </c>
       <c r="D32" s="10">
-        <f>SUMIF('SPRINT-BACKLOG'!D2:D39,"="&amp;VALUE(A32),'SPRINT-BACKLOG'!B2:B39)</f>
+        <f>SUMIF('SPRINT-BACKLOG'!D2:D38,"="&amp;VALUE(A32),'SPRINT-BACKLOG'!B2:B38)</f>
         <v>0</v>
       </c>
       <c r="E32" s="9">
         <f t="shared" si="1"/>
-        <v>22</v>
+        <v>16</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.35">
@@ -5833,15 +5814,15 @@
       </c>
       <c r="C33" s="9">
         <f t="shared" si="0"/>
-        <v>2.3703703703703951</v>
+        <v>2.2962962962962843</v>
       </c>
       <c r="D33" s="10">
-        <f>SUMIF('SPRINT-BACKLOG'!D2:D39,"="&amp;VALUE(A33),'SPRINT-BACKLOG'!B2:B39)</f>
+        <f>SUMIF('SPRINT-BACKLOG'!D2:D38,"="&amp;VALUE(A33),'SPRINT-BACKLOG'!B2:B38)</f>
         <v>0</v>
       </c>
       <c r="E33" s="9">
         <f t="shared" si="1"/>
-        <v>22</v>
+        <v>16</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.35">
@@ -5853,15 +5834,15 @@
       </c>
       <c r="C34" s="9">
         <f t="shared" si="0"/>
-        <v>1.18518518518521</v>
+        <v>1.1481481481481361</v>
       </c>
       <c r="D34" s="10">
-        <f>SUMIF('SPRINT-BACKLOG'!D2:D39,"="&amp;VALUE(A34),'SPRINT-BACKLOG'!B2:B39)</f>
+        <f>SUMIF('SPRINT-BACKLOG'!D2:D38,"="&amp;VALUE(A34),'SPRINT-BACKLOG'!B2:B38)</f>
         <v>0</v>
       </c>
       <c r="E34" s="9">
         <f t="shared" si="1"/>
-        <v>22</v>
+        <v>16</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.35">
@@ -5873,15 +5854,15 @@
       </c>
       <c r="C35" s="9">
         <f t="shared" si="0"/>
-        <v>2.4868995751603507E-14</v>
+        <v>-1.1990408665951691E-14</v>
       </c>
       <c r="D35" s="10">
-        <f>SUMIF('SPRINT-BACKLOG'!D2:D39,"="&amp;VALUE(A35),'SPRINT-BACKLOG'!B2:B39)</f>
+        <f>SUMIF('SPRINT-BACKLOG'!D2:D38,"="&amp;VALUE(A35),'SPRINT-BACKLOG'!B2:B38)</f>
         <v>0</v>
       </c>
       <c r="E35" s="9">
         <f t="shared" si="1"/>
-        <v>22</v>
+        <v>16</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
[IMPL] CRUD SOL.SERVICIO, SERVICIO (EMPRESA) Se ha implementado correctamente la funcionalidad de CRUD para los servicios y solicitudes de servicio para el rol de empresa.
</commit_message>
<xml_diff>
--- a/documentación/Product Backlog/SP2.xlsx
+++ b/documentación/Product Backlog/SP2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alesk\Desktop\Universidad\TFG_app\TFG_app\documentación\Product Backlog\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27948566-F67F-4B91-AD15-0EA5148155B8}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D86BAF6-A4C0-4C36-B693-4991120B28B5}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="29610" yWindow="-120" windowWidth="19800" windowHeight="11760" xr2:uid="{41FE112A-4516-4423-9CD7-320A9C032A6D}"/>
   </bookViews>
@@ -867,46 +867,46 @@
                   <c:v>16</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>16</c:v>
+                  <c:v>14</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>16</c:v>
+                  <c:v>14</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>16</c:v>
+                  <c:v>14</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>16</c:v>
+                  <c:v>14</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>16</c:v>
+                  <c:v>14</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>16</c:v>
+                  <c:v>14</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>16</c:v>
+                  <c:v>14</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>16</c:v>
+                  <c:v>14</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>16</c:v>
+                  <c:v>14</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>16</c:v>
+                  <c:v>14</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>16</c:v>
+                  <c:v>14</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>16</c:v>
+                  <c:v>14</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>16</c:v>
+                  <c:v>14</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>16</c:v>
+                  <c:v>14</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2710,8 +2710,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2BB024A1-16E4-467A-A83B-A5E93171F59F}">
   <dimension ref="A1:O235"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A14" sqref="A14:XFD14"/>
+    <sheetView tabSelected="1" topLeftCell="A34" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D37" sqref="D37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3158,7 +3158,9 @@
       <c r="C21" s="5">
         <v>44236</v>
       </c>
-      <c r="D21" s="5"/>
+      <c r="D21" s="5">
+        <v>44242</v>
+      </c>
       <c r="E21" s="5">
         <v>44237</v>
       </c>
@@ -3196,7 +3198,9 @@
       <c r="C23" s="5">
         <v>44237</v>
       </c>
-      <c r="D23" s="5"/>
+      <c r="D23" s="5">
+        <v>44242</v>
+      </c>
       <c r="E23" s="5">
         <v>44238</v>
       </c>
@@ -3452,7 +3456,7 @@
       </c>
       <c r="G36" s="1"/>
     </row>
-    <row r="37" spans="1:7" ht="31" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A37" s="3" t="s">
         <v>45</v>
       </c>
@@ -5247,7 +5251,7 @@
     </row>
   </sheetData>
   <dataValidations xWindow="821" yWindow="357" count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Estado" prompt="Por favor, introduzca un valor para el estado (PENDIENTE, EN PROGRESO O REALIZADO )" sqref="F28:F38 F1:F27" xr:uid="{01248019-FD26-4D39-BA8E-80B22E1EE596}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Estado" prompt="Por favor, introduzca un valor para el estado (PENDIENTE, EN PROGRESO O REALIZADO )" sqref="F1:F38" xr:uid="{01248019-FD26-4D39-BA8E-80B22E1EE596}">
       <formula1>$N$2:$N$4</formula1>
     </dataValidation>
   </dataValidations>
@@ -5261,8 +5265,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{25ACDF49-AC43-4CCD-856F-6ED289E70C3E}">
   <dimension ref="A2:G35"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D22" sqref="D22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -5599,11 +5603,11 @@
       </c>
       <c r="D22" s="10">
         <f>SUMIF('SPRINT-BACKLOG'!D2:D38,"="&amp;VALUE(A22),'SPRINT-BACKLOG'!B2:B38)</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E22" s="9">
         <f t="shared" si="1"/>
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.35">
@@ -5623,7 +5627,7 @@
       </c>
       <c r="E23" s="9">
         <f t="shared" si="1"/>
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.35">
@@ -5643,7 +5647,7 @@
       </c>
       <c r="E24" s="9">
         <f t="shared" si="1"/>
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.35">
@@ -5663,7 +5667,7 @@
       </c>
       <c r="E25" s="9">
         <f t="shared" si="1"/>
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.35">
@@ -5683,7 +5687,7 @@
       </c>
       <c r="E26" s="9">
         <f>E25 - D26</f>
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.35">
@@ -5703,7 +5707,7 @@
       </c>
       <c r="E27" s="9">
         <f t="shared" si="1"/>
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.35">
@@ -5723,7 +5727,7 @@
       </c>
       <c r="E28" s="9">
         <f t="shared" si="1"/>
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.35">
@@ -5742,7 +5746,7 @@
       </c>
       <c r="E29" s="9">
         <f t="shared" si="1"/>
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.35">
@@ -5762,7 +5766,7 @@
       </c>
       <c r="E30" s="9">
         <f t="shared" si="1"/>
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.35">
@@ -5782,7 +5786,7 @@
       </c>
       <c r="E31" s="9">
         <f t="shared" si="1"/>
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.35">
@@ -5802,7 +5806,7 @@
       </c>
       <c r="E32" s="9">
         <f t="shared" si="1"/>
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.35">
@@ -5822,7 +5826,7 @@
       </c>
       <c r="E33" s="9">
         <f t="shared" si="1"/>
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.35">
@@ -5842,7 +5846,7 @@
       </c>
       <c r="E34" s="9">
         <f t="shared" si="1"/>
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.35">
@@ -5862,7 +5866,7 @@
       </c>
       <c r="E35" s="9">
         <f t="shared" si="1"/>
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
[IMP] Funcionalidad rol trabajador I Se ha implemementado la funcionalidad de listar, mostrar y editar servicios para el rol de trabajador. Además, se ha implementado la funcionalidad de mostrar y editar los datos del trabajador. Falta mostrar el vehículo asignado al trabajador
</commit_message>
<xml_diff>
--- a/documentación/Product Backlog/SP2.xlsx
+++ b/documentación/Product Backlog/SP2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alesk\Desktop\Universidad\TFG_app\TFG_app\documentación\Product Backlog\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D86BAF6-A4C0-4C36-B693-4991120B28B5}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{326E1ACE-456C-4182-BD01-2B1B362CF0D3}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="29610" yWindow="-120" windowWidth="19800" windowHeight="11760" xr2:uid="{41FE112A-4516-4423-9CD7-320A9C032A6D}"/>
   </bookViews>
@@ -870,43 +870,43 @@
                   <c:v>14</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>14</c:v>
+                  <c:v>12</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>14</c:v>
+                  <c:v>12</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>14</c:v>
+                  <c:v>12</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>14</c:v>
+                  <c:v>12</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>14</c:v>
+                  <c:v>12</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>14</c:v>
+                  <c:v>12</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>14</c:v>
+                  <c:v>12</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>14</c:v>
+                  <c:v>12</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>14</c:v>
+                  <c:v>12</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>14</c:v>
+                  <c:v>12</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>14</c:v>
+                  <c:v>12</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>14</c:v>
+                  <c:v>12</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>14</c:v>
+                  <c:v>12</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2710,8 +2710,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2BB024A1-16E4-467A-A83B-A5E93171F59F}">
   <dimension ref="A1:O235"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D37" sqref="D37"/>
+    <sheetView tabSelected="1" topLeftCell="A40" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F22" sqref="F22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2743,7 +2743,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:15" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:15" ht="31" x14ac:dyDescent="0.35">
       <c r="A2" s="3" t="s">
         <v>10</v>
       </c>
@@ -2856,7 +2856,7 @@
         <v>44230</v>
       </c>
       <c r="F6" s="4" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="G6" s="1"/>
     </row>
@@ -2877,7 +2877,7 @@
         <v>44230</v>
       </c>
       <c r="F7" s="4" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="G7" s="1"/>
     </row>
@@ -2936,7 +2936,7 @@
         <v>44232</v>
       </c>
       <c r="F10" s="4" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="G10" s="1"/>
     </row>
@@ -2957,7 +2957,7 @@
         <v>44232</v>
       </c>
       <c r="F11" s="4" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="G11" s="1"/>
     </row>
@@ -2978,7 +2978,7 @@
         <v>44232</v>
       </c>
       <c r="F12" s="4" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="G12" s="1"/>
     </row>
@@ -2999,7 +2999,7 @@
         <v>44235</v>
       </c>
       <c r="F13" s="4" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="G13" s="1"/>
     </row>
@@ -3020,7 +3020,7 @@
         <v>44235</v>
       </c>
       <c r="F14" s="4" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="G14" s="1"/>
     </row>
@@ -3041,7 +3041,7 @@
         <v>44236</v>
       </c>
       <c r="F15" s="4" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="G15" s="1"/>
     </row>
@@ -3062,7 +3062,7 @@
         <v>44242</v>
       </c>
       <c r="F16" s="4" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="G16" s="1"/>
     </row>
@@ -3083,7 +3083,7 @@
         <v>44243</v>
       </c>
       <c r="F17" s="4" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="G17" s="1"/>
     </row>
@@ -3104,7 +3104,7 @@
         <v>44243</v>
       </c>
       <c r="F18" s="4" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="G18" s="1"/>
     </row>
@@ -3125,7 +3125,7 @@
         <v>44244</v>
       </c>
       <c r="F19" s="4" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="G19" s="1"/>
     </row>
@@ -3139,12 +3139,14 @@
       <c r="C20" s="5">
         <v>44235</v>
       </c>
-      <c r="D20" s="5"/>
+      <c r="D20" s="5">
+        <v>44243</v>
+      </c>
       <c r="E20" s="5">
         <v>44236</v>
       </c>
       <c r="F20" s="4" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="G20" s="1"/>
     </row>
@@ -3165,7 +3167,7 @@
         <v>44237</v>
       </c>
       <c r="F21" s="4" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="G21" s="1"/>
     </row>
@@ -3179,12 +3181,14 @@
       <c r="C22" s="5">
         <v>44236</v>
       </c>
-      <c r="D22" s="5"/>
+      <c r="D22" s="5">
+        <v>44243</v>
+      </c>
       <c r="E22" s="5">
         <v>44237</v>
       </c>
       <c r="F22" s="4" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="G22" s="1"/>
     </row>
@@ -3205,7 +3209,7 @@
         <v>44238</v>
       </c>
       <c r="F23" s="4" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="G23" s="1"/>
     </row>
@@ -5623,11 +5627,11 @@
       </c>
       <c r="D23" s="10">
         <f>SUMIF('SPRINT-BACKLOG'!D2:D38,"="&amp;VALUE(A23),'SPRINT-BACKLOG'!B2:B38)</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E23" s="9">
         <f t="shared" si="1"/>
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.35">
@@ -5647,7 +5651,7 @@
       </c>
       <c r="E24" s="9">
         <f t="shared" si="1"/>
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.35">
@@ -5667,7 +5671,7 @@
       </c>
       <c r="E25" s="9">
         <f t="shared" si="1"/>
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.35">
@@ -5687,7 +5691,7 @@
       </c>
       <c r="E26" s="9">
         <f>E25 - D26</f>
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.35">
@@ -5707,7 +5711,7 @@
       </c>
       <c r="E27" s="9">
         <f t="shared" si="1"/>
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.35">
@@ -5727,7 +5731,7 @@
       </c>
       <c r="E28" s="9">
         <f t="shared" si="1"/>
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.35">
@@ -5746,7 +5750,7 @@
       </c>
       <c r="E29" s="9">
         <f t="shared" si="1"/>
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.35">
@@ -5766,7 +5770,7 @@
       </c>
       <c r="E30" s="9">
         <f t="shared" si="1"/>
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.35">
@@ -5786,7 +5790,7 @@
       </c>
       <c r="E31" s="9">
         <f t="shared" si="1"/>
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.35">
@@ -5806,7 +5810,7 @@
       </c>
       <c r="E32" s="9">
         <f t="shared" si="1"/>
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.35">
@@ -5826,7 +5830,7 @@
       </c>
       <c r="E33" s="9">
         <f t="shared" si="1"/>
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.35">
@@ -5846,7 +5850,7 @@
       </c>
       <c r="E34" s="9">
         <f t="shared" si="1"/>
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.35">
@@ -5866,7 +5870,7 @@
       </c>
       <c r="E35" s="9">
         <f t="shared" si="1"/>
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
[IMP] Trabajador completo Se ha finalizado de desarrollar la funcionalidad básica para el rol de trabajador.
</commit_message>
<xml_diff>
--- a/documentación/Product Backlog/SP2.xlsx
+++ b/documentación/Product Backlog/SP2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alesk\Desktop\Universidad\TFG_app\TFG_app\documentación\Product Backlog\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{326E1ACE-456C-4182-BD01-2B1B362CF0D3}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{317055F7-F968-49E7-8233-F8C026499112}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="29610" yWindow="-120" windowWidth="19800" windowHeight="11760" xr2:uid="{41FE112A-4516-4423-9CD7-320A9C032A6D}"/>
   </bookViews>
@@ -870,43 +870,43 @@
                   <c:v>14</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>12</c:v>
+                  <c:v>9</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>12</c:v>
+                  <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>12</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>12</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>12</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>12</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>12</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>12</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>12</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>12</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>12</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>12</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>12</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2710,8 +2710,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2BB024A1-16E4-467A-A83B-A5E93171F59F}">
   <dimension ref="A1:O235"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A40" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F22" sqref="F22"/>
+    <sheetView tabSelected="1" topLeftCell="A46" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2743,7 +2743,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:15" ht="31" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:15" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A2" s="3" t="s">
         <v>10</v>
       </c>
@@ -2839,7 +2839,7 @@
       </c>
       <c r="G5" s="1"/>
     </row>
-    <row r="6" spans="1:15" ht="31" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:15" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A6" s="3" t="s">
         <v>13</v>
       </c>
@@ -2860,7 +2860,7 @@
       </c>
       <c r="G6" s="1"/>
     </row>
-    <row r="7" spans="1:15" ht="31" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:15" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A7" s="3" t="s">
         <v>28</v>
       </c>
@@ -2891,7 +2891,9 @@
       <c r="C8" s="5">
         <v>44230</v>
       </c>
-      <c r="D8" s="5"/>
+      <c r="D8" s="5">
+        <v>44245</v>
+      </c>
       <c r="E8" s="5">
         <v>44231</v>
       </c>
@@ -2919,7 +2921,7 @@
       </c>
       <c r="G9" s="1"/>
     </row>
-    <row r="10" spans="1:15" ht="31" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:15" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A10" s="3" t="s">
         <v>42</v>
       </c>
@@ -3045,7 +3047,7 @@
       </c>
       <c r="G15" s="1"/>
     </row>
-    <row r="16" spans="1:15" ht="31" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:15" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A16" s="3" t="s">
         <v>43</v>
       </c>
@@ -3066,7 +3068,7 @@
       </c>
       <c r="G16" s="1"/>
     </row>
-    <row r="17" spans="1:7" ht="31" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A17" s="3" t="s">
         <v>44</v>
       </c>
@@ -3299,12 +3301,14 @@
       <c r="C28" s="5">
         <v>44244</v>
       </c>
-      <c r="D28" s="5"/>
+      <c r="D28" s="5">
+        <v>44243</v>
+      </c>
       <c r="E28" s="5">
         <v>44245</v>
       </c>
       <c r="F28" s="4" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="G28" s="1"/>
     </row>
@@ -3318,12 +3322,14 @@
       <c r="C29" s="5">
         <v>44244</v>
       </c>
-      <c r="D29" s="5"/>
+      <c r="D29" s="5">
+        <v>44243</v>
+      </c>
       <c r="E29" s="5">
         <v>44245</v>
       </c>
       <c r="F29" s="4" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="G29" s="1"/>
     </row>
@@ -3337,12 +3343,14 @@
       <c r="C30" s="5">
         <v>44245</v>
       </c>
-      <c r="D30" s="5"/>
+      <c r="D30" s="5">
+        <v>44243</v>
+      </c>
       <c r="E30" s="5">
         <v>44246</v>
       </c>
       <c r="F30" s="4" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="G30" s="1"/>
     </row>
@@ -3356,12 +3364,14 @@
       <c r="C31" s="5">
         <v>44245</v>
       </c>
-      <c r="D31" s="5"/>
+      <c r="D31" s="5">
+        <v>44244</v>
+      </c>
       <c r="E31" s="5">
         <v>44246</v>
       </c>
       <c r="F31" s="4" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="G31" s="1"/>
     </row>
@@ -3375,12 +3385,14 @@
       <c r="C32" s="5">
         <v>44246</v>
       </c>
-      <c r="D32" s="5"/>
+      <c r="D32" s="5">
+        <v>44244</v>
+      </c>
       <c r="E32" s="5">
         <v>44249</v>
       </c>
       <c r="F32" s="4" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="G32" s="1"/>
     </row>
@@ -3394,12 +3406,14 @@
       <c r="C33" s="5">
         <v>44246</v>
       </c>
-      <c r="D33" s="5"/>
+      <c r="D33" s="5">
+        <v>44245</v>
+      </c>
       <c r="E33" s="5">
         <v>44249</v>
       </c>
       <c r="F33" s="4" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="G33" s="1"/>
     </row>
@@ -5627,11 +5641,11 @@
       </c>
       <c r="D23" s="10">
         <f>SUMIF('SPRINT-BACKLOG'!D2:D38,"="&amp;VALUE(A23),'SPRINT-BACKLOG'!B2:B38)</f>
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="E23" s="9">
         <f t="shared" si="1"/>
-        <v>12</v>
+        <v>9</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.35">
@@ -5647,11 +5661,11 @@
       </c>
       <c r="D24" s="10">
         <f>SUMIF('SPRINT-BACKLOG'!D2:D38,"="&amp;VALUE(A24),'SPRINT-BACKLOG'!B2:B38)</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E24" s="9">
         <f t="shared" si="1"/>
-        <v>12</v>
+        <v>7</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.35">
@@ -5667,11 +5681,11 @@
       </c>
       <c r="D25" s="10">
         <f>SUMIF('SPRINT-BACKLOG'!D2:D38,"="&amp;VALUE(A25),'SPRINT-BACKLOG'!B2:B38)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E25" s="9">
         <f t="shared" si="1"/>
-        <v>12</v>
+        <v>6</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.35">
@@ -5691,7 +5705,7 @@
       </c>
       <c r="E26" s="9">
         <f>E25 - D26</f>
-        <v>12</v>
+        <v>6</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.35">
@@ -5711,7 +5725,7 @@
       </c>
       <c r="E27" s="9">
         <f t="shared" si="1"/>
-        <v>12</v>
+        <v>6</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.35">
@@ -5731,7 +5745,7 @@
       </c>
       <c r="E28" s="9">
         <f t="shared" si="1"/>
-        <v>12</v>
+        <v>6</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.35">
@@ -5750,7 +5764,7 @@
       </c>
       <c r="E29" s="9">
         <f t="shared" si="1"/>
-        <v>12</v>
+        <v>6</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.35">
@@ -5770,7 +5784,7 @@
       </c>
       <c r="E30" s="9">
         <f t="shared" si="1"/>
-        <v>12</v>
+        <v>6</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.35">
@@ -5790,7 +5804,7 @@
       </c>
       <c r="E31" s="9">
         <f t="shared" si="1"/>
-        <v>12</v>
+        <v>6</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.35">
@@ -5810,7 +5824,7 @@
       </c>
       <c r="E32" s="9">
         <f t="shared" si="1"/>
-        <v>12</v>
+        <v>6</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.35">
@@ -5830,7 +5844,7 @@
       </c>
       <c r="E33" s="9">
         <f t="shared" si="1"/>
-        <v>12</v>
+        <v>6</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.35">
@@ -5850,7 +5864,7 @@
       </c>
       <c r="E34" s="9">
         <f t="shared" si="1"/>
-        <v>12</v>
+        <v>6</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.35">
@@ -5870,7 +5884,7 @@
       </c>
       <c r="E35" s="9">
         <f t="shared" si="1"/>
-        <v>12</v>
+        <v>6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
[IMPL] LIST/SHOW (Servicios y solicitud Servicio) Se ha añadido las funcionalidades de listar y mostrar servicios y solicitudes de servicios para el rol de administrador.
Falta por implementar la funcionalidad de editar un servicio y una solicitud de servicio. Además, se tiene que implementar la funcionalidad de mostrar y editar el perfil del administrador.
</commit_message>
<xml_diff>
--- a/documentación/Product Backlog/SP2.xlsx
+++ b/documentación/Product Backlog/SP2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alesk\Desktop\Universidad\TFG_app\TFG_app\documentación\Product Backlog\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{317055F7-F968-49E7-8233-F8C026499112}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9FD061A4-81F8-4BCA-BE2B-E057ADC431CE}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="29610" yWindow="-120" windowWidth="19800" windowHeight="11760" xr2:uid="{41FE112A-4516-4423-9CD7-320A9C032A6D}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{41FE112A-4516-4423-9CD7-320A9C032A6D}"/>
   </bookViews>
   <sheets>
     <sheet name="SPRINT-BACKLOG" sheetId="1" r:id="rId1"/>
@@ -321,7 +321,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -358,9 +358,6 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="2" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -882,31 +879,31 @@
                   <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>6</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>6</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>6</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>6</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>6</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>6</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>6</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>6</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>6</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2710,8 +2707,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2BB024A1-16E4-467A-A83B-A5E93171F59F}">
   <dimension ref="A1:O235"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A46" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+    <sheetView tabSelected="1" topLeftCell="A28" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D34" sqref="D34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2719,7 +2716,7 @@
     <col min="1" max="1" width="53.6328125" customWidth="1"/>
     <col min="2" max="2" width="11" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="13.1796875" customWidth="1"/>
-    <col min="4" max="4" width="13.08984375" customWidth="1"/>
+    <col min="4" max="4" width="13.36328125" customWidth="1"/>
     <col min="5" max="5" width="12.81640625" customWidth="1"/>
   </cols>
   <sheetData>
@@ -2747,7 +2744,7 @@
       <c r="A2" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="B2" s="14" t="s">
+      <c r="B2" s="13" t="s">
         <v>25</v>
       </c>
       <c r="C2" s="5">
@@ -2771,7 +2768,7 @@
       <c r="A3" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="14" t="s">
+      <c r="B3" s="13" t="s">
         <v>25</v>
       </c>
       <c r="C3" s="5">
@@ -2798,7 +2795,7 @@
       <c r="A4" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="B4" s="14" t="s">
+      <c r="B4" s="13" t="s">
         <v>25</v>
       </c>
       <c r="C4" s="5">
@@ -2822,7 +2819,7 @@
       <c r="A5" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="B5" s="14" t="s">
+      <c r="B5" s="13" t="s">
         <v>25</v>
       </c>
       <c r="C5" s="5">
@@ -2843,7 +2840,7 @@
       <c r="A6" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="B6" s="14" t="s">
+      <c r="B6" s="13" t="s">
         <v>27</v>
       </c>
       <c r="C6" s="5">
@@ -2864,7 +2861,7 @@
       <c r="A7" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="B7" s="14" t="s">
+      <c r="B7" s="13" t="s">
         <v>27</v>
       </c>
       <c r="C7" s="5">
@@ -2885,7 +2882,7 @@
       <c r="A8" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="B8" s="14" t="s">
+      <c r="B8" s="13" t="s">
         <v>27</v>
       </c>
       <c r="C8" s="5">
@@ -2906,13 +2903,15 @@
       <c r="A9" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="B9" s="14" t="s">
+      <c r="B9" s="13" t="s">
         <v>27</v>
       </c>
       <c r="C9" s="5">
         <v>44230</v>
       </c>
-      <c r="D9" s="5"/>
+      <c r="D9" s="5">
+        <v>44249</v>
+      </c>
       <c r="E9" s="5">
         <v>44231</v>
       </c>
@@ -2925,7 +2924,7 @@
       <c r="A10" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="B10" s="14">
+      <c r="B10" s="13">
         <v>1</v>
       </c>
       <c r="C10" s="5">
@@ -2946,7 +2945,7 @@
       <c r="A11" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="B11" s="14">
+      <c r="B11" s="13">
         <v>1</v>
       </c>
       <c r="C11" s="5">
@@ -2967,7 +2966,7 @@
       <c r="A12" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="B12" s="14">
+      <c r="B12" s="13">
         <v>1</v>
       </c>
       <c r="C12" s="5">
@@ -2988,7 +2987,7 @@
       <c r="A13" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="B13" s="14">
+      <c r="B13" s="13">
         <v>1</v>
       </c>
       <c r="C13" s="5">
@@ -3009,7 +3008,7 @@
       <c r="A14" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="B14" s="14">
+      <c r="B14" s="13">
         <v>1</v>
       </c>
       <c r="C14" s="5">
@@ -3030,7 +3029,7 @@
       <c r="A15" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="B15" s="14">
+      <c r="B15" s="13">
         <v>1</v>
       </c>
       <c r="C15" s="5">
@@ -3051,7 +3050,7 @@
       <c r="A16" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="B16" s="14">
+      <c r="B16" s="13">
         <v>1</v>
       </c>
       <c r="C16" s="5">
@@ -3072,7 +3071,7 @@
       <c r="A17" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="B17" s="14">
+      <c r="B17" s="13">
         <v>1</v>
       </c>
       <c r="C17" s="5">
@@ -3093,7 +3092,7 @@
       <c r="A18" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="B18" s="14">
+      <c r="B18" s="13">
         <v>1</v>
       </c>
       <c r="C18" s="5">
@@ -3114,7 +3113,7 @@
       <c r="A19" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="B19" s="14">
+      <c r="B19" s="13">
         <v>1</v>
       </c>
       <c r="C19" s="5">
@@ -3135,7 +3134,7 @@
       <c r="A20" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="B20" s="14">
+      <c r="B20" s="13">
         <v>1</v>
       </c>
       <c r="C20" s="5">
@@ -3156,7 +3155,7 @@
       <c r="A21" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="B21" s="14">
+      <c r="B21" s="13">
         <v>1</v>
       </c>
       <c r="C21" s="5">
@@ -3177,7 +3176,7 @@
       <c r="A22" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="B22" s="14">
+      <c r="B22" s="13">
         <v>1</v>
       </c>
       <c r="C22" s="5">
@@ -3198,7 +3197,7 @@
       <c r="A23" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="B23" s="14">
+      <c r="B23" s="13">
         <v>1</v>
       </c>
       <c r="C23" s="5">
@@ -3219,13 +3218,15 @@
       <c r="A24" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="B24" s="14">
+      <c r="B24" s="13">
         <v>1</v>
       </c>
       <c r="C24" s="5">
         <v>44237</v>
       </c>
-      <c r="D24" s="5"/>
+      <c r="D24" s="5">
+        <v>44249</v>
+      </c>
       <c r="E24" s="5">
         <v>44238</v>
       </c>
@@ -3238,13 +3239,15 @@
       <c r="A25" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="B25" s="14">
+      <c r="B25" s="13">
         <v>1</v>
       </c>
       <c r="C25" s="5">
         <v>44238</v>
       </c>
-      <c r="D25" s="5"/>
+      <c r="D25" s="5">
+        <v>44249</v>
+      </c>
       <c r="E25" s="5">
         <v>44239</v>
       </c>
@@ -3257,7 +3260,7 @@
       <c r="A26" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="B26" s="14">
+      <c r="B26" s="13">
         <v>1</v>
       </c>
       <c r="C26" s="5">
@@ -3276,13 +3279,15 @@
       <c r="A27" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="B27" s="14">
+      <c r="B27" s="13">
         <v>1</v>
       </c>
       <c r="C27" s="5">
         <v>44239</v>
       </c>
-      <c r="D27" s="5"/>
+      <c r="D27" s="5">
+        <v>44249</v>
+      </c>
       <c r="E27" s="5">
         <v>44242</v>
       </c>
@@ -3295,7 +3300,7 @@
       <c r="A28" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="B28" s="14">
+      <c r="B28" s="13">
         <v>1</v>
       </c>
       <c r="C28" s="5">
@@ -3316,7 +3321,7 @@
       <c r="A29" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="B29" s="14">
+      <c r="B29" s="13">
         <v>1</v>
       </c>
       <c r="C29" s="5">
@@ -3337,7 +3342,7 @@
       <c r="A30" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="B30" s="14">
+      <c r="B30" s="13">
         <v>1</v>
       </c>
       <c r="C30" s="5">
@@ -3358,7 +3363,7 @@
       <c r="A31" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="B31" s="14">
+      <c r="B31" s="13">
         <v>1</v>
       </c>
       <c r="C31" s="5">
@@ -3379,7 +3384,7 @@
       <c r="A32" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="B32" s="14">
+      <c r="B32" s="13">
         <v>1</v>
       </c>
       <c r="C32" s="5">
@@ -3400,7 +3405,7 @@
       <c r="A33" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="B33" s="14">
+      <c r="B33" s="13">
         <v>1</v>
       </c>
       <c r="C33" s="5">
@@ -3421,13 +3426,15 @@
       <c r="A34" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="B34" s="14">
+      <c r="B34" s="13">
         <v>1</v>
       </c>
       <c r="C34" s="5">
         <v>44249</v>
       </c>
-      <c r="D34" s="5"/>
+      <c r="D34" s="5">
+        <v>44249</v>
+      </c>
       <c r="E34" s="5">
         <v>44250</v>
       </c>
@@ -3440,13 +3447,15 @@
       <c r="A35" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="B35" s="14">
+      <c r="B35" s="13">
         <v>1</v>
       </c>
       <c r="C35" s="5">
         <v>44249</v>
       </c>
-      <c r="D35" s="5"/>
+      <c r="D35" s="5">
+        <v>44247</v>
+      </c>
       <c r="E35" s="5">
         <v>44250</v>
       </c>
@@ -3459,7 +3468,7 @@
       <c r="A36" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="B36" s="14">
+      <c r="B36" s="13">
         <v>1</v>
       </c>
       <c r="C36" s="5">
@@ -3474,17 +3483,17 @@
       </c>
       <c r="G36" s="1"/>
     </row>
-    <row r="37" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:7" ht="31" x14ac:dyDescent="0.35">
       <c r="A37" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="B37" s="14">
+      <c r="B37" s="13">
         <v>2</v>
       </c>
       <c r="C37" s="5">
         <v>44197</v>
       </c>
-      <c r="D37" s="13">
+      <c r="D37" s="5">
         <v>44228</v>
       </c>
       <c r="E37" s="5">
@@ -3499,7 +3508,7 @@
       <c r="A38" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="B38" s="14">
+      <c r="B38" s="13">
         <v>2</v>
       </c>
       <c r="C38" s="5">
@@ -5284,7 +5293,7 @@
   <dimension ref="A2:G35"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D22" sqref="D22"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -5296,10 +5305,10 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="B2" s="15" t="s">
+      <c r="B2" s="14" t="s">
         <v>51</v>
       </c>
-      <c r="C2" s="15"/>
+      <c r="C2" s="14"/>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.35">
       <c r="B3" s="11" t="s">
@@ -5721,11 +5730,11 @@
       </c>
       <c r="D27" s="10">
         <f>SUMIF('SPRINT-BACKLOG'!D2:D38,"="&amp;VALUE(A27),'SPRINT-BACKLOG'!B2:B38)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E27" s="9">
         <f t="shared" si="1"/>
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.35">
@@ -5745,7 +5754,7 @@
       </c>
       <c r="E28" s="9">
         <f t="shared" si="1"/>
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.35">
@@ -5760,11 +5769,11 @@
         <v>6.888888888888876</v>
       </c>
       <c r="D29" s="10">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="E29" s="9">
         <f t="shared" si="1"/>
-        <v>6</v>
+        <v>0</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.35">
@@ -5784,7 +5793,7 @@
       </c>
       <c r="E30" s="9">
         <f t="shared" si="1"/>
-        <v>6</v>
+        <v>0</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.35">
@@ -5804,7 +5813,7 @@
       </c>
       <c r="E31" s="9">
         <f t="shared" si="1"/>
-        <v>6</v>
+        <v>0</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.35">
@@ -5824,7 +5833,7 @@
       </c>
       <c r="E32" s="9">
         <f t="shared" si="1"/>
-        <v>6</v>
+        <v>0</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.35">
@@ -5844,7 +5853,7 @@
       </c>
       <c r="E33" s="9">
         <f t="shared" si="1"/>
-        <v>6</v>
+        <v>0</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.35">
@@ -5864,7 +5873,7 @@
       </c>
       <c r="E34" s="9">
         <f t="shared" si="1"/>
-        <v>6</v>
+        <v>0</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.35">
@@ -5884,7 +5893,7 @@
       </c>
       <c r="E35" s="9">
         <f t="shared" si="1"/>
-        <v>6</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
[MOD] Actualizado el sprint backlog Se ha actualizado el contenido del sprint backlog, añadiendo correctamente el sprint burndown.
</commit_message>
<xml_diff>
--- a/documentación/Product Backlog/SP2.xlsx
+++ b/documentación/Product Backlog/SP2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alesk\Desktop\Universidad\TFG_app\TFG_app\documentación\Product Backlog\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9FD061A4-81F8-4BCA-BE2B-E057ADC431CE}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8121735E-ABCB-4A00-9C07-2F831DC3FA02}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{41FE112A-4516-4423-9CD7-320A9C032A6D}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" activeTab="1" xr2:uid="{41FE112A-4516-4423-9CD7-320A9C032A6D}"/>
   </bookViews>
   <sheets>
     <sheet name="SPRINT-BACKLOG" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="51">
   <si>
     <t>Puntos de historia</t>
   </si>
@@ -113,15 +113,6 @@
     <t>Implementación de la funcionalidad de modificar los detalles de una solicitud de servicio (ADM)</t>
   </si>
   <si>
-    <t>0.5</t>
-  </si>
-  <si>
-    <t>Q</t>
-  </si>
-  <si>
-    <t>1.5</t>
-  </si>
-  <si>
     <t>Creación de la vista principal (EMP)</t>
   </si>
   <si>
@@ -144,12 +135,6 @@
   </si>
   <si>
     <t>Implementación de la funcionalidad de listar los Servicios (ADM)</t>
-  </si>
-  <si>
-    <t>Implementación de la funcionalidad de modificar los detalles de un Servicio (EMP)</t>
-  </si>
-  <si>
-    <t>Implemtación de la funcionalidad de registrar un servicio a partir de una Solicitud de servicio (ADM)</t>
   </si>
   <si>
     <t>Implementación de la funcionalidad de modificar los detalles de un Servicio (TRA)</t>
@@ -201,6 +186,9 @@
   </si>
   <si>
     <t>Creación de la vista principal (TRA)</t>
+  </si>
+  <si>
+    <t>Implementación de la funcionalidad de listar los Servicios (EMP)</t>
   </si>
 </sst>
 </file>
@@ -321,7 +309,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -365,6 +353,13 @@
     <xf numFmtId="0" fontId="6" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="2" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="4" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -390,197 +385,6 @@
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
-  <c:date1904 val="0"/>
-  <c:lang val="es-ES"/>
-  <c:roundedCorners val="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="102"/>
-    </mc:Choice>
-    <mc:Fallback>
-      <c:style val="2"/>
-    </mc:Fallback>
-  </mc:AlternateContent>
-  <c:chart>
-    <c:autoTitleDeleted val="0"/>
-    <c:plotArea>
-      <c:layout/>
-      <c:lineChart>
-        <c:grouping val="standard"/>
-        <c:varyColors val="0"/>
-        <c:dLbls>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-        </c:dLbls>
-        <c:marker val="1"/>
-        <c:smooth val="0"/>
-        <c:axId val="428214632"/>
-        <c:axId val="428217584"/>
-      </c:lineChart>
-      <c:catAx>
-        <c:axId val="428214632"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="b"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-            <a:solidFill>
-              <a:schemeClr val="tx1">
-                <a:lumMod val="15000"/>
-                <a:lumOff val="85000"/>
-              </a:schemeClr>
-            </a:solidFill>
-            <a:round/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="es-ES"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="428217584"/>
-        <c:crosses val="autoZero"/>
-        <c:auto val="1"/>
-        <c:lblAlgn val="ctr"/>
-        <c:lblOffset val="100"/>
-        <c:noMultiLvlLbl val="0"/>
-      </c:catAx>
-      <c:valAx>
-        <c:axId val="428217584"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="l"/>
-        <c:majorGridlines>
-          <c:spPr>
-            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="15000"/>
-                  <a:lumOff val="85000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-        </c:majorGridlines>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln>
-            <a:noFill/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="es-ES"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="428214632"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="between"/>
-      </c:valAx>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-    </c:plotArea>
-    <c:plotVisOnly val="1"/>
-    <c:dispBlanksAs val="gap"/>
-    <c:extLst>
-      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
-        <c16r3:dataDisplayOptions16>
-          <c16r3:dispNaAsBlank val="1"/>
-        </c16r3:dataDisplayOptions16>
-      </c:ext>
-    </c:extLst>
-    <c:showDLblsOverMax val="0"/>
-  </c:chart>
-  <c:spPr>
-    <a:solidFill>
-      <a:schemeClr val="bg1"/>
-    </a:solidFill>
-    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-      <a:solidFill>
-        <a:schemeClr val="tx1">
-          <a:lumMod val="15000"/>
-          <a:lumOff val="85000"/>
-        </a:schemeClr>
-      </a:solidFill>
-      <a:round/>
-    </a:ln>
-    <a:effectLst/>
-  </c:spPr>
-  <c:txPr>
-    <a:bodyPr/>
-    <a:lstStyle/>
-    <a:p>
-      <a:pPr>
-        <a:defRPr/>
-      </a:pPr>
-      <a:endParaRPr lang="es-ES"/>
-    </a:p>
-  </c:txPr>
-  <c:printSettings>
-    <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
-    <c:pageSetup/>
-  </c:printSettings>
-</c:chartSpace>
-</file>
-
-<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="es-ES"/>
@@ -698,88 +502,88 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="28"/>
                 <c:pt idx="0">
-                  <c:v>31</c:v>
+                  <c:v>37</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>29.851851851851851</c:v>
+                  <c:v>35.629629629629626</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>28.703703703703702</c:v>
+                  <c:v>34.259259259259252</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>27.555555555555554</c:v>
+                  <c:v>32.888888888888879</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>26.407407407407405</c:v>
+                  <c:v>31.518518518518508</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>25.259259259259256</c:v>
+                  <c:v>30.148148148148138</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>24.111111111111107</c:v>
+                  <c:v>28.777777777777768</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>22.962962962962958</c:v>
+                  <c:v>27.407407407407398</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>21.81481481481481</c:v>
+                  <c:v>26.037037037037027</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>20.666666666666661</c:v>
+                  <c:v>24.666666666666657</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>19.518518518518512</c:v>
+                  <c:v>23.296296296296287</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>18.370370370370363</c:v>
+                  <c:v>21.925925925925917</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>17.222222222222214</c:v>
+                  <c:v>20.555555555555546</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>16.074074074074066</c:v>
+                  <c:v>19.185185185185176</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>14.925925925925917</c:v>
+                  <c:v>17.814814814814806</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>13.777777777777768</c:v>
+                  <c:v>16.444444444444436</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>12.629629629629619</c:v>
+                  <c:v>15.074074074074066</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>11.48148148148147</c:v>
+                  <c:v>13.703703703703695</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>10.333333333333321</c:v>
+                  <c:v>12.333333333333325</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>9.1851851851851727</c:v>
+                  <c:v>10.962962962962955</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>8.0370370370370239</c:v>
+                  <c:v>9.5925925925925846</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>6.888888888888876</c:v>
+                  <c:v>8.2222222222222143</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>5.740740740740728</c:v>
+                  <c:v>6.8518518518518441</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>4.5925925925925801</c:v>
+                  <c:v>5.4814814814814738</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>3.4444444444444322</c:v>
+                  <c:v>4.1111111111111036</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>2.2962962962962843</c:v>
+                  <c:v>2.7407407407407334</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>1.1481481481481361</c:v>
+                  <c:v>1.3703703703703629</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>-1.1990408665951691E-14</c:v>
+                  <c:v>-7.5495165674510645E-15</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -822,79 +626,79 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="28"/>
                 <c:pt idx="0">
-                  <c:v>29</c:v>
+                  <c:v>35</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>27</c:v>
+                  <c:v>33</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>27</c:v>
+                  <c:v>31</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>22</c:v>
+                  <c:v>29.5</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>22</c:v>
+                  <c:v>26.5</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>21</c:v>
+                  <c:v>26.5</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>21</c:v>
+                  <c:v>26.5</c:v>
                 </c:pt>
                 <c:pt idx="7">
+                  <c:v>24.5</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>22.5</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>21.5</c:v>
+                </c:pt>
+                <c:pt idx="10">
                   <c:v>18</c:v>
                 </c:pt>
-                <c:pt idx="8">
-                  <c:v>16</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>16</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>16</c:v>
-                </c:pt>
                 <c:pt idx="11">
-                  <c:v>16</c:v>
+                  <c:v>18</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>16</c:v>
+                  <c:v>18</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>16</c:v>
+                  <c:v>18</c:v>
                 </c:pt>
                 <c:pt idx="14">
                   <c:v>14</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>9</c:v>
+                  <c:v>12.5</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>7</c:v>
+                  <c:v>9.5</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>6</c:v>
+                  <c:v>9.5</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>6</c:v>
+                  <c:v>9.5</c:v>
                 </c:pt>
                 <c:pt idx="19">
+                  <c:v>9.5</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>9.5</c:v>
+                </c:pt>
+                <c:pt idx="21">
                   <c:v>5</c:v>
                 </c:pt>
-                <c:pt idx="20">
-                  <c:v>5</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>0</c:v>
-                </c:pt>
                 <c:pt idx="22">
-                  <c:v>0</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>0</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>0</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="25">
                   <c:v>0</c:v>
@@ -1292,550 +1096,7 @@
 </cs:colorStyle>
 </file>
 
-<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
-  <a:schemeClr val="accent1"/>
-  <a:schemeClr val="accent2"/>
-  <a:schemeClr val="accent3"/>
-  <a:schemeClr val="accent4"/>
-  <a:schemeClr val="accent5"/>
-  <a:schemeClr val="accent6"/>
-  <cs:variation/>
-  <cs:variation>
-    <a:lumMod val="60000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="80000"/>
-    <a:lumOff val="20000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="80000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="60000"/>
-    <a:lumOff val="40000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="50000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="70000"/>
-    <a:lumOff val="30000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="70000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="50000"/>
-    <a:lumOff val="50000"/>
-  </cs:variation>
-</cs:colorStyle>
-</file>
-
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="332">
-  <cs:axisTitle>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="1000" kern="1200"/>
-  </cs:axisTitle>
-  <cs:categoryAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:categoryAxis>
-  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="bg1"/>
-      </a:solidFill>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="1000" kern="1200"/>
-  </cs:chartArea>
-  <cs:dataLabel>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="75000"/>
-        <a:lumOff val="25000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:dataLabel>
-  <cs:dataLabelCallout>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="lt1"/>
-      </a:solidFill>
-      <a:ln>
-        <a:solidFill>
-          <a:schemeClr val="dk1">
-            <a:lumMod val="25000"/>
-            <a:lumOff val="75000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
-      <a:spAutoFit/>
-    </cs:bodyPr>
-  </cs:dataLabelCallout>
-  <cs:dataPoint>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="1">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:dataPoint>
-  <cs:dataPoint3D>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="1">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:dataPoint3D>
-  <cs:dataPointLine>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="1"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="28575" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointLine>
-  <cs:dataPointMarker>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="1">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointMarker>
-  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
-  <cs:dataPointWireframe>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="1"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointWireframe>
-  <cs:dataTable>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:dataTable>
-  <cs:downBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="dk1">
-          <a:lumMod val="65000"/>
-          <a:lumOff val="35000"/>
-        </a:schemeClr>
-      </a:solidFill>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-  </cs:downBar>
-  <cs:dropLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dropLine>
-  <cs:errorBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:errorBar>
-  <cs:floor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln>
-        <a:noFill/>
-      </a:ln>
-    </cs:spPr>
-  </cs:floor>
-  <cs:gridlineMajor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:gridlineMajor>
-  <cs:gridlineMinor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="5000"/>
-            <a:lumOff val="95000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:gridlineMinor>
-  <cs:hiLoLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="75000"/>
-            <a:lumOff val="25000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:hiLoLine>
-  <cs:leaderLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:leaderLine>
-  <cs:legend>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:legend>
-  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:plotArea>
-  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:plotArea3D>
-  <cs:seriesAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:seriesAxis>
-  <cs:seriesLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:seriesLine>
-  <cs:title>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
-  </cs:title>
-  <cs:trendline>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="19050" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:prstDash val="sysDot"/>
-      </a:ln>
-    </cs:spPr>
-  </cs:trendline>
-  <cs:trendlineLabel>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:trendlineLabel>
-  <cs:upBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="lt1"/>
-      </a:solidFill>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-  </cs:upBar>
-  <cs:valueAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:valueAxis>
-  <cs:wall>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln>
-        <a:noFill/>
-      </a:ln>
-    </cs:spPr>
-  </cs:wall>
-</cs:chartStyle>
-</file>
-
-<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="233">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -2335,51 +1596,15 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>35718</xdr:colOff>
-      <xdr:row>10</xdr:row>
-      <xdr:rowOff>307180</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>35718</xdr:colOff>
-      <xdr:row>18</xdr:row>
-      <xdr:rowOff>2380</xdr:rowOff>
-    </xdr:to>
-    <xdr:graphicFrame macro="">
-      <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="5" name="Gráfico 4">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4A424B49-5972-48F7-9D00-04C1C9494812}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvGraphicFramePr/>
-      </xdr:nvGraphicFramePr>
-      <xdr:xfrm>
-        <a:off x="0" y="0"/>
-        <a:ext cx="0" cy="0"/>
-      </xdr:xfrm>
-      <a:graphic>
-        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
-        </a:graphicData>
-      </a:graphic>
-    </xdr:graphicFrame>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>38</xdr:row>
+      <xdr:row>36</xdr:row>
       <xdr:rowOff>160336</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
       <xdr:colOff>752475</xdr:colOff>
-      <xdr:row>63</xdr:row>
+      <xdr:row>61</xdr:row>
       <xdr:rowOff>9524</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -2399,7 +1624,7 @@
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -2705,10 +1930,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2BB024A1-16E4-467A-A83B-A5E93171F59F}">
-  <dimension ref="A1:O235"/>
+  <dimension ref="A1:N233"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D34" sqref="D34"/>
+    <sheetView topLeftCell="A40" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2720,7 +1945,7 @@
     <col min="5" max="5" width="12.81640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" ht="31" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:14" ht="31" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>8</v>
       </c>
@@ -2740,21 +1965,21 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:15" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:14" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A2" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="B2" s="13" t="s">
-        <v>25</v>
+        <v>40</v>
+      </c>
+      <c r="B2" s="13">
+        <v>2</v>
       </c>
       <c r="C2" s="5">
-        <v>44228</v>
+        <v>44197</v>
       </c>
       <c r="D2" s="5">
         <v>44228</v>
       </c>
       <c r="E2" s="5">
-        <v>44229</v>
+        <v>44197</v>
       </c>
       <c r="F2" s="4" t="s">
         <v>7</v>
@@ -2764,15 +1989,15 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:15" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:14" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A3" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="B3" s="13" t="s">
-        <v>25</v>
+        <v>10</v>
+      </c>
+      <c r="B3" s="13">
+        <v>0.5</v>
       </c>
       <c r="C3" s="5">
-        <v>44228</v>
+        <v>44229</v>
       </c>
       <c r="D3" s="5">
         <v>44229</v>
@@ -2787,19 +2012,16 @@
       <c r="N3" t="s">
         <v>6</v>
       </c>
-      <c r="O3" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="4" spans="1:15" ht="15.5" x14ac:dyDescent="0.35">
+    </row>
+    <row r="4" spans="1:14" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A4" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="B4" s="13" t="s">
-        <v>25</v>
+        <v>9</v>
+      </c>
+      <c r="B4" s="13">
+        <v>0.5</v>
       </c>
       <c r="C4" s="5">
-        <v>44228</v>
+        <v>44229</v>
       </c>
       <c r="D4" s="5">
         <v>44229</v>
@@ -2815,15 +2037,15 @@
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:15" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:14" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A5" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="B5" s="13" t="s">
-        <v>25</v>
+        <v>12</v>
+      </c>
+      <c r="B5" s="13">
+        <v>0.5</v>
       </c>
       <c r="C5" s="5">
-        <v>44228</v>
+        <v>44229</v>
       </c>
       <c r="D5" s="5">
         <v>44229</v>
@@ -2836,39 +2058,39 @@
       </c>
       <c r="G5" s="1"/>
     </row>
-    <row r="6" spans="1:15" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:14" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A6" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="B6" s="13" t="s">
-        <v>27</v>
+        <v>11</v>
+      </c>
+      <c r="B6" s="13">
+        <v>0.5</v>
       </c>
       <c r="C6" s="5">
         <v>44229</v>
       </c>
       <c r="D6" s="5">
-        <v>44231</v>
+        <v>44229</v>
       </c>
       <c r="E6" s="5">
-        <v>44230</v>
+        <v>44229</v>
       </c>
       <c r="F6" s="4" t="s">
         <v>7</v>
       </c>
       <c r="G6" s="1"/>
     </row>
-    <row r="7" spans="1:15" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:14" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A7" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="B7" s="13" t="s">
-        <v>27</v>
+        <v>37</v>
+      </c>
+      <c r="B7" s="13">
+        <v>1</v>
       </c>
       <c r="C7" s="5">
-        <v>44229</v>
+        <v>44230</v>
       </c>
       <c r="D7" s="5">
-        <v>44231</v>
+        <v>44230</v>
       </c>
       <c r="E7" s="5">
         <v>44230</v>
@@ -2878,51 +2100,51 @@
       </c>
       <c r="G7" s="1"/>
     </row>
-    <row r="8" spans="1:15" ht="31" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:14" ht="31" x14ac:dyDescent="0.35">
       <c r="A8" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="B8" s="13" t="s">
-        <v>27</v>
+        <v>36</v>
+      </c>
+      <c r="B8" s="13">
+        <v>1</v>
       </c>
       <c r="C8" s="5">
         <v>44230</v>
       </c>
       <c r="D8" s="5">
-        <v>44245</v>
+        <v>44230</v>
       </c>
       <c r="E8" s="5">
+        <v>44230</v>
+      </c>
+      <c r="F8" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="G8" s="1"/>
+    </row>
+    <row r="9" spans="1:14" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A9" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B9" s="13">
+        <v>1.5</v>
+      </c>
+      <c r="C9" s="5">
         <v>44231</v>
       </c>
-      <c r="F8" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="G8" s="1"/>
-    </row>
-    <row r="9" spans="1:15" ht="31" x14ac:dyDescent="0.35">
-      <c r="A9" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="B9" s="13" t="s">
-        <v>27</v>
-      </c>
-      <c r="C9" s="5">
-        <v>44230</v>
-      </c>
       <c r="D9" s="5">
-        <v>44249</v>
+        <v>44231</v>
       </c>
       <c r="E9" s="5">
         <v>44231</v>
       </c>
       <c r="F9" s="4" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="G9" s="1"/>
     </row>
-    <row r="10" spans="1:15" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:14" ht="31" x14ac:dyDescent="0.35">
       <c r="A10" s="3" t="s">
-        <v>42</v>
+        <v>16</v>
       </c>
       <c r="B10" s="13">
         <v>1</v>
@@ -2931,7 +2153,7 @@
         <v>44231</v>
       </c>
       <c r="D10" s="5">
-        <v>44231</v>
+        <v>44232</v>
       </c>
       <c r="E10" s="5">
         <v>44232</v>
@@ -2941,168 +2163,168 @@
       </c>
       <c r="G10" s="1"/>
     </row>
-    <row r="11" spans="1:15" ht="31" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:14" ht="31" x14ac:dyDescent="0.35">
       <c r="A11" s="3" t="s">
-        <v>41</v>
+        <v>15</v>
       </c>
       <c r="B11" s="13">
         <v>1</v>
       </c>
       <c r="C11" s="5">
-        <v>44231</v>
+        <v>44232</v>
       </c>
       <c r="D11" s="5">
-        <v>44231</v>
+        <v>44232</v>
       </c>
       <c r="E11" s="5">
-        <v>44232</v>
+        <v>44235</v>
       </c>
       <c r="F11" s="4" t="s">
         <v>7</v>
       </c>
       <c r="G11" s="1"/>
     </row>
-    <row r="12" spans="1:15" ht="31" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:14" ht="31" x14ac:dyDescent="0.35">
       <c r="A12" s="3" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="B12" s="13">
         <v>1</v>
       </c>
       <c r="C12" s="5">
-        <v>44231</v>
+        <v>44232</v>
       </c>
       <c r="D12" s="5">
+        <v>44232</v>
+      </c>
+      <c r="E12" s="5">
         <v>44235</v>
-      </c>
-      <c r="E12" s="5">
-        <v>44232</v>
       </c>
       <c r="F12" s="4" t="s">
         <v>7</v>
       </c>
       <c r="G12" s="1"/>
     </row>
-    <row r="13" spans="1:15" ht="31" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:14" ht="31" x14ac:dyDescent="0.35">
       <c r="A13" s="3" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B13" s="13">
         <v>1</v>
       </c>
       <c r="C13" s="5">
-        <v>44232</v>
+        <v>44235</v>
       </c>
       <c r="D13" s="5">
-        <v>44233</v>
+        <v>44235</v>
       </c>
       <c r="E13" s="5">
-        <v>44235</v>
+        <v>44236</v>
       </c>
       <c r="F13" s="4" t="s">
         <v>7</v>
       </c>
       <c r="G13" s="1"/>
     </row>
-    <row r="14" spans="1:15" ht="31" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:14" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A14" s="3" t="s">
-        <v>15</v>
+        <v>38</v>
       </c>
       <c r="B14" s="13">
         <v>1</v>
       </c>
       <c r="C14" s="5">
-        <v>44232</v>
+        <v>44235</v>
       </c>
       <c r="D14" s="5">
-        <v>44234</v>
+        <v>44235</v>
       </c>
       <c r="E14" s="5">
-        <v>44235</v>
+        <v>44236</v>
       </c>
       <c r="F14" s="4" t="s">
         <v>7</v>
       </c>
       <c r="G14" s="1"/>
     </row>
-    <row r="15" spans="1:15" ht="31" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:14" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A15" s="3" t="s">
-        <v>17</v>
+        <v>39</v>
       </c>
       <c r="B15" s="13">
         <v>1</v>
       </c>
       <c r="C15" s="5">
-        <v>44235</v>
+        <v>44236</v>
       </c>
       <c r="D15" s="5">
-        <v>44234</v>
+        <v>44236</v>
       </c>
       <c r="E15" s="5">
-        <v>44236</v>
+        <v>44237</v>
       </c>
       <c r="F15" s="4" t="s">
         <v>7</v>
       </c>
       <c r="G15" s="1"/>
     </row>
-    <row r="16" spans="1:15" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:14" ht="31" x14ac:dyDescent="0.35">
       <c r="A16" s="3" t="s">
-        <v>43</v>
+        <v>27</v>
       </c>
       <c r="B16" s="13">
         <v>1</v>
       </c>
       <c r="C16" s="5">
-        <v>44239</v>
+        <v>44236</v>
       </c>
       <c r="D16" s="5">
-        <v>44235</v>
+        <v>44236</v>
       </c>
       <c r="E16" s="5">
-        <v>44242</v>
+        <v>44237</v>
       </c>
       <c r="F16" s="4" t="s">
         <v>7</v>
       </c>
       <c r="G16" s="1"/>
     </row>
-    <row r="17" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:7" ht="31" x14ac:dyDescent="0.35">
       <c r="A17" s="3" t="s">
-        <v>44</v>
+        <v>28</v>
       </c>
       <c r="B17" s="13">
         <v>1</v>
       </c>
       <c r="C17" s="5">
-        <v>44242</v>
+        <v>44237</v>
       </c>
       <c r="D17" s="5">
-        <v>44235</v>
+        <v>44237</v>
       </c>
       <c r="E17" s="5">
-        <v>44243</v>
+        <v>44238</v>
       </c>
       <c r="F17" s="4" t="s">
         <v>7</v>
       </c>
       <c r="G17" s="1"/>
     </row>
-    <row r="18" spans="1:7" ht="31" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A18" s="3" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="B18" s="13">
-        <v>1</v>
+        <v>1.5</v>
       </c>
       <c r="C18" s="5">
-        <v>44242</v>
+        <v>44237</v>
       </c>
       <c r="D18" s="5">
-        <v>44236</v>
+        <v>44238</v>
       </c>
       <c r="E18" s="5">
-        <v>44243</v>
+        <v>44238</v>
       </c>
       <c r="F18" s="4" t="s">
         <v>7</v>
@@ -3111,19 +2333,19 @@
     </row>
     <row r="19" spans="1:7" ht="31" x14ac:dyDescent="0.35">
       <c r="A19" s="3" t="s">
-        <v>31</v>
+        <v>19</v>
       </c>
       <c r="B19" s="13">
         <v>1</v>
       </c>
       <c r="C19" s="5">
-        <v>44243</v>
+        <v>44238</v>
       </c>
       <c r="D19" s="5">
-        <v>44236</v>
+        <v>44238</v>
       </c>
       <c r="E19" s="5">
-        <v>44244</v>
+        <v>44239</v>
       </c>
       <c r="F19" s="4" t="s">
         <v>7</v>
@@ -3132,19 +2354,19 @@
     </row>
     <row r="20" spans="1:7" ht="31" x14ac:dyDescent="0.35">
       <c r="A20" s="3" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="B20" s="13">
         <v>1</v>
       </c>
       <c r="C20" s="5">
-        <v>44235</v>
+        <v>44238</v>
       </c>
       <c r="D20" s="5">
-        <v>44243</v>
+        <v>44238</v>
       </c>
       <c r="E20" s="5">
-        <v>44236</v>
+        <v>44239</v>
       </c>
       <c r="F20" s="4" t="s">
         <v>7</v>
@@ -3153,19 +2375,19 @@
     </row>
     <row r="21" spans="1:7" ht="31" x14ac:dyDescent="0.35">
       <c r="A21" s="3" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="B21" s="13">
         <v>1</v>
       </c>
       <c r="C21" s="5">
-        <v>44236</v>
+        <v>44239</v>
       </c>
       <c r="D21" s="5">
         <v>44242</v>
       </c>
       <c r="E21" s="5">
-        <v>44237</v>
+        <v>44240</v>
       </c>
       <c r="F21" s="4" t="s">
         <v>7</v>
@@ -3174,19 +2396,19 @@
     </row>
     <row r="22" spans="1:7" ht="31" x14ac:dyDescent="0.35">
       <c r="A22" s="3" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B22" s="13">
         <v>1</v>
       </c>
       <c r="C22" s="5">
-        <v>44236</v>
+        <v>44239</v>
       </c>
       <c r="D22" s="5">
-        <v>44243</v>
+        <v>44242</v>
       </c>
       <c r="E22" s="5">
-        <v>44237</v>
+        <v>44240</v>
       </c>
       <c r="F22" s="4" t="s">
         <v>7</v>
@@ -3195,19 +2417,19 @@
     </row>
     <row r="23" spans="1:7" ht="31" x14ac:dyDescent="0.35">
       <c r="A23" s="3" t="s">
-        <v>21</v>
+        <v>50</v>
       </c>
       <c r="B23" s="13">
         <v>1</v>
       </c>
       <c r="C23" s="5">
-        <v>44237</v>
+        <v>44240</v>
       </c>
       <c r="D23" s="5">
         <v>44242</v>
       </c>
       <c r="E23" s="5">
-        <v>44238</v>
+        <v>44242</v>
       </c>
       <c r="F23" s="4" t="s">
         <v>7</v>
@@ -3216,40 +2438,40 @@
     </row>
     <row r="24" spans="1:7" ht="31" x14ac:dyDescent="0.35">
       <c r="A24" s="3" t="s">
-        <v>22</v>
+        <v>29</v>
       </c>
       <c r="B24" s="13">
         <v>1</v>
       </c>
       <c r="C24" s="5">
-        <v>44237</v>
+        <v>44240</v>
       </c>
       <c r="D24" s="5">
-        <v>44249</v>
+        <v>44242</v>
       </c>
       <c r="E24" s="5">
-        <v>44238</v>
+        <v>44242</v>
       </c>
       <c r="F24" s="4" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="G24" s="1"/>
     </row>
     <row r="25" spans="1:7" ht="31" x14ac:dyDescent="0.35">
       <c r="A25" s="3" t="s">
-        <v>23</v>
+        <v>49</v>
       </c>
       <c r="B25" s="13">
-        <v>1</v>
+        <v>1.5</v>
       </c>
       <c r="C25" s="5">
-        <v>44238</v>
+        <v>44243</v>
       </c>
       <c r="D25" s="5">
-        <v>44249</v>
+        <v>44243</v>
       </c>
       <c r="E25" s="5">
-        <v>44239</v>
+        <v>44244</v>
       </c>
       <c r="F25" s="4" t="s">
         <v>5</v>
@@ -3258,47 +2480,49 @@
     </row>
     <row r="26" spans="1:7" ht="31" x14ac:dyDescent="0.35">
       <c r="A26" s="3" t="s">
-        <v>24</v>
+        <v>35</v>
       </c>
       <c r="B26" s="13">
         <v>1</v>
       </c>
       <c r="C26" s="5">
-        <v>44238</v>
-      </c>
-      <c r="D26" s="5"/>
+        <v>44243</v>
+      </c>
+      <c r="D26" s="5">
+        <v>44244</v>
+      </c>
       <c r="E26" s="5">
-        <v>44239</v>
+        <v>44244</v>
       </c>
       <c r="F26" s="4" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="G26" s="1"/>
     </row>
     <row r="27" spans="1:7" ht="31" x14ac:dyDescent="0.35">
       <c r="A27" s="3" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="B27" s="13">
         <v>1</v>
       </c>
       <c r="C27" s="5">
-        <v>44239</v>
+        <v>44244</v>
       </c>
       <c r="D27" s="5">
-        <v>44249</v>
+        <v>44244</v>
       </c>
       <c r="E27" s="5">
-        <v>44242</v>
+        <v>44245</v>
       </c>
       <c r="F27" s="4" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="G27" s="1"/>
     </row>
     <row r="28" spans="1:7" ht="31" x14ac:dyDescent="0.35">
       <c r="A28" s="3" t="s">
-        <v>19</v>
+        <v>33</v>
       </c>
       <c r="B28" s="13">
         <v>1</v>
@@ -3307,7 +2531,7 @@
         <v>44244</v>
       </c>
       <c r="D28" s="5">
-        <v>44243</v>
+        <v>44244</v>
       </c>
       <c r="E28" s="5">
         <v>44245</v>
@@ -3317,21 +2541,21 @@
       </c>
       <c r="G28" s="1"/>
     </row>
-    <row r="29" spans="1:7" ht="31" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A29" s="3" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="B29" s="13">
-        <v>1</v>
+        <v>1.5</v>
       </c>
       <c r="C29" s="5">
-        <v>44244</v>
+        <v>44245</v>
       </c>
       <c r="D29" s="5">
-        <v>44243</v>
+        <v>44249</v>
       </c>
       <c r="E29" s="5">
-        <v>44245</v>
+        <v>44246</v>
       </c>
       <c r="F29" s="4" t="s">
         <v>7</v>
@@ -3340,7 +2564,7 @@
     </row>
     <row r="30" spans="1:7" ht="31" x14ac:dyDescent="0.35">
       <c r="A30" s="3" t="s">
-        <v>36</v>
+        <v>22</v>
       </c>
       <c r="B30" s="13">
         <v>1</v>
@@ -3349,7 +2573,7 @@
         <v>44245</v>
       </c>
       <c r="D30" s="5">
-        <v>44243</v>
+        <v>44249</v>
       </c>
       <c r="E30" s="5">
         <v>44246</v>
@@ -3361,19 +2585,19 @@
     </row>
     <row r="31" spans="1:7" ht="31" x14ac:dyDescent="0.35">
       <c r="A31" s="3" t="s">
-        <v>40</v>
+        <v>23</v>
       </c>
       <c r="B31" s="13">
         <v>1</v>
       </c>
       <c r="C31" s="5">
-        <v>44245</v>
+        <v>44246</v>
       </c>
       <c r="D31" s="5">
-        <v>44244</v>
+        <v>44249</v>
       </c>
       <c r="E31" s="5">
-        <v>44246</v>
+        <v>44249</v>
       </c>
       <c r="F31" s="4" t="s">
         <v>7</v>
@@ -3382,7 +2606,7 @@
     </row>
     <row r="32" spans="1:7" ht="31" x14ac:dyDescent="0.35">
       <c r="A32" s="3" t="s">
-        <v>39</v>
+        <v>24</v>
       </c>
       <c r="B32" s="13">
         <v>1</v>
@@ -3391,7 +2615,7 @@
         <v>44246</v>
       </c>
       <c r="D32" s="5">
-        <v>44244</v>
+        <v>44249</v>
       </c>
       <c r="E32" s="5">
         <v>44249</v>
@@ -3403,19 +2627,19 @@
     </row>
     <row r="33" spans="1:7" ht="31" x14ac:dyDescent="0.35">
       <c r="A33" s="3" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="B33" s="13">
         <v>1</v>
       </c>
       <c r="C33" s="5">
-        <v>44246</v>
+        <v>44249</v>
       </c>
       <c r="D33" s="5">
-        <v>44245</v>
+        <v>44250</v>
       </c>
       <c r="E33" s="5">
-        <v>44249</v>
+        <v>44250</v>
       </c>
       <c r="F33" s="4" t="s">
         <v>7</v>
@@ -3424,7 +2648,7 @@
     </row>
     <row r="34" spans="1:7" ht="31" x14ac:dyDescent="0.35">
       <c r="A34" s="3" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="B34" s="13">
         <v>1</v>
@@ -3433,94 +2657,74 @@
         <v>44249</v>
       </c>
       <c r="D34" s="5">
-        <v>44249</v>
+        <v>44250</v>
       </c>
       <c r="E34" s="5">
         <v>44250</v>
       </c>
       <c r="F34" s="4" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="G34" s="1"/>
     </row>
     <row r="35" spans="1:7" ht="31" x14ac:dyDescent="0.35">
       <c r="A35" s="3" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="B35" s="13">
         <v>1</v>
       </c>
       <c r="C35" s="5">
-        <v>44249</v>
+        <v>44250</v>
       </c>
       <c r="D35" s="5">
-        <v>44247</v>
+        <v>44251</v>
       </c>
       <c r="E35" s="5">
-        <v>44250</v>
+        <v>44251</v>
       </c>
       <c r="F35" s="4" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="G35" s="1"/>
     </row>
-    <row r="36" spans="1:7" ht="31" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A36" s="3" t="s">
-        <v>33</v>
+        <v>41</v>
       </c>
       <c r="B36" s="13">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C36" s="5">
-        <v>44250</v>
-      </c>
-      <c r="D36" s="5"/>
+        <v>44220</v>
+      </c>
+      <c r="D36" s="5">
+        <v>44253</v>
+      </c>
       <c r="E36" s="5">
-        <v>44251</v>
+        <v>44221</v>
       </c>
       <c r="F36" s="4" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="G36" s="1"/>
     </row>
-    <row r="37" spans="1:7" ht="31" x14ac:dyDescent="0.35">
-      <c r="A37" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="B37" s="13">
-        <v>2</v>
-      </c>
-      <c r="C37" s="5">
-        <v>44197</v>
-      </c>
-      <c r="D37" s="5">
-        <v>44228</v>
-      </c>
-      <c r="E37" s="5">
-        <v>44197</v>
-      </c>
-      <c r="F37" s="4" t="s">
-        <v>7</v>
-      </c>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A37" s="1"/>
+      <c r="B37" s="1"/>
+      <c r="C37" s="1"/>
+      <c r="D37" s="1"/>
+      <c r="E37" s="1"/>
+      <c r="F37" s="1"/>
       <c r="G37" s="1"/>
     </row>
-    <row r="38" spans="1:7" ht="31" x14ac:dyDescent="0.35">
-      <c r="A38" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="B38" s="13">
-        <v>2</v>
-      </c>
-      <c r="C38" s="5">
-        <v>44220</v>
-      </c>
-      <c r="D38" s="5"/>
-      <c r="E38" s="5">
-        <v>44221</v>
-      </c>
-      <c r="F38" s="4" t="s">
-        <v>5</v>
-      </c>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A38" s="1"/>
+      <c r="B38" s="1"/>
+      <c r="C38" s="1"/>
+      <c r="D38" s="1"/>
+      <c r="E38" s="1"/>
+      <c r="F38" s="1"/>
       <c r="G38" s="1"/>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.35">
@@ -3776,27 +2980,27 @@
       <c r="G66" s="1"/>
     </row>
     <row r="67" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A67" s="1"/>
-      <c r="B67" s="1"/>
-      <c r="C67" s="1"/>
-      <c r="D67" s="1"/>
-      <c r="E67" s="1"/>
-      <c r="F67" s="1"/>
       <c r="G67" s="1"/>
     </row>
     <row r="68" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A68" s="1"/>
-      <c r="B68" s="1"/>
-      <c r="C68" s="1"/>
-      <c r="D68" s="1"/>
-      <c r="E68" s="1"/>
-      <c r="F68" s="1"/>
       <c r="G68" s="1"/>
     </row>
     <row r="69" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A69" s="1"/>
+      <c r="B69" s="1"/>
+      <c r="C69" s="1"/>
+      <c r="D69" s="1"/>
+      <c r="E69" s="1"/>
+      <c r="F69" s="1"/>
       <c r="G69" s="1"/>
     </row>
     <row r="70" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A70" s="1"/>
+      <c r="B70" s="1"/>
+      <c r="C70" s="1"/>
+      <c r="D70" s="1"/>
+      <c r="E70" s="1"/>
+      <c r="F70" s="1"/>
       <c r="G70" s="1"/>
     </row>
     <row r="71" spans="1:7" x14ac:dyDescent="0.35">
@@ -5258,27 +4462,14 @@
       <c r="G232" s="1"/>
     </row>
     <row r="233" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A233" s="1"/>
-      <c r="B233" s="1"/>
       <c r="C233" s="1"/>
-      <c r="D233" s="1"/>
-      <c r="E233" s="1"/>
-      <c r="F233" s="1"/>
-    </row>
-    <row r="234" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A234" s="1"/>
-      <c r="B234" s="1"/>
-      <c r="C234" s="1"/>
-      <c r="D234" s="1"/>
-      <c r="E234" s="1"/>
-      <c r="F234" s="1"/>
-    </row>
-    <row r="235" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="C235" s="1"/>
     </row>
   </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F36">
+    <sortCondition ref="D3:D36"/>
+  </sortState>
   <dataValidations xWindow="821" yWindow="357" count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Estado" prompt="Por favor, introduzca un valor para el estado (PENDIENTE, EN PROGRESO O REALIZADO )" sqref="F1:F38" xr:uid="{01248019-FD26-4D39-BA8E-80B22E1EE596}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Estado" prompt="Por favor, introduzca un valor para el estado (PENDIENTE, EN PROGRESO O REALIZADO )" sqref="F1:F36" xr:uid="{01248019-FD26-4D39-BA8E-80B22E1EE596}">
       <formula1>$N$2:$N$4</formula1>
     </dataValidation>
   </dataValidations>
@@ -5290,10 +4481,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{25ACDF49-AC43-4CCD-856F-6ED289E70C3E}">
-  <dimension ref="A2:G35"/>
+  <dimension ref="A2:I35"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="D36" sqref="D36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -5304,48 +4495,48 @@
     <col min="6" max="6" width="11.26953125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
       <c r="B2" s="14" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="C2" s="14"/>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
       <c r="B3" s="11" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="C3" s="11">
         <v>28</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
       <c r="B4" s="11" t="s">
+        <v>43</v>
+      </c>
+      <c r="C4" s="15">
+        <f>SUM('SPRINT-BACKLOG'!B2:B36)</f>
+        <v>37</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" ht="26" x14ac:dyDescent="0.35">
+      <c r="A7" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="C4" s="11">
-        <f>SUM('SPRINT-BACKLOG'!B2:B38)</f>
-        <v>31</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" ht="26" x14ac:dyDescent="0.35">
-      <c r="A7" s="7" t="s">
-        <v>53</v>
-      </c>
       <c r="B7" s="7" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="C7" s="7" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="D7" s="7" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="E7" s="7" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="G7" s="6"/>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A8" s="8">
         <v>44228</v>
       </c>
@@ -5354,19 +4545,19 @@
       </c>
       <c r="C8" s="9">
         <f>C4</f>
-        <v>31</v>
+        <v>37</v>
       </c>
       <c r="D8" s="10">
-        <f>SUMIF('SPRINT-BACKLOG'!D2:D38,"="&amp;VALUE(A8),'SPRINT-BACKLOG'!B2:B38)</f>
+        <f>SUMIF('SPRINT-BACKLOG'!D2:D36,"="&amp;VALUE(A8),'SPRINT-BACKLOG'!B2:B36)</f>
         <v>2</v>
       </c>
       <c r="E8" s="9">
         <f>C4 - D8</f>
-        <v>29</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A9" s="5">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A9" s="16">
         <v>44229</v>
       </c>
       <c r="B9" s="12">
@@ -5374,17 +4565,18 @@
       </c>
       <c r="C9" s="9">
         <f t="shared" ref="C9:C35" si="0">C8-$C$4/($C$3-1)</f>
-        <v>29.851851851851851</v>
+        <v>35.629629629629626</v>
       </c>
       <c r="D9" s="10">
+        <f>SUMIF('SPRINT-BACKLOG'!D2:D36,"="&amp;VALUE(A9),'SPRINT-BACKLOG'!B2:B36)</f>
         <v>2</v>
       </c>
       <c r="E9" s="9">
         <f>E8 - D9</f>
-        <v>27</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A10" s="8">
         <v>44230</v>
       </c>
@@ -5393,17 +4585,18 @@
       </c>
       <c r="C10" s="9">
         <f t="shared" si="0"/>
-        <v>28.703703703703702</v>
+        <v>34.259259259259252</v>
       </c>
       <c r="D10" s="10">
-        <v>0</v>
+        <f>SUMIF('SPRINT-BACKLOG'!D2:D36,"="&amp;VALUE(A10),'SPRINT-BACKLOG'!B2:B36)</f>
+        <v>2</v>
       </c>
       <c r="E10" s="9">
         <f>E9 - D10</f>
-        <v>27</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A11" s="8">
         <v>44231</v>
       </c>
@@ -5412,17 +4605,18 @@
       </c>
       <c r="C11" s="9">
         <f t="shared" si="0"/>
-        <v>27.555555555555554</v>
+        <v>32.888888888888879</v>
       </c>
       <c r="D11" s="10">
-        <v>5</v>
+        <f>SUMIF('SPRINT-BACKLOG'!D2:D36,"="&amp;VALUE(A11),'SPRINT-BACKLOG'!B2:B36)</f>
+        <v>1.5</v>
       </c>
       <c r="E11" s="9">
         <f t="shared" ref="E11:E35" si="1">E10 - D11</f>
-        <v>22</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.35">
+        <v>29.5</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A12" s="8">
         <v>44232</v>
       </c>
@@ -5431,17 +4625,18 @@
       </c>
       <c r="C12" s="9">
         <f t="shared" si="0"/>
-        <v>26.407407407407405</v>
+        <v>31.518518518518508</v>
       </c>
       <c r="D12" s="10">
-        <v>0</v>
+        <f>SUMIF('SPRINT-BACKLOG'!D2:D36,"="&amp;VALUE(A12),'SPRINT-BACKLOG'!B2:B36)</f>
+        <v>3</v>
       </c>
       <c r="E12" s="9">
         <f t="shared" si="1"/>
-        <v>22</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
+        <v>26.5</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A13" s="8">
         <v>44233</v>
       </c>
@@ -5450,17 +4645,18 @@
       </c>
       <c r="C13" s="9">
         <f t="shared" si="0"/>
-        <v>25.259259259259256</v>
+        <v>30.148148148148138</v>
       </c>
       <c r="D13" s="10">
-        <v>1</v>
+        <f>SUMIF('SPRINT-BACKLOG'!D2:D36,"="&amp;VALUE(A13),'SPRINT-BACKLOG'!B2:B36)</f>
+        <v>0</v>
       </c>
       <c r="E13" s="9">
         <f t="shared" si="1"/>
-        <v>21</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.35">
+        <v>26.5</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A14" s="8">
         <v>44234</v>
       </c>
@@ -5469,17 +4665,18 @@
       </c>
       <c r="C14" s="9">
         <f t="shared" si="0"/>
-        <v>24.111111111111107</v>
+        <v>28.777777777777768</v>
       </c>
       <c r="D14" s="10">
+        <f>SUMIF('SPRINT-BACKLOG'!D2:D36,"="&amp;VALUE(A14),'SPRINT-BACKLOG'!B2:B36)</f>
         <v>0</v>
       </c>
       <c r="E14" s="9">
         <f t="shared" si="1"/>
-        <v>21</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.35">
+        <v>26.5</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A15" s="8">
         <v>44235</v>
       </c>
@@ -5488,17 +4685,18 @@
       </c>
       <c r="C15" s="9">
         <f t="shared" si="0"/>
-        <v>22.962962962962958</v>
+        <v>27.407407407407398</v>
       </c>
       <c r="D15" s="10">
-        <v>3</v>
+        <f>SUMIF('SPRINT-BACKLOG'!D2:D36,"="&amp;VALUE(A15),'SPRINT-BACKLOG'!B2:B36)</f>
+        <v>2</v>
       </c>
       <c r="E15" s="9">
         <f t="shared" si="1"/>
-        <v>18</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.35">
+        <v>24.5</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A16" s="8">
         <v>44236</v>
       </c>
@@ -5507,15 +4705,20 @@
       </c>
       <c r="C16" s="9">
         <f t="shared" si="0"/>
-        <v>21.81481481481481</v>
+        <v>26.037037037037027</v>
       </c>
       <c r="D16" s="10">
+        <f>SUMIF('SPRINT-BACKLOG'!D2:D36,"="&amp;VALUE(A16),'SPRINT-BACKLOG'!B2:B36)</f>
         <v>2</v>
       </c>
       <c r="E16" s="9">
         <f t="shared" si="1"/>
-        <v>16</v>
-      </c>
+        <v>22.5</v>
+      </c>
+      <c r="F16" s="17"/>
+      <c r="G16" s="17"/>
+      <c r="H16" s="17"/>
+      <c r="I16" s="17"/>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A17" s="8">
@@ -5526,15 +4729,15 @@
       </c>
       <c r="C17" s="9">
         <f t="shared" si="0"/>
-        <v>20.666666666666661</v>
+        <v>24.666666666666657</v>
       </c>
       <c r="D17" s="10">
-        <f>SUMIF('SPRINT-BACKLOG'!D2:D38,"="&amp;VALUE(A17),'SPRINT-BACKLOG'!B2:B38)</f>
-        <v>0</v>
+        <f>SUMIF('SPRINT-BACKLOG'!D2:D36,"="&amp;VALUE(A17),'SPRINT-BACKLOG'!B2:B36)</f>
+        <v>1</v>
       </c>
       <c r="E17" s="9">
         <f t="shared" si="1"/>
-        <v>16</v>
+        <v>21.5</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.35">
@@ -5546,15 +4749,15 @@
       </c>
       <c r="C18" s="9">
         <f t="shared" si="0"/>
-        <v>19.518518518518512</v>
+        <v>23.296296296296287</v>
       </c>
       <c r="D18" s="10">
-        <f>SUMIF('SPRINT-BACKLOG'!D2:D38,"="&amp;VALUE(A18),'SPRINT-BACKLOG'!B2:B38)</f>
-        <v>0</v>
+        <f>SUMIF('SPRINT-BACKLOG'!D2:D36,"="&amp;VALUE(A18),'SPRINT-BACKLOG'!B2:B36)</f>
+        <v>3.5</v>
       </c>
       <c r="E18" s="9">
         <f t="shared" si="1"/>
-        <v>16</v>
+        <v>18</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.35">
@@ -5566,15 +4769,15 @@
       </c>
       <c r="C19" s="9">
         <f t="shared" si="0"/>
-        <v>18.370370370370363</v>
+        <v>21.925925925925917</v>
       </c>
       <c r="D19" s="10">
-        <f>SUMIF('SPRINT-BACKLOG'!D2:D38,"="&amp;VALUE(A19),'SPRINT-BACKLOG'!B2:B38)</f>
+        <f>SUMIF('SPRINT-BACKLOG'!D2:D36,"="&amp;VALUE(A19),'SPRINT-BACKLOG'!B2:B36)</f>
         <v>0</v>
       </c>
       <c r="E19" s="9">
         <f t="shared" si="1"/>
-        <v>16</v>
+        <v>18</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.35">
@@ -5586,15 +4789,15 @@
       </c>
       <c r="C20" s="9">
         <f t="shared" si="0"/>
-        <v>17.222222222222214</v>
+        <v>20.555555555555546</v>
       </c>
       <c r="D20" s="10">
-        <f>SUMIF('SPRINT-BACKLOG'!D2:D38,"="&amp;VALUE(A20),'SPRINT-BACKLOG'!B2:B38)</f>
+        <f>SUMIF('SPRINT-BACKLOG'!D2:D36,"="&amp;VALUE(A20),'SPRINT-BACKLOG'!B2:B36)</f>
         <v>0</v>
       </c>
       <c r="E20" s="9">
         <f t="shared" si="1"/>
-        <v>16</v>
+        <v>18</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.35">
@@ -5606,15 +4809,15 @@
       </c>
       <c r="C21" s="9">
         <f t="shared" si="0"/>
-        <v>16.074074074074066</v>
+        <v>19.185185185185176</v>
       </c>
       <c r="D21" s="10">
-        <f>SUMIF('SPRINT-BACKLOG'!D2:D38,"="&amp;VALUE(A21),'SPRINT-BACKLOG'!B2:B38)</f>
+        <f>SUMIF('SPRINT-BACKLOG'!D2:D36,"="&amp;VALUE(A21),'SPRINT-BACKLOG'!B2:B36)</f>
         <v>0</v>
       </c>
       <c r="E21" s="9">
         <f t="shared" si="1"/>
-        <v>16</v>
+        <v>18</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.35">
@@ -5626,11 +4829,11 @@
       </c>
       <c r="C22" s="9">
         <f t="shared" si="0"/>
-        <v>14.925925925925917</v>
+        <v>17.814814814814806</v>
       </c>
       <c r="D22" s="10">
-        <f>SUMIF('SPRINT-BACKLOG'!D2:D38,"="&amp;VALUE(A22),'SPRINT-BACKLOG'!B2:B38)</f>
-        <v>2</v>
+        <f>SUMIF('SPRINT-BACKLOG'!D2:D36,"="&amp;VALUE(A22),'SPRINT-BACKLOG'!B2:B36)</f>
+        <v>4</v>
       </c>
       <c r="E22" s="9">
         <f t="shared" si="1"/>
@@ -5646,15 +4849,15 @@
       </c>
       <c r="C23" s="9">
         <f t="shared" si="0"/>
-        <v>13.777777777777768</v>
+        <v>16.444444444444436</v>
       </c>
       <c r="D23" s="10">
-        <f>SUMIF('SPRINT-BACKLOG'!D2:D38,"="&amp;VALUE(A23),'SPRINT-BACKLOG'!B2:B38)</f>
-        <v>5</v>
+        <f>SUMIF('SPRINT-BACKLOG'!D2:D36,"="&amp;VALUE(A23),'SPRINT-BACKLOG'!B2:B36)</f>
+        <v>1.5</v>
       </c>
       <c r="E23" s="9">
         <f t="shared" si="1"/>
-        <v>9</v>
+        <v>12.5</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.35">
@@ -5666,15 +4869,15 @@
       </c>
       <c r="C24" s="9">
         <f t="shared" si="0"/>
-        <v>12.629629629629619</v>
+        <v>15.074074074074066</v>
       </c>
       <c r="D24" s="10">
-        <f>SUMIF('SPRINT-BACKLOG'!D2:D38,"="&amp;VALUE(A24),'SPRINT-BACKLOG'!B2:B38)</f>
-        <v>2</v>
+        <f>SUMIF('SPRINT-BACKLOG'!D2:D36,"="&amp;VALUE(A24),'SPRINT-BACKLOG'!B2:B36)</f>
+        <v>3</v>
       </c>
       <c r="E24" s="9">
         <f t="shared" si="1"/>
-        <v>7</v>
+        <v>9.5</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.35">
@@ -5686,15 +4889,15 @@
       </c>
       <c r="C25" s="9">
         <f t="shared" si="0"/>
-        <v>11.48148148148147</v>
+        <v>13.703703703703695</v>
       </c>
       <c r="D25" s="10">
-        <f>SUMIF('SPRINT-BACKLOG'!D2:D38,"="&amp;VALUE(A25),'SPRINT-BACKLOG'!B2:B38)</f>
-        <v>1</v>
+        <f>SUMIF('SPRINT-BACKLOG'!D2:D36,"="&amp;VALUE(A25),'SPRINT-BACKLOG'!B2:B36)</f>
+        <v>0</v>
       </c>
       <c r="E25" s="9">
         <f t="shared" si="1"/>
-        <v>6</v>
+        <v>9.5</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.35">
@@ -5706,15 +4909,15 @@
       </c>
       <c r="C26" s="9">
         <f t="shared" si="0"/>
-        <v>10.333333333333321</v>
+        <v>12.333333333333325</v>
       </c>
       <c r="D26" s="10">
-        <f>SUMIF('SPRINT-BACKLOG'!D2:D38,"="&amp;VALUE(A26),'SPRINT-BACKLOG'!B2:B38)</f>
+        <f>SUMIF('SPRINT-BACKLOG'!D2:D36,"="&amp;VALUE(A26),'SPRINT-BACKLOG'!B2:B36)</f>
         <v>0</v>
       </c>
       <c r="E26" s="9">
         <f>E25 - D26</f>
-        <v>6</v>
+        <v>9.5</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.35">
@@ -5726,15 +4929,15 @@
       </c>
       <c r="C27" s="9">
         <f t="shared" si="0"/>
-        <v>9.1851851851851727</v>
+        <v>10.962962962962955</v>
       </c>
       <c r="D27" s="10">
-        <f>SUMIF('SPRINT-BACKLOG'!D2:D38,"="&amp;VALUE(A27),'SPRINT-BACKLOG'!B2:B38)</f>
-        <v>1</v>
+        <f>SUMIF('SPRINT-BACKLOG'!D2:D36,"="&amp;VALUE(A27),'SPRINT-BACKLOG'!B2:B36)</f>
+        <v>0</v>
       </c>
       <c r="E27" s="9">
         <f t="shared" si="1"/>
-        <v>5</v>
+        <v>9.5</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.35">
@@ -5746,15 +4949,15 @@
       </c>
       <c r="C28" s="9">
         <f t="shared" si="0"/>
-        <v>8.0370370370370239</v>
+        <v>9.5925925925925846</v>
       </c>
       <c r="D28" s="10">
-        <f>SUMIF('SPRINT-BACKLOG'!D2:D38,"="&amp;VALUE(A28),'SPRINT-BACKLOG'!B2:B38)</f>
+        <f>SUMIF('SPRINT-BACKLOG'!D2:D36,"="&amp;VALUE(A28),'SPRINT-BACKLOG'!B2:B36)</f>
         <v>0</v>
       </c>
       <c r="E28" s="9">
         <f t="shared" si="1"/>
-        <v>5</v>
+        <v>9.5</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.35">
@@ -5766,14 +4969,15 @@
       </c>
       <c r="C29" s="9">
         <f t="shared" si="0"/>
-        <v>6.888888888888876</v>
+        <v>8.2222222222222143</v>
       </c>
       <c r="D29" s="10">
-        <v>5</v>
+        <f>SUMIF('SPRINT-BACKLOG'!D2:D36,"="&amp;VALUE(A29),'SPRINT-BACKLOG'!B2:B36)</f>
+        <v>4.5</v>
       </c>
       <c r="E29" s="9">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>5</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.35">
@@ -5785,15 +4989,15 @@
       </c>
       <c r="C30" s="9">
         <f t="shared" si="0"/>
-        <v>5.740740740740728</v>
+        <v>6.8518518518518441</v>
       </c>
       <c r="D30" s="10">
-        <f>SUMIF('SPRINT-BACKLOG'!D2:D38,"="&amp;VALUE(A30),'SPRINT-BACKLOG'!B2:B38)</f>
-        <v>0</v>
+        <f>SUMIF('SPRINT-BACKLOG'!D2:D36,"="&amp;VALUE(A30),'SPRINT-BACKLOG'!B2:B36)</f>
+        <v>2</v>
       </c>
       <c r="E30" s="9">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.35">
@@ -5805,15 +5009,15 @@
       </c>
       <c r="C31" s="9">
         <f t="shared" si="0"/>
-        <v>4.5925925925925801</v>
+        <v>5.4814814814814738</v>
       </c>
       <c r="D31" s="10">
-        <f>SUMIF('SPRINT-BACKLOG'!D2:D38,"="&amp;VALUE(A31),'SPRINT-BACKLOG'!B2:B38)</f>
-        <v>0</v>
+        <f>SUMIF('SPRINT-BACKLOG'!D2:D36,"="&amp;VALUE(A31),'SPRINT-BACKLOG'!B2:B36)</f>
+        <v>1</v>
       </c>
       <c r="E31" s="9">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.35">
@@ -5825,15 +5029,15 @@
       </c>
       <c r="C32" s="9">
         <f t="shared" si="0"/>
-        <v>3.4444444444444322</v>
+        <v>4.1111111111111036</v>
       </c>
       <c r="D32" s="10">
-        <f>SUMIF('SPRINT-BACKLOG'!D2:D38,"="&amp;VALUE(A32),'SPRINT-BACKLOG'!B2:B38)</f>
+        <f>SUMIF('SPRINT-BACKLOG'!D2:D36,"="&amp;VALUE(A32),'SPRINT-BACKLOG'!B2:B36)</f>
         <v>0</v>
       </c>
       <c r="E32" s="9">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.35">
@@ -5845,11 +5049,11 @@
       </c>
       <c r="C33" s="9">
         <f t="shared" si="0"/>
-        <v>2.2962962962962843</v>
+        <v>2.7407407407407334</v>
       </c>
       <c r="D33" s="10">
-        <f>SUMIF('SPRINT-BACKLOG'!D2:D38,"="&amp;VALUE(A33),'SPRINT-BACKLOG'!B2:B38)</f>
-        <v>0</v>
+        <f>SUMIF('SPRINT-BACKLOG'!D2:D36,"="&amp;VALUE(A33),'SPRINT-BACKLOG'!B2:B36)</f>
+        <v>2</v>
       </c>
       <c r="E33" s="9">
         <f t="shared" si="1"/>
@@ -5865,10 +5069,10 @@
       </c>
       <c r="C34" s="9">
         <f t="shared" si="0"/>
-        <v>1.1481481481481361</v>
+        <v>1.3703703703703629</v>
       </c>
       <c r="D34" s="10">
-        <f>SUMIF('SPRINT-BACKLOG'!D2:D38,"="&amp;VALUE(A34),'SPRINT-BACKLOG'!B2:B38)</f>
+        <f>SUMIF('SPRINT-BACKLOG'!D2:D36,"="&amp;VALUE(A34),'SPRINT-BACKLOG'!B2:B36)</f>
         <v>0</v>
       </c>
       <c r="E34" s="9">
@@ -5885,10 +5089,10 @@
       </c>
       <c r="C35" s="9">
         <f t="shared" si="0"/>
-        <v>-1.1990408665951691E-14</v>
+        <v>-7.5495165674510645E-15</v>
       </c>
       <c r="D35" s="10">
-        <f>SUMIF('SPRINT-BACKLOG'!D2:D38,"="&amp;VALUE(A35),'SPRINT-BACKLOG'!B2:B38)</f>
+        <f>SUMIF('SPRINT-BACKLOG'!D2:D36,"="&amp;VALUE(A35),'SPRINT-BACKLOG'!B2:B36)</f>
         <v>0</v>
       </c>
       <c r="E35" s="9">

</xml_diff>

<commit_message>
[IMPL] Documentación final del SP2 Se ha añadido la documentación necesaria para dar por finalizado el sprint 2. [FALTA] Falta añadir la documentación a la memoria debido a que falta el visto bueno por parte de la tutora del tfg.
</commit_message>
<xml_diff>
--- a/documentación/Product Backlog/SP2.xlsx
+++ b/documentación/Product Backlog/SP2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alesk\Desktop\Universidad\TFG_app\TFG_app\documentación\Product Backlog\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8121735E-ABCB-4A00-9C07-2F831DC3FA02}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DFD69940-326C-40F3-A10F-47E34A114EF5}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" activeTab="1" xr2:uid="{41FE112A-4516-4423-9CD7-320A9C032A6D}"/>
+    <workbookView xWindow="29100" yWindow="1140" windowWidth="20175" windowHeight="9705" xr2:uid="{41FE112A-4516-4423-9CD7-320A9C032A6D}"/>
   </bookViews>
   <sheets>
     <sheet name="SPRINT-BACKLOG" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="52">
   <si>
     <t>Puntos de historia</t>
   </si>
@@ -190,6 +190,9 @@
   <si>
     <t>Implementación de la funcionalidad de listar los Servicios (EMP)</t>
   </si>
+  <si>
+    <t xml:space="preserve"> ESTADO DE LA TAREA</t>
+  </si>
 </sst>
 </file>
 
@@ -273,7 +276,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -305,11 +308,48 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -350,9 +390,6 @@
     <xf numFmtId="2" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="2" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -360,6 +397,24 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -369,6 +424,9 @@
   <colors>
     <mruColors>
       <color rgb="FF74B9FF"/>
+      <color rgb="FFFCBF49"/>
+      <color rgb="FFF77F00"/>
+      <color rgb="FF003049"/>
       <color rgb="FF0984E3"/>
       <color rgb="FFFDCB6E"/>
     </mruColors>
@@ -1598,14 +1656,14 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>36</xdr:row>
-      <xdr:rowOff>160336</xdr:rowOff>
+      <xdr:row>37</xdr:row>
+      <xdr:rowOff>163511</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>6</xdr:col>
+      <xdr:col>5</xdr:col>
       <xdr:colOff>752475</xdr:colOff>
-      <xdr:row>61</xdr:row>
-      <xdr:rowOff>9524</xdr:rowOff>
+      <xdr:row>59</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1930,22 +1988,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2BB024A1-16E4-467A-A83B-A5E93171F59F}">
-  <dimension ref="A1:N233"/>
+  <dimension ref="A1:G234"/>
   <sheetViews>
-    <sheetView topLeftCell="A40" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView tabSelected="1" topLeftCell="A37" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G60" sqref="G60"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" outlineLevelRow="1" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="53.6328125" customWidth="1"/>
+    <col min="1" max="1" width="25.90625" customWidth="1"/>
     <col min="2" max="2" width="11" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="13.1796875" customWidth="1"/>
     <col min="4" max="4" width="13.36328125" customWidth="1"/>
     <col min="5" max="5" width="12.81640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="31" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:7" ht="31" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>8</v>
       </c>
@@ -1965,57 +2023,41 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:14" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A2" s="3" t="s">
+    <row r="2" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A2" s="18" t="s">
+        <v>46</v>
+      </c>
+      <c r="B2" s="19"/>
+      <c r="C2" s="19"/>
+      <c r="D2" s="19"/>
+      <c r="E2" s="19"/>
+      <c r="F2" s="20"/>
+      <c r="G2" s="1"/>
+    </row>
+    <row r="3" spans="1:7" ht="31" outlineLevel="1" x14ac:dyDescent="0.35">
+      <c r="A3" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="B2" s="13">
+      <c r="B3" s="13">
         <v>2</v>
       </c>
-      <c r="C2" s="5">
+      <c r="C3" s="5">
         <v>44197</v>
       </c>
-      <c r="D2" s="5">
+      <c r="D3" s="5">
         <v>44228</v>
       </c>
-      <c r="E2" s="5">
+      <c r="E3" s="5">
         <v>44197</v>
-      </c>
-      <c r="F2" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="G2" s="1"/>
-      <c r="N2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="3" spans="1:14" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A3" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="B3" s="13">
-        <v>0.5</v>
-      </c>
-      <c r="C3" s="5">
-        <v>44229</v>
-      </c>
-      <c r="D3" s="5">
-        <v>44229</v>
-      </c>
-      <c r="E3" s="5">
-        <v>44229</v>
       </c>
       <c r="F3" s="4" t="s">
         <v>7</v>
       </c>
       <c r="G3" s="1"/>
-      <c r="N3" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="4" spans="1:14" ht="15.5" x14ac:dyDescent="0.35">
+    </row>
+    <row r="4" spans="1:7" ht="31" outlineLevel="1" x14ac:dyDescent="0.35">
       <c r="A4" s="3" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B4" s="13">
         <v>0.5</v>
@@ -2033,13 +2075,10 @@
         <v>7</v>
       </c>
       <c r="G4" s="1"/>
-      <c r="N4" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="5" spans="1:14" ht="15.5" x14ac:dyDescent="0.35">
+    </row>
+    <row r="5" spans="1:7" ht="31" outlineLevel="1" x14ac:dyDescent="0.35">
       <c r="A5" s="3" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="B5" s="13">
         <v>0.5</v>
@@ -2058,9 +2097,9 @@
       </c>
       <c r="G5" s="1"/>
     </row>
-    <row r="6" spans="1:14" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:7" ht="31" outlineLevel="1" x14ac:dyDescent="0.35">
       <c r="A6" s="3" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B6" s="13">
         <v>0.5</v>
@@ -2079,30 +2118,30 @@
       </c>
       <c r="G6" s="1"/>
     </row>
-    <row r="7" spans="1:14" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:7" ht="31" outlineLevel="1" x14ac:dyDescent="0.35">
       <c r="A7" s="3" t="s">
-        <v>37</v>
+        <v>11</v>
       </c>
       <c r="B7" s="13">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="C7" s="5">
-        <v>44230</v>
+        <v>44229</v>
       </c>
       <c r="D7" s="5">
-        <v>44230</v>
+        <v>44229</v>
       </c>
       <c r="E7" s="5">
-        <v>44230</v>
+        <v>44229</v>
       </c>
       <c r="F7" s="4" t="s">
         <v>7</v>
       </c>
       <c r="G7" s="1"/>
     </row>
-    <row r="8" spans="1:14" ht="31" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:7" ht="46.5" outlineLevel="1" x14ac:dyDescent="0.35">
       <c r="A8" s="3" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B8" s="13">
         <v>1</v>
@@ -2121,72 +2160,72 @@
       </c>
       <c r="G8" s="1"/>
     </row>
-    <row r="9" spans="1:14" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:7" ht="46.5" outlineLevel="1" x14ac:dyDescent="0.35">
       <c r="A9" s="3" t="s">
-        <v>13</v>
+        <v>36</v>
       </c>
       <c r="B9" s="13">
-        <v>1.5</v>
+        <v>1</v>
       </c>
       <c r="C9" s="5">
-        <v>44231</v>
+        <v>44230</v>
       </c>
       <c r="D9" s="5">
-        <v>44231</v>
+        <v>44230</v>
       </c>
       <c r="E9" s="5">
-        <v>44231</v>
+        <v>44230</v>
       </c>
       <c r="F9" s="4" t="s">
         <v>7</v>
       </c>
       <c r="G9" s="1"/>
     </row>
-    <row r="10" spans="1:14" ht="31" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:7" ht="31" outlineLevel="1" x14ac:dyDescent="0.35">
       <c r="A10" s="3" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="B10" s="13">
-        <v>1</v>
+        <v>1.5</v>
       </c>
       <c r="C10" s="5">
         <v>44231</v>
       </c>
       <c r="D10" s="5">
-        <v>44232</v>
+        <v>44231</v>
       </c>
       <c r="E10" s="5">
-        <v>44232</v>
+        <v>44231</v>
       </c>
       <c r="F10" s="4" t="s">
         <v>7</v>
       </c>
       <c r="G10" s="1"/>
     </row>
-    <row r="11" spans="1:14" ht="31" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:7" ht="46.5" outlineLevel="1" x14ac:dyDescent="0.35">
       <c r="A11" s="3" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B11" s="13">
         <v>1</v>
       </c>
       <c r="C11" s="5">
-        <v>44232</v>
+        <v>44231</v>
       </c>
       <c r="D11" s="5">
         <v>44232</v>
       </c>
       <c r="E11" s="5">
-        <v>44235</v>
+        <v>44232</v>
       </c>
       <c r="F11" s="4" t="s">
         <v>7</v>
       </c>
       <c r="G11" s="1"/>
     </row>
-    <row r="12" spans="1:14" ht="31" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:7" ht="62" outlineLevel="1" x14ac:dyDescent="0.35">
       <c r="A12" s="3" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B12" s="13">
         <v>1</v>
@@ -2205,30 +2244,30 @@
       </c>
       <c r="G12" s="1"/>
     </row>
-    <row r="13" spans="1:14" ht="31" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:7" ht="62" outlineLevel="1" x14ac:dyDescent="0.35">
       <c r="A13" s="3" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="B13" s="13">
         <v>1</v>
       </c>
       <c r="C13" s="5">
+        <v>44232</v>
+      </c>
+      <c r="D13" s="5">
+        <v>44232</v>
+      </c>
+      <c r="E13" s="5">
         <v>44235</v>
-      </c>
-      <c r="D13" s="5">
-        <v>44235</v>
-      </c>
-      <c r="E13" s="5">
-        <v>44236</v>
       </c>
       <c r="F13" s="4" t="s">
         <v>7</v>
       </c>
       <c r="G13" s="1"/>
     </row>
-    <row r="14" spans="1:14" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:7" ht="46.5" outlineLevel="1" x14ac:dyDescent="0.35">
       <c r="A14" s="3" t="s">
-        <v>38</v>
+        <v>14</v>
       </c>
       <c r="B14" s="13">
         <v>1</v>
@@ -2247,30 +2286,30 @@
       </c>
       <c r="G14" s="1"/>
     </row>
-    <row r="15" spans="1:14" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:7" ht="31" outlineLevel="1" x14ac:dyDescent="0.35">
       <c r="A15" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B15" s="13">
         <v>1</v>
       </c>
       <c r="C15" s="5">
+        <v>44235</v>
+      </c>
+      <c r="D15" s="5">
+        <v>44235</v>
+      </c>
+      <c r="E15" s="5">
         <v>44236</v>
-      </c>
-      <c r="D15" s="5">
-        <v>44236</v>
-      </c>
-      <c r="E15" s="5">
-        <v>44237</v>
       </c>
       <c r="F15" s="4" t="s">
         <v>7</v>
       </c>
       <c r="G15" s="1"/>
     </row>
-    <row r="16" spans="1:14" ht="31" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:7" ht="31" outlineLevel="1" x14ac:dyDescent="0.35">
       <c r="A16" s="3" t="s">
-        <v>27</v>
+        <v>39</v>
       </c>
       <c r="B16" s="13">
         <v>1</v>
@@ -2289,39 +2328,39 @@
       </c>
       <c r="G16" s="1"/>
     </row>
-    <row r="17" spans="1:7" ht="31" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:7" ht="46.5" outlineLevel="1" x14ac:dyDescent="0.35">
       <c r="A17" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B17" s="13">
         <v>1</v>
       </c>
       <c r="C17" s="5">
+        <v>44236</v>
+      </c>
+      <c r="D17" s="5">
+        <v>44236</v>
+      </c>
+      <c r="E17" s="5">
         <v>44237</v>
-      </c>
-      <c r="D17" s="5">
-        <v>44237</v>
-      </c>
-      <c r="E17" s="5">
-        <v>44238</v>
       </c>
       <c r="F17" s="4" t="s">
         <v>7</v>
       </c>
       <c r="G17" s="1"/>
     </row>
-    <row r="18" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:7" ht="62" outlineLevel="1" x14ac:dyDescent="0.35">
       <c r="A18" s="3" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="B18" s="13">
-        <v>1.5</v>
+        <v>1</v>
       </c>
       <c r="C18" s="5">
         <v>44237</v>
       </c>
       <c r="D18" s="5">
-        <v>44238</v>
+        <v>44237</v>
       </c>
       <c r="E18" s="5">
         <v>44238</v>
@@ -2331,30 +2370,30 @@
       </c>
       <c r="G18" s="1"/>
     </row>
-    <row r="19" spans="1:7" ht="31" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:7" ht="31" outlineLevel="1" x14ac:dyDescent="0.35">
       <c r="A19" s="3" t="s">
-        <v>19</v>
+        <v>25</v>
       </c>
       <c r="B19" s="13">
-        <v>1</v>
+        <v>1.5</v>
       </c>
       <c r="C19" s="5">
-        <v>44238</v>
+        <v>44237</v>
       </c>
       <c r="D19" s="5">
         <v>44238</v>
       </c>
       <c r="E19" s="5">
-        <v>44239</v>
+        <v>44238</v>
       </c>
       <c r="F19" s="4" t="s">
         <v>7</v>
       </c>
       <c r="G19" s="1"/>
     </row>
-    <row r="20" spans="1:7" ht="31" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:7" ht="62" outlineLevel="1" x14ac:dyDescent="0.35">
       <c r="A20" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B20" s="13">
         <v>1</v>
@@ -2373,30 +2412,30 @@
       </c>
       <c r="G20" s="1"/>
     </row>
-    <row r="21" spans="1:7" ht="31" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:7" ht="62" outlineLevel="1" x14ac:dyDescent="0.35">
       <c r="A21" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B21" s="13">
         <v>1</v>
       </c>
       <c r="C21" s="5">
+        <v>44238</v>
+      </c>
+      <c r="D21" s="5">
+        <v>44238</v>
+      </c>
+      <c r="E21" s="5">
         <v>44239</v>
-      </c>
-      <c r="D21" s="5">
-        <v>44242</v>
-      </c>
-      <c r="E21" s="5">
-        <v>44240</v>
       </c>
       <c r="F21" s="4" t="s">
         <v>7</v>
       </c>
       <c r="G21" s="1"/>
     </row>
-    <row r="22" spans="1:7" ht="31" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:7" ht="62" outlineLevel="1" x14ac:dyDescent="0.35">
       <c r="A22" s="3" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="B22" s="13">
         <v>1</v>
@@ -2415,30 +2454,30 @@
       </c>
       <c r="G22" s="1"/>
     </row>
-    <row r="23" spans="1:7" ht="31" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:7" ht="62" outlineLevel="1" x14ac:dyDescent="0.35">
       <c r="A23" s="3" t="s">
-        <v>50</v>
+        <v>18</v>
       </c>
       <c r="B23" s="13">
         <v>1</v>
       </c>
       <c r="C23" s="5">
-        <v>44240</v>
+        <v>44239</v>
       </c>
       <c r="D23" s="5">
         <v>44242</v>
       </c>
       <c r="E23" s="5">
-        <v>44242</v>
+        <v>44240</v>
       </c>
       <c r="F23" s="4" t="s">
         <v>7</v>
       </c>
       <c r="G23" s="1"/>
     </row>
-    <row r="24" spans="1:7" ht="31" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:7" ht="46.5" outlineLevel="1" x14ac:dyDescent="0.35">
       <c r="A24" s="3" t="s">
-        <v>29</v>
+        <v>50</v>
       </c>
       <c r="B24" s="13">
         <v>1</v>
@@ -2457,72 +2496,72 @@
       </c>
       <c r="G24" s="1"/>
     </row>
-    <row r="25" spans="1:7" ht="31" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:7" ht="62" outlineLevel="1" x14ac:dyDescent="0.35">
       <c r="A25" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="B25" s="13">
+        <v>1</v>
+      </c>
+      <c r="C25" s="5">
+        <v>44240</v>
+      </c>
+      <c r="D25" s="5">
+        <v>44242</v>
+      </c>
+      <c r="E25" s="5">
+        <v>44242</v>
+      </c>
+      <c r="F25" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="G25" s="1"/>
+    </row>
+    <row r="26" spans="1:7" ht="31" outlineLevel="1" x14ac:dyDescent="0.35">
+      <c r="A26" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="B25" s="13">
+      <c r="B26" s="13">
         <v>1.5</v>
-      </c>
-      <c r="C25" s="5">
-        <v>44243</v>
-      </c>
-      <c r="D25" s="5">
-        <v>44243</v>
-      </c>
-      <c r="E25" s="5">
-        <v>44244</v>
-      </c>
-      <c r="F25" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="G25" s="1"/>
-    </row>
-    <row r="26" spans="1:7" ht="31" x14ac:dyDescent="0.35">
-      <c r="A26" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="B26" s="13">
-        <v>1</v>
       </c>
       <c r="C26" s="5">
         <v>44243</v>
       </c>
       <c r="D26" s="5">
-        <v>44244</v>
+        <v>44243</v>
       </c>
       <c r="E26" s="5">
         <v>44244</v>
       </c>
       <c r="F26" s="4" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="G26" s="1"/>
     </row>
-    <row r="27" spans="1:7" ht="31" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:7" ht="46.5" outlineLevel="1" x14ac:dyDescent="0.35">
       <c r="A27" s="3" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B27" s="13">
         <v>1</v>
       </c>
       <c r="C27" s="5">
-        <v>44244</v>
+        <v>44243</v>
       </c>
       <c r="D27" s="5">
         <v>44244</v>
       </c>
       <c r="E27" s="5">
-        <v>44245</v>
+        <v>44244</v>
       </c>
       <c r="F27" s="4" t="s">
         <v>7</v>
       </c>
       <c r="G27" s="1"/>
     </row>
-    <row r="28" spans="1:7" ht="31" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:7" ht="62" outlineLevel="1" x14ac:dyDescent="0.35">
       <c r="A28" s="3" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B28" s="13">
         <v>1</v>
@@ -2541,33 +2580,33 @@
       </c>
       <c r="G28" s="1"/>
     </row>
-    <row r="29" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:7" ht="62" outlineLevel="1" x14ac:dyDescent="0.35">
       <c r="A29" s="3" t="s">
-        <v>26</v>
+        <v>33</v>
       </c>
       <c r="B29" s="13">
-        <v>1.5</v>
+        <v>1</v>
       </c>
       <c r="C29" s="5">
+        <v>44244</v>
+      </c>
+      <c r="D29" s="5">
+        <v>44244</v>
+      </c>
+      <c r="E29" s="5">
         <v>44245</v>
-      </c>
-      <c r="D29" s="5">
-        <v>44249</v>
-      </c>
-      <c r="E29" s="5">
-        <v>44246</v>
       </c>
       <c r="F29" s="4" t="s">
         <v>7</v>
       </c>
       <c r="G29" s="1"/>
     </row>
-    <row r="30" spans="1:7" ht="31" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:7" ht="31" outlineLevel="1" x14ac:dyDescent="0.35">
       <c r="A30" s="3" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="B30" s="13">
-        <v>1</v>
+        <v>1.5</v>
       </c>
       <c r="C30" s="5">
         <v>44245</v>
@@ -2583,30 +2622,30 @@
       </c>
       <c r="G30" s="1"/>
     </row>
-    <row r="31" spans="1:7" ht="31" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:7" ht="62" outlineLevel="1" x14ac:dyDescent="0.35">
       <c r="A31" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B31" s="13">
         <v>1</v>
       </c>
       <c r="C31" s="5">
-        <v>44246</v>
+        <v>44245</v>
       </c>
       <c r="D31" s="5">
         <v>44249</v>
       </c>
       <c r="E31" s="5">
-        <v>44249</v>
+        <v>44246</v>
       </c>
       <c r="F31" s="4" t="s">
         <v>7</v>
       </c>
       <c r="G31" s="1"/>
     </row>
-    <row r="32" spans="1:7" ht="31" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:7" ht="62" outlineLevel="1" x14ac:dyDescent="0.35">
       <c r="A32" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B32" s="13">
         <v>1</v>
@@ -2625,30 +2664,30 @@
       </c>
       <c r="G32" s="1"/>
     </row>
-    <row r="33" spans="1:7" ht="31" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:7" ht="62" outlineLevel="1" x14ac:dyDescent="0.35">
       <c r="A33" s="3" t="s">
-        <v>32</v>
+        <v>24</v>
       </c>
       <c r="B33" s="13">
         <v>1</v>
       </c>
       <c r="C33" s="5">
+        <v>44246</v>
+      </c>
+      <c r="D33" s="5">
         <v>44249</v>
       </c>
-      <c r="D33" s="5">
-        <v>44250</v>
-      </c>
       <c r="E33" s="5">
-        <v>44250</v>
+        <v>44249</v>
       </c>
       <c r="F33" s="4" t="s">
         <v>7</v>
       </c>
       <c r="G33" s="1"/>
     </row>
-    <row r="34" spans="1:7" ht="31" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:7" ht="46.5" outlineLevel="1" x14ac:dyDescent="0.35">
       <c r="A34" s="3" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B34" s="13">
         <v>1</v>
@@ -2667,55 +2706,67 @@
       </c>
       <c r="G34" s="1"/>
     </row>
-    <row r="35" spans="1:7" ht="31" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:7" ht="62" outlineLevel="1" x14ac:dyDescent="0.35">
       <c r="A35" s="3" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B35" s="13">
         <v>1</v>
       </c>
       <c r="C35" s="5">
+        <v>44249</v>
+      </c>
+      <c r="D35" s="5">
         <v>44250</v>
       </c>
-      <c r="D35" s="5">
-        <v>44251</v>
-      </c>
       <c r="E35" s="5">
-        <v>44251</v>
+        <v>44250</v>
       </c>
       <c r="F35" s="4" t="s">
         <v>7</v>
       </c>
       <c r="G35" s="1"/>
     </row>
-    <row r="36" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:7" ht="62" outlineLevel="1" x14ac:dyDescent="0.35">
       <c r="A36" s="3" t="s">
-        <v>41</v>
+        <v>30</v>
       </c>
       <c r="B36" s="13">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C36" s="5">
-        <v>44220</v>
+        <v>44250</v>
       </c>
       <c r="D36" s="5">
-        <v>44253</v>
+        <v>44251</v>
       </c>
       <c r="E36" s="5">
-        <v>44221</v>
+        <v>44251</v>
       </c>
       <c r="F36" s="4" t="s">
         <v>7</v>
       </c>
       <c r="G36" s="1"/>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A37" s="1"/>
-      <c r="B37" s="1"/>
-      <c r="C37" s="1"/>
-      <c r="D37" s="1"/>
-      <c r="E37" s="1"/>
-      <c r="F37" s="1"/>
+    <row r="37" spans="1:7" ht="31" outlineLevel="1" x14ac:dyDescent="0.35">
+      <c r="A37" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="B37" s="13">
+        <v>2</v>
+      </c>
+      <c r="C37" s="5">
+        <v>44220</v>
+      </c>
+      <c r="D37" s="5">
+        <v>44253</v>
+      </c>
+      <c r="E37" s="5">
+        <v>44221</v>
+      </c>
+      <c r="F37" s="4" t="s">
+        <v>7</v>
+      </c>
       <c r="G37" s="1"/>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.35">
@@ -2980,18 +3031,18 @@
       <c r="G66" s="1"/>
     </row>
     <row r="67" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A67" s="1"/>
+      <c r="B67" s="1"/>
+      <c r="C67" s="1"/>
+      <c r="D67" s="1"/>
+      <c r="E67" s="1"/>
+      <c r="F67" s="1"/>
       <c r="G67" s="1"/>
     </row>
     <row r="68" spans="1:7" x14ac:dyDescent="0.35">
       <c r="G68" s="1"/>
     </row>
     <row r="69" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A69" s="1"/>
-      <c r="B69" s="1"/>
-      <c r="C69" s="1"/>
-      <c r="D69" s="1"/>
-      <c r="E69" s="1"/>
-      <c r="F69" s="1"/>
       <c r="G69" s="1"/>
     </row>
     <row r="70" spans="1:7" x14ac:dyDescent="0.35">
@@ -4462,20 +4513,43 @@
       <c r="G232" s="1"/>
     </row>
     <row r="233" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A233" s="1"/>
+      <c r="B233" s="1"/>
       <c r="C233" s="1"/>
+      <c r="D233" s="1"/>
+      <c r="E233" s="1"/>
+      <c r="F233" s="1"/>
+    </row>
+    <row r="234" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="C234" s="1"/>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F36">
-    <sortCondition ref="D3:D36"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A3:F37">
+    <sortCondition ref="D4:D37"/>
   </sortState>
+  <mergeCells count="1">
+    <mergeCell ref="A2:F2"/>
+  </mergeCells>
   <dataValidations xWindow="821" yWindow="357" count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Estado" prompt="Por favor, introduzca un valor para el estado (PENDIENTE, EN PROGRESO O REALIZADO )" sqref="F1:F36" xr:uid="{01248019-FD26-4D39-BA8E-80B22E1EE596}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Estado" prompt="Por favor, introduzca un valor para el estado (PENDIENTE, EN PROGRESO O REALIZADO )" sqref="F1" xr:uid="{01248019-FD26-4D39-BA8E-80B22E1EE596}">
       <formula1>$N$2:$N$4</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xWindow="821" yWindow="357" count="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Estado" prompt="Por favor, introduzca un valor para el estado (PENDIENTE, EN PROGRESO O REALIZADO )" xr:uid="{D8412D15-E0AC-4AA5-A178-52FD91FADEED}">
+          <x14:formula1>
+            <xm:f>AUX!$F$3:$H$3</xm:f>
+          </x14:formula1>
+          <xm:sqref>F3:F37</xm:sqref>
+        </x14:dataValidation>
+      </x14:dataValidations>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -4483,8 +4557,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{25ACDF49-AC43-4CCD-856F-6ED289E70C3E}">
   <dimension ref="A2:I35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="D36" sqref="D36"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -4493,13 +4567,19 @@
     <col min="3" max="3" width="11.36328125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="13.08984375" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="11.26953125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.54296875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="B2" s="14" t="s">
+      <c r="B2" s="17" t="s">
         <v>46</v>
       </c>
-      <c r="C2" s="14"/>
+      <c r="C2" s="17"/>
+      <c r="F2" s="21" t="s">
+        <v>51</v>
+      </c>
+      <c r="G2" s="21"/>
+      <c r="H2" s="21"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.35">
       <c r="B3" s="11" t="s">
@@ -4508,13 +4588,22 @@
       <c r="C3" s="11">
         <v>28</v>
       </c>
+      <c r="F3" s="22" t="s">
+        <v>5</v>
+      </c>
+      <c r="G3" s="22" t="s">
+        <v>6</v>
+      </c>
+      <c r="H3" s="22" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.35">
       <c r="B4" s="11" t="s">
         <v>43</v>
       </c>
-      <c r="C4" s="15">
-        <f>SUM('SPRINT-BACKLOG'!B2:B36)</f>
+      <c r="C4" s="14">
+        <f>SUM('SPRINT-BACKLOG'!B3:B37)</f>
         <v>37</v>
       </c>
     </row>
@@ -4548,7 +4637,7 @@
         <v>37</v>
       </c>
       <c r="D8" s="10">
-        <f>SUMIF('SPRINT-BACKLOG'!D2:D36,"="&amp;VALUE(A8),'SPRINT-BACKLOG'!B2:B36)</f>
+        <f>SUMIF('SPRINT-BACKLOG'!D3:D37,"="&amp;VALUE(A8),'SPRINT-BACKLOG'!B3:B37)</f>
         <v>2</v>
       </c>
       <c r="E8" s="9">
@@ -4557,7 +4646,7 @@
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A9" s="16">
+      <c r="A9" s="15">
         <v>44229</v>
       </c>
       <c r="B9" s="12">
@@ -4568,7 +4657,7 @@
         <v>35.629629629629626</v>
       </c>
       <c r="D9" s="10">
-        <f>SUMIF('SPRINT-BACKLOG'!D2:D36,"="&amp;VALUE(A9),'SPRINT-BACKLOG'!B2:B36)</f>
+        <f>SUMIF('SPRINT-BACKLOG'!D3:D37,"="&amp;VALUE(A9),'SPRINT-BACKLOG'!B3:B37)</f>
         <v>2</v>
       </c>
       <c r="E9" s="9">
@@ -4588,7 +4677,7 @@
         <v>34.259259259259252</v>
       </c>
       <c r="D10" s="10">
-        <f>SUMIF('SPRINT-BACKLOG'!D2:D36,"="&amp;VALUE(A10),'SPRINT-BACKLOG'!B2:B36)</f>
+        <f>SUMIF('SPRINT-BACKLOG'!D3:D37,"="&amp;VALUE(A10),'SPRINT-BACKLOG'!B3:B37)</f>
         <v>2</v>
       </c>
       <c r="E10" s="9">
@@ -4608,7 +4697,7 @@
         <v>32.888888888888879</v>
       </c>
       <c r="D11" s="10">
-        <f>SUMIF('SPRINT-BACKLOG'!D2:D36,"="&amp;VALUE(A11),'SPRINT-BACKLOG'!B2:B36)</f>
+        <f>SUMIF('SPRINT-BACKLOG'!D3:D37,"="&amp;VALUE(A11),'SPRINT-BACKLOG'!B3:B37)</f>
         <v>1.5</v>
       </c>
       <c r="E11" s="9">
@@ -4628,7 +4717,7 @@
         <v>31.518518518518508</v>
       </c>
       <c r="D12" s="10">
-        <f>SUMIF('SPRINT-BACKLOG'!D2:D36,"="&amp;VALUE(A12),'SPRINT-BACKLOG'!B2:B36)</f>
+        <f>SUMIF('SPRINT-BACKLOG'!D3:D37,"="&amp;VALUE(A12),'SPRINT-BACKLOG'!B3:B37)</f>
         <v>3</v>
       </c>
       <c r="E12" s="9">
@@ -4648,7 +4737,7 @@
         <v>30.148148148148138</v>
       </c>
       <c r="D13" s="10">
-        <f>SUMIF('SPRINT-BACKLOG'!D2:D36,"="&amp;VALUE(A13),'SPRINT-BACKLOG'!B2:B36)</f>
+        <f>SUMIF('SPRINT-BACKLOG'!D3:D37,"="&amp;VALUE(A13),'SPRINT-BACKLOG'!B3:B37)</f>
         <v>0</v>
       </c>
       <c r="E13" s="9">
@@ -4668,7 +4757,7 @@
         <v>28.777777777777768</v>
       </c>
       <c r="D14" s="10">
-        <f>SUMIF('SPRINT-BACKLOG'!D2:D36,"="&amp;VALUE(A14),'SPRINT-BACKLOG'!B2:B36)</f>
+        <f>SUMIF('SPRINT-BACKLOG'!D3:D37,"="&amp;VALUE(A14),'SPRINT-BACKLOG'!B3:B37)</f>
         <v>0</v>
       </c>
       <c r="E14" s="9">
@@ -4688,7 +4777,7 @@
         <v>27.407407407407398</v>
       </c>
       <c r="D15" s="10">
-        <f>SUMIF('SPRINT-BACKLOG'!D2:D36,"="&amp;VALUE(A15),'SPRINT-BACKLOG'!B2:B36)</f>
+        <f>SUMIF('SPRINT-BACKLOG'!D3:D37,"="&amp;VALUE(A15),'SPRINT-BACKLOG'!B3:B37)</f>
         <v>2</v>
       </c>
       <c r="E15" s="9">
@@ -4708,17 +4797,17 @@
         <v>26.037037037037027</v>
       </c>
       <c r="D16" s="10">
-        <f>SUMIF('SPRINT-BACKLOG'!D2:D36,"="&amp;VALUE(A16),'SPRINT-BACKLOG'!B2:B36)</f>
+        <f>SUMIF('SPRINT-BACKLOG'!D3:D37,"="&amp;VALUE(A16),'SPRINT-BACKLOG'!B3:B37)</f>
         <v>2</v>
       </c>
       <c r="E16" s="9">
         <f t="shared" si="1"/>
         <v>22.5</v>
       </c>
-      <c r="F16" s="17"/>
-      <c r="G16" s="17"/>
-      <c r="H16" s="17"/>
-      <c r="I16" s="17"/>
+      <c r="F16" s="16"/>
+      <c r="G16" s="16"/>
+      <c r="H16" s="16"/>
+      <c r="I16" s="16"/>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A17" s="8">
@@ -4732,7 +4821,7 @@
         <v>24.666666666666657</v>
       </c>
       <c r="D17" s="10">
-        <f>SUMIF('SPRINT-BACKLOG'!D2:D36,"="&amp;VALUE(A17),'SPRINT-BACKLOG'!B2:B36)</f>
+        <f>SUMIF('SPRINT-BACKLOG'!D3:D37,"="&amp;VALUE(A17),'SPRINT-BACKLOG'!B3:B37)</f>
         <v>1</v>
       </c>
       <c r="E17" s="9">
@@ -4752,7 +4841,7 @@
         <v>23.296296296296287</v>
       </c>
       <c r="D18" s="10">
-        <f>SUMIF('SPRINT-BACKLOG'!D2:D36,"="&amp;VALUE(A18),'SPRINT-BACKLOG'!B2:B36)</f>
+        <f>SUMIF('SPRINT-BACKLOG'!D3:D37,"="&amp;VALUE(A18),'SPRINT-BACKLOG'!B3:B37)</f>
         <v>3.5</v>
       </c>
       <c r="E18" s="9">
@@ -4772,7 +4861,7 @@
         <v>21.925925925925917</v>
       </c>
       <c r="D19" s="10">
-        <f>SUMIF('SPRINT-BACKLOG'!D2:D36,"="&amp;VALUE(A19),'SPRINT-BACKLOG'!B2:B36)</f>
+        <f>SUMIF('SPRINT-BACKLOG'!D3:D37,"="&amp;VALUE(A19),'SPRINT-BACKLOG'!B3:B37)</f>
         <v>0</v>
       </c>
       <c r="E19" s="9">
@@ -4792,7 +4881,7 @@
         <v>20.555555555555546</v>
       </c>
       <c r="D20" s="10">
-        <f>SUMIF('SPRINT-BACKLOG'!D2:D36,"="&amp;VALUE(A20),'SPRINT-BACKLOG'!B2:B36)</f>
+        <f>SUMIF('SPRINT-BACKLOG'!D3:D37,"="&amp;VALUE(A20),'SPRINT-BACKLOG'!B3:B37)</f>
         <v>0</v>
       </c>
       <c r="E20" s="9">
@@ -4812,7 +4901,7 @@
         <v>19.185185185185176</v>
       </c>
       <c r="D21" s="10">
-        <f>SUMIF('SPRINT-BACKLOG'!D2:D36,"="&amp;VALUE(A21),'SPRINT-BACKLOG'!B2:B36)</f>
+        <f>SUMIF('SPRINT-BACKLOG'!D3:D37,"="&amp;VALUE(A21),'SPRINT-BACKLOG'!B3:B37)</f>
         <v>0</v>
       </c>
       <c r="E21" s="9">
@@ -4832,7 +4921,7 @@
         <v>17.814814814814806</v>
       </c>
       <c r="D22" s="10">
-        <f>SUMIF('SPRINT-BACKLOG'!D2:D36,"="&amp;VALUE(A22),'SPRINT-BACKLOG'!B2:B36)</f>
+        <f>SUMIF('SPRINT-BACKLOG'!D3:D37,"="&amp;VALUE(A22),'SPRINT-BACKLOG'!B3:B37)</f>
         <v>4</v>
       </c>
       <c r="E22" s="9">
@@ -4852,7 +4941,7 @@
         <v>16.444444444444436</v>
       </c>
       <c r="D23" s="10">
-        <f>SUMIF('SPRINT-BACKLOG'!D2:D36,"="&amp;VALUE(A23),'SPRINT-BACKLOG'!B2:B36)</f>
+        <f>SUMIF('SPRINT-BACKLOG'!D3:D37,"="&amp;VALUE(A23),'SPRINT-BACKLOG'!B3:B37)</f>
         <v>1.5</v>
       </c>
       <c r="E23" s="9">
@@ -4872,7 +4961,7 @@
         <v>15.074074074074066</v>
       </c>
       <c r="D24" s="10">
-        <f>SUMIF('SPRINT-BACKLOG'!D2:D36,"="&amp;VALUE(A24),'SPRINT-BACKLOG'!B2:B36)</f>
+        <f>SUMIF('SPRINT-BACKLOG'!D3:D37,"="&amp;VALUE(A24),'SPRINT-BACKLOG'!B3:B37)</f>
         <v>3</v>
       </c>
       <c r="E24" s="9">
@@ -4892,7 +4981,7 @@
         <v>13.703703703703695</v>
       </c>
       <c r="D25" s="10">
-        <f>SUMIF('SPRINT-BACKLOG'!D2:D36,"="&amp;VALUE(A25),'SPRINT-BACKLOG'!B2:B36)</f>
+        <f>SUMIF('SPRINT-BACKLOG'!D3:D37,"="&amp;VALUE(A25),'SPRINT-BACKLOG'!B3:B37)</f>
         <v>0</v>
       </c>
       <c r="E25" s="9">
@@ -4912,7 +5001,7 @@
         <v>12.333333333333325</v>
       </c>
       <c r="D26" s="10">
-        <f>SUMIF('SPRINT-BACKLOG'!D2:D36,"="&amp;VALUE(A26),'SPRINT-BACKLOG'!B2:B36)</f>
+        <f>SUMIF('SPRINT-BACKLOG'!D3:D37,"="&amp;VALUE(A26),'SPRINT-BACKLOG'!B3:B37)</f>
         <v>0</v>
       </c>
       <c r="E26" s="9">
@@ -4932,7 +5021,7 @@
         <v>10.962962962962955</v>
       </c>
       <c r="D27" s="10">
-        <f>SUMIF('SPRINT-BACKLOG'!D2:D36,"="&amp;VALUE(A27),'SPRINT-BACKLOG'!B2:B36)</f>
+        <f>SUMIF('SPRINT-BACKLOG'!D3:D37,"="&amp;VALUE(A27),'SPRINT-BACKLOG'!B3:B37)</f>
         <v>0</v>
       </c>
       <c r="E27" s="9">
@@ -4952,7 +5041,7 @@
         <v>9.5925925925925846</v>
       </c>
       <c r="D28" s="10">
-        <f>SUMIF('SPRINT-BACKLOG'!D2:D36,"="&amp;VALUE(A28),'SPRINT-BACKLOG'!B2:B36)</f>
+        <f>SUMIF('SPRINT-BACKLOG'!D3:D37,"="&amp;VALUE(A28),'SPRINT-BACKLOG'!B3:B37)</f>
         <v>0</v>
       </c>
       <c r="E28" s="9">
@@ -4972,7 +5061,7 @@
         <v>8.2222222222222143</v>
       </c>
       <c r="D29" s="10">
-        <f>SUMIF('SPRINT-BACKLOG'!D2:D36,"="&amp;VALUE(A29),'SPRINT-BACKLOG'!B2:B36)</f>
+        <f>SUMIF('SPRINT-BACKLOG'!D3:D37,"="&amp;VALUE(A29),'SPRINT-BACKLOG'!B3:B37)</f>
         <v>4.5</v>
       </c>
       <c r="E29" s="9">
@@ -4992,7 +5081,7 @@
         <v>6.8518518518518441</v>
       </c>
       <c r="D30" s="10">
-        <f>SUMIF('SPRINT-BACKLOG'!D2:D36,"="&amp;VALUE(A30),'SPRINT-BACKLOG'!B2:B36)</f>
+        <f>SUMIF('SPRINT-BACKLOG'!D3:D37,"="&amp;VALUE(A30),'SPRINT-BACKLOG'!B3:B37)</f>
         <v>2</v>
       </c>
       <c r="E30" s="9">
@@ -5012,7 +5101,7 @@
         <v>5.4814814814814738</v>
       </c>
       <c r="D31" s="10">
-        <f>SUMIF('SPRINT-BACKLOG'!D2:D36,"="&amp;VALUE(A31),'SPRINT-BACKLOG'!B2:B36)</f>
+        <f>SUMIF('SPRINT-BACKLOG'!D3:D37,"="&amp;VALUE(A31),'SPRINT-BACKLOG'!B3:B37)</f>
         <v>1</v>
       </c>
       <c r="E31" s="9">
@@ -5032,7 +5121,7 @@
         <v>4.1111111111111036</v>
       </c>
       <c r="D32" s="10">
-        <f>SUMIF('SPRINT-BACKLOG'!D2:D36,"="&amp;VALUE(A32),'SPRINT-BACKLOG'!B2:B36)</f>
+        <f>SUMIF('SPRINT-BACKLOG'!D3:D37,"="&amp;VALUE(A32),'SPRINT-BACKLOG'!B3:B37)</f>
         <v>0</v>
       </c>
       <c r="E32" s="9">
@@ -5052,7 +5141,7 @@
         <v>2.7407407407407334</v>
       </c>
       <c r="D33" s="10">
-        <f>SUMIF('SPRINT-BACKLOG'!D2:D36,"="&amp;VALUE(A33),'SPRINT-BACKLOG'!B2:B36)</f>
+        <f>SUMIF('SPRINT-BACKLOG'!D3:D37,"="&amp;VALUE(A33),'SPRINT-BACKLOG'!B3:B37)</f>
         <v>2</v>
       </c>
       <c r="E33" s="9">
@@ -5072,7 +5161,7 @@
         <v>1.3703703703703629</v>
       </c>
       <c r="D34" s="10">
-        <f>SUMIF('SPRINT-BACKLOG'!D2:D36,"="&amp;VALUE(A34),'SPRINT-BACKLOG'!B2:B36)</f>
+        <f>SUMIF('SPRINT-BACKLOG'!D3:D37,"="&amp;VALUE(A34),'SPRINT-BACKLOG'!B3:B37)</f>
         <v>0</v>
       </c>
       <c r="E34" s="9">
@@ -5092,7 +5181,7 @@
         <v>-7.5495165674510645E-15</v>
       </c>
       <c r="D35" s="10">
-        <f>SUMIF('SPRINT-BACKLOG'!D2:D36,"="&amp;VALUE(A35),'SPRINT-BACKLOG'!B2:B36)</f>
+        <f>SUMIF('SPRINT-BACKLOG'!D3:D37,"="&amp;VALUE(A35),'SPRINT-BACKLOG'!B3:B37)</f>
         <v>0</v>
       </c>
       <c r="E35" s="9">
@@ -5101,8 +5190,9 @@
       </c>
     </row>
   </sheetData>
-  <mergeCells count="1">
+  <mergeCells count="2">
     <mergeCell ref="B2:C2"/>
+    <mergeCell ref="F2:H2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>